<commit_message>
minor update to lab list for spring 2020
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
@@ -1994,8 +1994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2628,7 +2628,7 @@
         <v>175</v>
       </c>
       <c r="C13" s="14">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E13" s="14">
         <v>6</v>
@@ -3100,16 +3100,16 @@
         <v>0</v>
       </c>
       <c r="X23" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W23,C$2:C$73)</f>
-        <v>306</v>
+        <f t="shared" ref="X23:X31" si="1">SUMIF(U$2:U$73,"&gt;=" &amp; W23,C$2:C$73)</f>
+        <v>304</v>
       </c>
       <c r="Y23" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W23,D$2:D$73)</f>
+        <f t="shared" ref="Y23:Y31" si="2">SUMIF(U$2:U$73,"&gt;=" &amp; W23,D$2:D$73)</f>
         <v>11</v>
       </c>
       <c r="Z23" s="8">
-        <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
-        <v>28.080000000000002</v>
+        <f t="shared" ref="Z23:Z31" si="3">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
+        <v>27.950000000000006</v>
       </c>
       <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
@@ -3176,16 +3176,16 @@
         <v>0.5</v>
       </c>
       <c r="X24" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W24,C$2:C$73)</f>
-        <v>276</v>
+        <f t="shared" si="1"/>
+        <v>274</v>
       </c>
       <c r="Y24" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W24,D$2:D$73)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z24" s="8">
-        <f t="shared" si="1"/>
-        <v>25.740000000000002</v>
+        <f t="shared" si="3"/>
+        <v>25.610000000000003</v>
       </c>
       <c r="AA24" s="33"/>
       <c r="AB24" s="33"/>
@@ -3236,16 +3236,16 @@
         <v>1</v>
       </c>
       <c r="X25" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W25,C$2:C$73)</f>
-        <v>236</v>
+        <f t="shared" si="1"/>
+        <v>234</v>
       </c>
       <c r="Y25" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W25,D$2:D$73)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z25" s="8">
-        <f t="shared" si="1"/>
-        <v>23.14</v>
+        <f t="shared" si="3"/>
+        <v>23.010000000000005</v>
       </c>
       <c r="AA25" s="33"/>
       <c r="AB25" s="33"/>
@@ -3306,16 +3306,16 @@
         <v>1.5</v>
       </c>
       <c r="X26" s="31">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W26,C$2:C$73)</f>
-        <v>222</v>
+        <f t="shared" si="1"/>
+        <v>220</v>
       </c>
       <c r="Y26" s="31">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W26,D$2:D$73)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z26" s="8">
-        <f t="shared" si="1"/>
-        <v>22.230000000000004</v>
+        <f t="shared" si="3"/>
+        <v>22.1</v>
       </c>
       <c r="AA26" s="33"/>
       <c r="AB26" s="33"/>
@@ -3384,16 +3384,16 @@
         <v>2</v>
       </c>
       <c r="X27" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W27,C$2:C$73)</f>
-        <v>205</v>
+        <f t="shared" si="1"/>
+        <v>203</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W27,D$2:D$73)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z27" s="8">
-        <f t="shared" si="1"/>
-        <v>21.125</v>
+        <f t="shared" si="3"/>
+        <v>20.994999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
@@ -3447,15 +3447,15 @@
         <v>2.5</v>
       </c>
       <c r="X28" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W28,C$2:C$73)</f>
+        <f t="shared" si="1"/>
         <v>161</v>
       </c>
       <c r="Y28" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W28,D$2:D$73)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z28" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>18.265000000000001</v>
       </c>
     </row>
@@ -3489,15 +3489,15 @@
         <v>3</v>
       </c>
       <c r="X29" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W29,C$2:C$73)</f>
+        <f t="shared" si="1"/>
         <v>148</v>
       </c>
       <c r="Y29" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W29,D$2:D$73)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="Z29" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>17.03</v>
       </c>
     </row>
@@ -3550,15 +3550,15 @@
         <v>3.5</v>
       </c>
       <c r="X30" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W30,C$2:C$73)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y30" s="6">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W30,D$2:D$73)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z30" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -3575,22 +3575,24 @@
       <c r="K31" s="34"/>
       <c r="L31" s="34"/>
       <c r="M31" s="36"/>
-      <c r="T31" s="34"/>
+      <c r="T31" s="34">
+        <v>2</v>
+      </c>
       <c r="U31" s="77"/>
       <c r="V31" s="15"/>
       <c r="W31" s="83">
         <v>4</v>
       </c>
       <c r="X31" s="47">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W31,C$2:C$73)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y31" s="47">
-        <f>SUMIF(U$2:U$73,"&gt;=" &amp; W31,D$2:D$73)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z31" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -5379,7 +5381,7 @@
       </c>
       <c r="T69" s="34"/>
       <c r="U69" s="77">
-        <f t="shared" ref="U69:U72" si="2">SUM(Q69:T69)</f>
+        <f t="shared" ref="U69:U72" si="4">SUM(Q69:T69)</f>
         <v>1</v>
       </c>
       <c r="V69" s="15"/>
@@ -5427,7 +5429,7 @@
       </c>
       <c r="T70" s="34"/>
       <c r="U70" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="V70" s="15"/>
@@ -5476,7 +5478,7 @@
       </c>
       <c r="T71" s="34"/>
       <c r="U71" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="V71" s="15"/>
@@ -5528,7 +5530,7 @@
       </c>
       <c r="T72" s="37"/>
       <c r="U72" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="V72" s="15"/>
@@ -5555,11 +5557,11 @@
       </c>
       <c r="R74" s="65">
         <f t="array" ref="R74">SUM($C2:$C72*(R2:R72&gt;=0.9)*($U2:$U72&gt;=$W$12))</f>
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="S74" s="65">
         <f t="array" ref="S74">SUM($C2:$C72*(S2:S72&gt;=0.9)*($U2:$U72&gt;=$W$12))</f>
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="T74" s="66"/>
       <c r="V74" s="15"/>
@@ -5585,11 +5587,11 @@
       </c>
       <c r="R75" s="68">
         <f t="array" ref="R75">SUM($C2:$C72*R2:R72*($U2:$U72&gt;=$W$12))</f>
-        <v>215.6</v>
+        <v>213.6</v>
       </c>
       <c r="S75" s="68">
         <f t="array" ref="S75">SUM($C2:$C72*S2:S72*($U2:$U72&gt;=$W$12))</f>
-        <v>207.23</v>
+        <v>205.23</v>
       </c>
       <c r="T75" s="69"/>
       <c r="V75" s="15"/>
@@ -5619,11 +5621,11 @@
       </c>
       <c r="R76" s="68">
         <f t="array" ref="R76">SUM($C$2:$C$72*(R$2:R$72&gt;=0.1)*($U$2:$U$72&gt;=$W$12))</f>
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="S76" s="68">
         <f t="array" ref="S76">SUM($C$2:$C$72*(S$2:S$72&gt;=0.1)*($U$2:$U$72&gt;=$W$12))</f>
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="T76" s="69"/>
       <c r="U76" s="3"/>
@@ -5649,16 +5651,16 @@
       <c r="O77" s="68"/>
       <c r="P77" s="68"/>
       <c r="Q77" s="68">
-        <f t="shared" ref="Q77:S77" si="3">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>236</v>
+        <f t="shared" ref="Q77:S77" si="5">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>234</v>
       </c>
       <c r="R77" s="68">
-        <f t="shared" si="3"/>
-        <v>236</v>
+        <f t="shared" si="5"/>
+        <v>234</v>
       </c>
       <c r="S77" s="68">
-        <f t="shared" si="3"/>
-        <v>236</v>
+        <f t="shared" si="5"/>
+        <v>234</v>
       </c>
       <c r="T77" s="69"/>
       <c r="V77" s="15"/>
@@ -5679,16 +5681,16 @@
       <c r="O78" s="70"/>
       <c r="P78" s="70"/>
       <c r="Q78" s="70">
-        <f t="shared" ref="Q78:S78" si="4">Q75/Q77</f>
-        <v>0.81779661016949157</v>
+        <f t="shared" ref="Q78:S78" si="6">Q75/Q77</f>
+        <v>0.82478632478632474</v>
       </c>
       <c r="R78" s="70">
-        <f t="shared" si="4"/>
-        <v>0.91355932203389834</v>
+        <f t="shared" si="6"/>
+        <v>0.9128205128205128</v>
       </c>
       <c r="S78" s="70">
-        <f t="shared" si="4"/>
-        <v>0.87809322033898296</v>
+        <f t="shared" si="6"/>
+        <v>0.87705128205128202</v>
       </c>
       <c r="T78" s="71"/>
       <c r="V78" s="15"/>
@@ -5706,15 +5708,15 @@
       <c r="O79" s="73"/>
       <c r="P79" s="73"/>
       <c r="Q79" s="73">
-        <f t="shared" ref="Q79:S79" si="5">Q77-Q75</f>
-        <v>43</v>
+        <f t="shared" ref="Q79:S79" si="7">Q77-Q75</f>
+        <v>41</v>
       </c>
       <c r="R79" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>20.400000000000006</v>
       </c>
       <c r="S79" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>28.77000000000001</v>
       </c>
       <c r="T79" s="74"/>

</xml_diff>

<commit_message>
small update to spring spreadsheet
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
@@ -1994,8 +1994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="X23" s="6">
         <f t="shared" ref="X23:X31" si="1">SUMIF(U$2:U$73,"&gt;=" &amp; W23,C$2:C$73)</f>
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Y23" s="6">
         <f t="shared" ref="Y23:Y31" si="2">SUMIF(U$2:U$73,"&gt;=" &amp; W23,D$2:D$73)</f>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="Z23" s="8">
         <f t="shared" ref="Z23:Z31" si="3">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
-        <v>27.950000000000006</v>
+        <v>27.885000000000002</v>
       </c>
       <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="X24" s="6">
         <f t="shared" si="1"/>
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Y24" s="6">
         <f t="shared" si="2"/>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="Z24" s="8">
         <f t="shared" si="3"/>
-        <v>25.610000000000003</v>
+        <v>25.544999999999998</v>
       </c>
       <c r="AA24" s="33"/>
       <c r="AB24" s="33"/>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="X25" s="6">
         <f t="shared" si="1"/>
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Y25" s="6">
         <f t="shared" si="2"/>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="Z25" s="8">
         <f t="shared" si="3"/>
-        <v>23.010000000000005</v>
+        <v>22.945</v>
       </c>
       <c r="AA25" s="33"/>
       <c r="AB25" s="33"/>
@@ -3307,7 +3307,7 @@
       </c>
       <c r="X26" s="31">
         <f t="shared" si="1"/>
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Y26" s="31">
         <f t="shared" si="2"/>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="Z26" s="8">
         <f t="shared" si="3"/>
-        <v>22.1</v>
+        <v>22.035000000000004</v>
       </c>
       <c r="AA26" s="33"/>
       <c r="AB26" s="33"/>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="X27" s="6">
         <f t="shared" si="1"/>
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Y27" s="6">
         <f t="shared" si="2"/>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="Z27" s="8">
         <f t="shared" si="3"/>
-        <v>20.994999999999997</v>
+        <v>20.930000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="X28" s="6">
         <f t="shared" si="1"/>
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Y28" s="6">
         <f t="shared" si="2"/>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="Z28" s="8">
         <f t="shared" si="3"/>
-        <v>18.265000000000001</v>
+        <v>18.2</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
@@ -3490,7 +3490,7 @@
       </c>
       <c r="X29" s="6">
         <f t="shared" si="1"/>
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Y29" s="6">
         <f t="shared" si="2"/>
@@ -3498,7 +3498,7 @@
       </c>
       <c r="Z29" s="8">
         <f t="shared" si="3"/>
-        <v>17.03</v>
+        <v>16.965</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
@@ -3602,7 +3602,7 @@
         <v>144</v>
       </c>
       <c r="C32" s="14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14">
@@ -5553,15 +5553,15 @@
       <c r="P74" s="65"/>
       <c r="Q74" s="65">
         <f t="array" ref="Q74">SUM($C2:$C72*(Q2:Q72&gt;=0.9)*($U2:$U72&gt;=$W$12))</f>
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R74" s="65">
         <f t="array" ref="R74">SUM($C2:$C72*(R2:R72&gt;=0.9)*($U2:$U72&gt;=$W$12))</f>
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S74" s="65">
         <f t="array" ref="S74">SUM($C2:$C72*(S2:S72&gt;=0.9)*($U2:$U72&gt;=$W$12))</f>
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T74" s="66"/>
       <c r="V74" s="15"/>
@@ -5583,15 +5583,15 @@
       <c r="P75" s="68"/>
       <c r="Q75" s="68">
         <f t="array" ref="Q75">SUM($C2:$C72*Q2:Q72*($U2:$U72&gt;=$W$12))</f>
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="R75" s="68">
         <f t="array" ref="R75">SUM($C2:$C72*R2:R72*($U2:$U72&gt;=$W$12))</f>
-        <v>213.6</v>
+        <v>212.6</v>
       </c>
       <c r="S75" s="68">
         <f t="array" ref="S75">SUM($C2:$C72*S2:S72*($U2:$U72&gt;=$W$12))</f>
-        <v>205.23</v>
+        <v>204.23</v>
       </c>
       <c r="T75" s="69"/>
       <c r="V75" s="15"/>
@@ -5617,15 +5617,15 @@
       <c r="P76" s="68"/>
       <c r="Q76" s="68">
         <f t="array" ref="Q76">SUM($C$2:$C$72*(Q$2:Q$72&gt;=0.1)*($U$2:$U$72&gt;=$W$12))</f>
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="R76" s="68">
         <f t="array" ref="R76">SUM($C$2:$C$72*(R$2:R$72&gt;=0.1)*($U$2:$U$72&gt;=$W$12))</f>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S76" s="68">
         <f t="array" ref="S76">SUM($C$2:$C$72*(S$2:S$72&gt;=0.1)*($U$2:$U$72&gt;=$W$12))</f>
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T76" s="69"/>
       <c r="U76" s="3"/>
@@ -5652,15 +5652,15 @@
       <c r="P77" s="68"/>
       <c r="Q77" s="68">
         <f t="shared" ref="Q77:S77" si="5">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R77" s="68">
         <f t="shared" si="5"/>
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S77" s="68">
         <f t="shared" si="5"/>
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="T77" s="69"/>
       <c r="V77" s="15"/>
@@ -5682,15 +5682,15 @@
       <c r="P78" s="70"/>
       <c r="Q78" s="70">
         <f t="shared" ref="Q78:S78" si="6">Q75/Q77</f>
-        <v>0.82478632478632474</v>
+        <v>0.82403433476394849</v>
       </c>
       <c r="R78" s="70">
         <f t="shared" si="6"/>
-        <v>0.9128205128205128</v>
+        <v>0.9124463519313305</v>
       </c>
       <c r="S78" s="70">
         <f t="shared" si="6"/>
-        <v>0.87705128205128202</v>
+        <v>0.87652360515021455</v>
       </c>
       <c r="T78" s="71"/>
       <c r="V78" s="15"/>

</xml_diff>

<commit_message>
New lab on a_t and a_c.
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="199">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -778,6 +778,9 @@
   </si>
   <si>
     <t>New by Matt 2019</t>
+  </si>
+  <si>
+    <t>Tangential Acceleration and Centripetal Acceleration</t>
   </si>
 </sst>
 </file>
@@ -1992,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD114"/>
+  <dimension ref="A1:AD115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2199,7 +2202,7 @@
       </c>
       <c r="T3" s="60"/>
       <c r="U3" s="76">
-        <f t="shared" ref="U3:U68" si="0">SUM(Q3:T3)</f>
+        <f t="shared" ref="U3:U69" si="0">SUM(Q3:T3)</f>
         <v>3</v>
       </c>
       <c r="V3" s="80"/>
@@ -3100,16 +3103,16 @@
         <v>0</v>
       </c>
       <c r="X23" s="6">
-        <f t="shared" ref="X23:X31" si="1">SUMIF(U$2:U$73,"&gt;=" &amp; W23,C$2:C$73)</f>
-        <v>303</v>
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W23,C$2:C$74)</f>
+        <v>307</v>
       </c>
       <c r="Y23" s="6">
-        <f t="shared" ref="Y23:Y31" si="2">SUMIF(U$2:U$73,"&gt;=" &amp; W23,D$2:D$73)</f>
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W23,D$2:D$74)</f>
         <v>11</v>
       </c>
       <c r="Z23" s="8">
-        <f t="shared" ref="Z23:Z31" si="3">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
-        <v>27.885000000000002</v>
+        <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
+        <v>28.145000000000003</v>
       </c>
       <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
@@ -3176,16 +3179,16 @@
         <v>0.5</v>
       </c>
       <c r="X24" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W24,C$2:C$74)</f>
+        <v>277</v>
+      </c>
+      <c r="Y24" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W24,D$2:D$74)</f>
+        <v>10</v>
+      </c>
+      <c r="Z24" s="8">
         <f t="shared" si="1"/>
-        <v>273</v>
-      </c>
-      <c r="Y24" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z24" s="8">
-        <f t="shared" si="3"/>
-        <v>25.544999999999998</v>
+        <v>25.805000000000003</v>
       </c>
       <c r="AA24" s="33"/>
       <c r="AB24" s="33"/>
@@ -3236,16 +3239,16 @@
         <v>1</v>
       </c>
       <c r="X25" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W25,C$2:C$74)</f>
+        <v>237</v>
+      </c>
+      <c r="Y25" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W25,D$2:D$74)</f>
+        <v>10</v>
+      </c>
+      <c r="Z25" s="8">
         <f t="shared" si="1"/>
-        <v>233</v>
-      </c>
-      <c r="Y25" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z25" s="8">
-        <f t="shared" si="3"/>
-        <v>22.945</v>
+        <v>23.205000000000002</v>
       </c>
       <c r="AA25" s="33"/>
       <c r="AB25" s="33"/>
@@ -3306,16 +3309,16 @@
         <v>1.5</v>
       </c>
       <c r="X26" s="31">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W26,C$2:C$74)</f>
+        <v>221</v>
+      </c>
+      <c r="Y26" s="31">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W26,D$2:D$74)</f>
+        <v>10</v>
+      </c>
+      <c r="Z26" s="8">
         <f t="shared" si="1"/>
-        <v>219</v>
-      </c>
-      <c r="Y26" s="31">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z26" s="8">
-        <f t="shared" si="3"/>
-        <v>22.035000000000004</v>
+        <v>22.165000000000003</v>
       </c>
       <c r="AA26" s="33"/>
       <c r="AB26" s="33"/>
@@ -3384,16 +3387,16 @@
         <v>2</v>
       </c>
       <c r="X27" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W27,C$2:C$74)</f>
+        <v>204</v>
+      </c>
+      <c r="Y27" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W27,D$2:D$74)</f>
+        <v>10</v>
+      </c>
+      <c r="Z27" s="8">
         <f t="shared" si="1"/>
-        <v>202</v>
-      </c>
-      <c r="Y27" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z27" s="8">
-        <f t="shared" si="3"/>
-        <v>20.930000000000003</v>
+        <v>21.060000000000006</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
@@ -3447,16 +3450,16 @@
         <v>2.5</v>
       </c>
       <c r="X28" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W28,C$2:C$74)</f>
+        <v>162</v>
+      </c>
+      <c r="Y28" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W28,D$2:D$74)</f>
+        <v>10</v>
+      </c>
+      <c r="Z28" s="8">
         <f t="shared" si="1"/>
-        <v>160</v>
-      </c>
-      <c r="Y28" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z28" s="8">
-        <f t="shared" si="3"/>
-        <v>18.2</v>
+        <v>18.330000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
@@ -3489,16 +3492,16 @@
         <v>3</v>
       </c>
       <c r="X29" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W29,C$2:C$74)</f>
+        <v>149</v>
+      </c>
+      <c r="Y29" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W29,D$2:D$74)</f>
+        <v>9</v>
+      </c>
+      <c r="Z29" s="8">
         <f t="shared" si="1"/>
-        <v>147</v>
-      </c>
-      <c r="Y29" s="6">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="Z29" s="8">
-        <f t="shared" si="3"/>
-        <v>16.965</v>
+        <v>17.094999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
@@ -3550,15 +3553,15 @@
         <v>3.5</v>
       </c>
       <c r="X30" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W30,C$2:C$74)</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="6">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W30,D$2:D$74)</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y30" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z30" s="8">
-        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -3575,24 +3578,30 @@
       <c r="K31" s="34"/>
       <c r="L31" s="34"/>
       <c r="M31" s="36"/>
+      <c r="S31" s="36">
+        <v>1</v>
+      </c>
       <c r="T31" s="34">
         <v>2</v>
       </c>
-      <c r="U31" s="77"/>
+      <c r="U31" s="77">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="V31" s="15"/>
       <c r="W31" s="83">
         <v>4</v>
       </c>
       <c r="X31" s="47">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W31,C$2:C$74)</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="47">
+        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W31,D$2:D$74)</f>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y31" s="47">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z31" s="9">
-        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -4637,212 +4646,220 @@
       <c r="AC51"/>
       <c r="AD51"/>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
       <c r="B52" s="23" t="s">
-        <v>163</v>
+        <v>198</v>
       </c>
       <c r="C52" s="14">
-        <v>4</v>
-      </c>
-      <c r="E52" s="14">
-        <v>33</v>
-      </c>
-      <c r="G52" s="14">
-        <v>29</v>
-      </c>
-      <c r="H52" s="14">
-        <v>29</v>
-      </c>
-      <c r="I52" s="22"/>
-      <c r="J52" s="36">
-        <v>1</v>
-      </c>
-      <c r="K52" s="2">
-        <v>1</v>
-      </c>
-      <c r="L52" s="2">
-        <v>1</v>
-      </c>
-      <c r="M52" s="20">
-        <v>1</v>
-      </c>
-      <c r="N52" s="36">
-        <v>1</v>
-      </c>
-      <c r="O52" s="36">
-        <v>1</v>
-      </c>
-      <c r="P52" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q52" s="36">
-        <v>1</v>
-      </c>
-      <c r="R52" s="36">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="J52" s="36"/>
+      <c r="K52" s="34"/>
+      <c r="L52" s="34"/>
+      <c r="M52" s="36"/>
+      <c r="N52" s="36"/>
+      <c r="O52" s="36"/>
+      <c r="P52" s="36"/>
+      <c r="Q52" s="36"/>
+      <c r="R52" s="36"/>
       <c r="S52" s="36">
         <v>1</v>
       </c>
       <c r="T52" s="34"/>
       <c r="U52" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V52" s="15"/>
+      <c r="W52" s="3"/>
+      <c r="X52" s="33"/>
+      <c r="Y52" s="33"/>
+      <c r="Z52" s="33"/>
       <c r="AA52" s="33"/>
-    </row>
-    <row r="53" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10"/>
+      <c r="AB52" s="33"/>
+      <c r="AC52" s="33"/>
+      <c r="AD52" s="33"/>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B53" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C53" s="14">
-        <v>3</v>
-      </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="E53" s="14">
+        <v>33</v>
+      </c>
+      <c r="G53" s="14">
+        <v>29</v>
+      </c>
+      <c r="H53" s="14">
+        <v>29</v>
+      </c>
       <c r="I53" s="22"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="2"/>
+      <c r="J53" s="36">
+        <v>1</v>
+      </c>
+      <c r="K53" s="2">
+        <v>1</v>
+      </c>
       <c r="L53" s="2">
-        <v>0</v>
-      </c>
-      <c r="M53" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="M53" s="20">
+        <v>1</v>
+      </c>
       <c r="N53" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="O53" s="36"/>
-      <c r="P53" s="36"/>
-      <c r="Q53" s="36"/>
-      <c r="R53" s="36"/>
+        <v>1</v>
+      </c>
+      <c r="O53" s="36">
+        <v>1</v>
+      </c>
+      <c r="P53" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="36">
+        <v>1</v>
+      </c>
+      <c r="R53" s="36">
+        <v>1</v>
+      </c>
       <c r="S53" s="36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T53" s="34"/>
       <c r="U53" s="77">
         <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V53" s="15"/>
+      <c r="AA53" s="33"/>
+    </row>
+    <row r="54" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
+      <c r="B54" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" s="14">
+        <v>3</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="36"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2">
+        <v>0</v>
+      </c>
+      <c r="M54" s="20"/>
+      <c r="N54" s="36">
         <v>0.5</v>
       </c>
-      <c r="V53" s="15"/>
-      <c r="W53" s="3"/>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B54" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="C54" s="14">
-        <v>1</v>
-      </c>
-      <c r="I54" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="K54" s="34"/>
-      <c r="L54" s="34"/>
-      <c r="M54" s="36"/>
+      <c r="O54" s="36"/>
+      <c r="P54" s="36"/>
+      <c r="Q54" s="36"/>
+      <c r="R54" s="36"/>
       <c r="S54" s="36">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="T54" s="34"/>
       <c r="U54" s="77">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="V54" s="15"/>
-      <c r="AA54" s="33"/>
-    </row>
-    <row r="55" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="10"/>
+      <c r="W54" s="3"/>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B55" s="23" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="C55" s="14">
-        <v>4</v>
-      </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="22"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2">
-        <v>0</v>
-      </c>
-      <c r="M55" s="20"/>
-      <c r="N55" s="36"/>
-      <c r="O55" s="36"/>
-      <c r="P55" s="36"/>
-      <c r="Q55" s="36"/>
-      <c r="R55" s="36"/>
+        <v>1</v>
+      </c>
+      <c r="I55" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="K55" s="34"/>
+      <c r="L55" s="34"/>
+      <c r="M55" s="36"/>
       <c r="S55" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T55" s="34"/>
       <c r="U55" s="77">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V55" s="15"/>
-      <c r="W55" s="3"/>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA55" s="33"/>
+    </row>
+    <row r="56" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="10"/>
       <c r="B56" s="23" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C56" s="14">
-        <v>3</v>
-      </c>
-      <c r="D56" s="14">
-        <v>0</v>
-      </c>
-      <c r="I56" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="K56" s="34"/>
-      <c r="L56" s="34"/>
-      <c r="M56" s="36"/>
-      <c r="R56" s="36">
-        <v>0.7</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2">
+        <v>0</v>
+      </c>
+      <c r="M56" s="20"/>
+      <c r="N56" s="36"/>
+      <c r="O56" s="36"/>
+      <c r="P56" s="36"/>
+      <c r="Q56" s="36"/>
+      <c r="R56" s="36"/>
       <c r="S56" s="36">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="T56" s="34"/>
       <c r="U56" s="77">
         <f t="shared" si="0"/>
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="V56" s="15"/>
-      <c r="Y56" s="6"/>
-      <c r="AA56" s="33"/>
+      <c r="W56" s="3"/>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B57" s="23" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="C57" s="14">
-        <v>6</v>
-      </c>
-      <c r="E57" s="14">
-        <v>34</v>
-      </c>
-      <c r="H57" s="14">
-        <v>30</v>
-      </c>
-      <c r="I57" s="22"/>
-      <c r="L57" s="2">
+        <v>3</v>
+      </c>
+      <c r="D57" s="14">
+        <v>0</v>
+      </c>
+      <c r="I57" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="K57" s="34"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="36"/>
+      <c r="R57" s="36">
         <v>0.7</v>
-      </c>
-      <c r="P57" s="36">
-        <v>1</v>
-      </c>
-      <c r="R57" s="36">
-        <v>1</v>
       </c>
       <c r="S57" s="36">
         <v>0.7</v>
@@ -4850,194 +4867,171 @@
       <c r="T57" s="34"/>
       <c r="U57" s="77">
         <f t="shared" si="0"/>
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="V57" s="15"/>
+      <c r="Y57" s="6"/>
       <c r="AA57" s="33"/>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C58" s="14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E58" s="14">
-        <v>35</v>
-      </c>
-      <c r="G58" s="14">
+        <v>34</v>
+      </c>
+      <c r="H58" s="14">
         <v>30</v>
       </c>
-      <c r="H58" s="14">
-        <v>31</v>
-      </c>
       <c r="I58" s="22"/>
-      <c r="J58" s="36">
-        <v>1</v>
-      </c>
-      <c r="K58" s="2">
-        <v>1</v>
-      </c>
       <c r="L58" s="2">
-        <v>1</v>
-      </c>
-      <c r="M58" s="20">
-        <v>1</v>
-      </c>
-      <c r="N58" s="36">
-        <v>1</v>
-      </c>
-      <c r="O58" s="36">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="P58" s="36">
         <v>1</v>
       </c>
-      <c r="Q58" s="36">
-        <v>1</v>
-      </c>
       <c r="R58" s="36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S58" s="36">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="T58" s="34"/>
       <c r="U58" s="77">
         <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="V58" s="15"/>
+      <c r="AA58" s="33"/>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B59" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C59" s="14">
+        <v>3</v>
+      </c>
+      <c r="E59" s="14">
+        <v>35</v>
+      </c>
+      <c r="G59" s="14">
+        <v>30</v>
+      </c>
+      <c r="H59" s="14">
+        <v>31</v>
+      </c>
+      <c r="I59" s="22"/>
+      <c r="J59" s="36">
+        <v>1</v>
+      </c>
+      <c r="K59" s="2">
+        <v>1</v>
+      </c>
+      <c r="L59" s="2">
+        <v>1</v>
+      </c>
+      <c r="M59" s="20">
+        <v>1</v>
+      </c>
+      <c r="N59" s="36">
+        <v>1</v>
+      </c>
+      <c r="O59" s="36">
+        <v>1</v>
+      </c>
+      <c r="P59" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="36">
+        <v>1</v>
+      </c>
+      <c r="R59" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="S59" s="36">
+        <v>1</v>
+      </c>
+      <c r="T59" s="34"/>
+      <c r="U59" s="77">
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="V58" s="15"/>
-      <c r="Z58" s="6"/>
-      <c r="AA58" s="33"/>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A59" s="11" t="s">
+      <c r="V59" s="15"/>
+      <c r="Z59" s="6"/>
+      <c r="AA59" s="33"/>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A60" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B59" s="26" t="s">
+      <c r="B60" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="C59" s="13">
+      <c r="C60" s="13">
         <v>2</v>
       </c>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13">
+      <c r="D60" s="13"/>
+      <c r="E60" s="13">
         <v>36</v>
       </c>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13">
+      <c r="F60" s="13"/>
+      <c r="G60" s="13">
         <v>31</v>
       </c>
-      <c r="H59" s="13">
+      <c r="H60" s="13">
         <v>32</v>
       </c>
-      <c r="I59" s="21"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="12"/>
-      <c r="L59" s="12">
-        <v>1</v>
-      </c>
-      <c r="M59" s="12">
-        <v>1</v>
-      </c>
-      <c r="N59" s="35">
-        <v>1</v>
-      </c>
-      <c r="O59" s="35">
-        <v>1</v>
-      </c>
-      <c r="P59" s="35"/>
-      <c r="Q59" s="35">
-        <v>1</v>
-      </c>
-      <c r="R59" s="35">
-        <v>1</v>
-      </c>
-      <c r="S59" s="35">
+      <c r="I60" s="21"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12">
+        <v>1</v>
+      </c>
+      <c r="M60" s="12">
+        <v>1</v>
+      </c>
+      <c r="N60" s="35">
+        <v>1</v>
+      </c>
+      <c r="O60" s="35">
+        <v>1</v>
+      </c>
+      <c r="P60" s="35"/>
+      <c r="Q60" s="35">
+        <v>1</v>
+      </c>
+      <c r="R60" s="35">
+        <v>1</v>
+      </c>
+      <c r="S60" s="35">
         <v>0.5</v>
       </c>
-      <c r="T59" s="35"/>
-      <c r="U59" s="78">
+      <c r="T60" s="35"/>
+      <c r="U60" s="78">
         <f t="shared" si="0"/>
         <v>2.5</v>
-      </c>
-      <c r="V59" s="15"/>
-      <c r="AA59" s="33"/>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B60" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="C60" s="14">
-        <v>7</v>
-      </c>
-      <c r="E60" s="14">
-        <v>37</v>
-      </c>
-      <c r="G60" s="14">
-        <v>32</v>
-      </c>
-      <c r="H60" s="14">
-        <v>33</v>
-      </c>
-      <c r="I60" s="22"/>
-      <c r="J60" s="36">
-        <v>1</v>
-      </c>
-      <c r="K60" s="2">
-        <v>1</v>
-      </c>
-      <c r="L60" s="2">
-        <v>1</v>
-      </c>
-      <c r="M60" s="20">
-        <v>1</v>
-      </c>
-      <c r="N60" s="36">
-        <v>1</v>
-      </c>
-      <c r="O60" s="36">
-        <v>1</v>
-      </c>
-      <c r="P60" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q60" s="36">
-        <v>1</v>
-      </c>
-      <c r="R60" s="36">
-        <v>1</v>
-      </c>
-      <c r="S60" s="36">
-        <v>1</v>
-      </c>
-      <c r="T60" s="34"/>
-      <c r="U60" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
       </c>
       <c r="V60" s="15"/>
       <c r="AA60" s="33"/>
-      <c r="AB60" s="6"/>
-      <c r="AC60" s="6"/>
-      <c r="AD60" s="6"/>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B61" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C61" s="14">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E61" s="14">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G61" s="14">
+        <v>32</v>
+      </c>
+      <c r="H61" s="14">
         <v>33</v>
-      </c>
-      <c r="H61" s="14">
-        <v>34</v>
       </c>
       <c r="I61" s="22"/>
       <c r="J61" s="36">
@@ -5061,231 +5055,235 @@
       <c r="P61" s="36">
         <v>1</v>
       </c>
+      <c r="Q61" s="36">
+        <v>1</v>
+      </c>
       <c r="R61" s="36">
         <v>1</v>
       </c>
       <c r="S61" s="36">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="T61" s="34"/>
       <c r="U61" s="77">
         <f t="shared" si="0"/>
-        <v>1.9</v>
+        <v>3</v>
       </c>
       <c r="V61" s="15"/>
       <c r="AA61" s="33"/>
+      <c r="AB61" s="6"/>
+      <c r="AC61" s="6"/>
+      <c r="AD61" s="6"/>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C62" s="14">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E62" s="14">
+        <v>38</v>
+      </c>
+      <c r="G62" s="14">
+        <v>33</v>
+      </c>
+      <c r="H62" s="14">
+        <v>34</v>
       </c>
       <c r="I62" s="22"/>
+      <c r="J62" s="36">
+        <v>1</v>
+      </c>
+      <c r="K62" s="2">
+        <v>1</v>
+      </c>
       <c r="L62" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="M62" s="20">
+        <v>1</v>
+      </c>
+      <c r="N62" s="36">
+        <v>1</v>
+      </c>
+      <c r="O62" s="36">
+        <v>1</v>
+      </c>
+      <c r="P62" s="36">
+        <v>1</v>
+      </c>
+      <c r="R62" s="36">
+        <v>1</v>
       </c>
       <c r="S62" s="36">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="T62" s="34"/>
       <c r="U62" s="77">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="V62" s="15"/>
-      <c r="Z62" s="6"/>
       <c r="AA62" s="33"/>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
+      <c r="B63" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="C63" s="14">
+        <v>3</v>
+      </c>
+      <c r="I63" s="22"/>
+      <c r="L63" s="2">
+        <v>0</v>
+      </c>
+      <c r="S63" s="36">
+        <v>0</v>
+      </c>
+      <c r="T63" s="34"/>
+      <c r="U63" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V63" s="15"/>
+      <c r="Z63" s="6"/>
+      <c r="AA63" s="33"/>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A64" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B63" s="26" t="s">
+      <c r="B64" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="C63" s="13">
+      <c r="C64" s="13">
         <v>4</v>
       </c>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13">
+      <c r="D64" s="13"/>
+      <c r="E64" s="13">
         <v>39</v>
       </c>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="21"/>
-      <c r="J63" s="35">
-        <v>1</v>
-      </c>
-      <c r="K63" s="12"/>
-      <c r="L63" s="12">
-        <v>0</v>
-      </c>
-      <c r="M63" s="12"/>
-      <c r="N63" s="35">
-        <v>1</v>
-      </c>
-      <c r="O63" s="35"/>
-      <c r="P63" s="35"/>
-      <c r="Q63" s="35">
-        <v>1</v>
-      </c>
-      <c r="R63" s="35"/>
-      <c r="S63" s="35">
-        <v>0</v>
-      </c>
-      <c r="T63" s="35"/>
-      <c r="U63" s="78">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V63" s="15"/>
-      <c r="AA63" s="33"/>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B64" s="23" t="s">
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="35">
+        <v>1</v>
+      </c>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12">
+        <v>0</v>
+      </c>
+      <c r="M64" s="12"/>
+      <c r="N64" s="35">
+        <v>1</v>
+      </c>
+      <c r="O64" s="35"/>
+      <c r="P64" s="35"/>
+      <c r="Q64" s="35">
+        <v>1</v>
+      </c>
+      <c r="R64" s="35"/>
+      <c r="S64" s="35">
+        <v>0</v>
+      </c>
+      <c r="T64" s="35"/>
+      <c r="U64" s="78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V64" s="15"/>
+      <c r="AA64" s="33"/>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B65" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="C64" s="14">
+      <c r="C65" s="14">
         <v>3</v>
       </c>
-      <c r="E64" s="14">
+      <c r="E65" s="14">
         <v>40</v>
       </c>
-      <c r="I64" s="22"/>
-      <c r="J64" s="36">
-        <v>1</v>
-      </c>
-      <c r="L64" s="2">
-        <v>0</v>
-      </c>
-      <c r="N64" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q64" s="36">
-        <v>1</v>
-      </c>
-      <c r="S64" s="36">
-        <v>0</v>
-      </c>
-      <c r="T64" s="34"/>
-      <c r="U64" s="77">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V64" s="15"/>
-    </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A65" s="11" t="s">
+      <c r="I65" s="22"/>
+      <c r="J65" s="36">
+        <v>1</v>
+      </c>
+      <c r="L65" s="2">
+        <v>0</v>
+      </c>
+      <c r="N65" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="36">
+        <v>1</v>
+      </c>
+      <c r="S65" s="36">
+        <v>0</v>
+      </c>
+      <c r="T65" s="34"/>
+      <c r="U65" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V65" s="15"/>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A66" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="26" t="s">
+      <c r="B66" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C65" s="13">
+      <c r="C66" s="13">
         <v>2</v>
       </c>
-      <c r="D65" s="13">
-        <v>0</v>
-      </c>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="21"/>
-      <c r="J65" s="35"/>
-      <c r="K65" s="12">
-        <v>1</v>
-      </c>
-      <c r="L65" s="12">
-        <v>1</v>
-      </c>
-      <c r="M65" s="12"/>
-      <c r="N65" s="35">
-        <v>1</v>
-      </c>
-      <c r="O65" s="35">
-        <v>1</v>
-      </c>
-      <c r="P65" s="35">
-        <v>1</v>
-      </c>
-      <c r="Q65" s="35">
-        <v>1</v>
-      </c>
-      <c r="R65" s="35">
-        <v>1</v>
-      </c>
-      <c r="S65" s="35">
+      <c r="D66" s="13">
+        <v>0</v>
+      </c>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="12">
+        <v>1</v>
+      </c>
+      <c r="L66" s="12">
+        <v>1</v>
+      </c>
+      <c r="M66" s="12"/>
+      <c r="N66" s="35">
+        <v>1</v>
+      </c>
+      <c r="O66" s="35">
+        <v>1</v>
+      </c>
+      <c r="P66" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="35">
+        <v>1</v>
+      </c>
+      <c r="R66" s="35">
+        <v>1</v>
+      </c>
+      <c r="S66" s="35">
         <v>0.9</v>
       </c>
-      <c r="T65" s="35"/>
-      <c r="U65" s="78">
+      <c r="T66" s="35"/>
+      <c r="U66" s="78">
         <f t="shared" si="0"/>
         <v>2.9</v>
       </c>
-      <c r="V65" s="15"/>
-    </row>
-    <row r="66" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="30"/>
-      <c r="B66" s="31" t="s">
+      <c r="V66" s="15"/>
+    </row>
+    <row r="67" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="30"/>
+      <c r="B67" s="31" t="s">
         <v>82</v>
-      </c>
-      <c r="C66" s="14">
-        <v>2</v>
-      </c>
-      <c r="D66" s="14">
-        <v>1</v>
-      </c>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="22"/>
-      <c r="J66" s="36"/>
-      <c r="K66" s="20"/>
-      <c r="L66" s="20">
-        <v>1</v>
-      </c>
-      <c r="M66" s="20"/>
-      <c r="N66" s="36">
-        <v>1</v>
-      </c>
-      <c r="O66" s="36">
-        <v>1</v>
-      </c>
-      <c r="P66" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q66" s="36">
-        <v>1</v>
-      </c>
-      <c r="R66" s="36">
-        <v>1</v>
-      </c>
-      <c r="S66" s="36">
-        <v>1</v>
-      </c>
-      <c r="T66" s="36"/>
-      <c r="U66" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V66" s="15"/>
-      <c r="W66" s="3"/>
-      <c r="X66"/>
-      <c r="Y66"/>
-      <c r="Z66"/>
-      <c r="AA66"/>
-      <c r="AB66"/>
-      <c r="AC66"/>
-      <c r="AD66"/>
-    </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B67" s="23" t="s">
-        <v>93</v>
       </c>
       <c r="C67" s="14">
         <v>2</v>
@@ -5293,87 +5291,115 @@
       <c r="D67" s="14">
         <v>1</v>
       </c>
-      <c r="I67" s="22" t="s">
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="36"/>
+      <c r="K67" s="20"/>
+      <c r="L67" s="20">
+        <v>1</v>
+      </c>
+      <c r="M67" s="20"/>
+      <c r="N67" s="36">
+        <v>1</v>
+      </c>
+      <c r="O67" s="36">
+        <v>1</v>
+      </c>
+      <c r="P67" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="36">
+        <v>1</v>
+      </c>
+      <c r="R67" s="36">
+        <v>1</v>
+      </c>
+      <c r="S67" s="36">
+        <v>1</v>
+      </c>
+      <c r="T67" s="36"/>
+      <c r="U67" s="77">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V67" s="15"/>
+      <c r="W67" s="3"/>
+      <c r="X67"/>
+      <c r="Y67"/>
+      <c r="Z67"/>
+      <c r="AA67"/>
+      <c r="AB67"/>
+      <c r="AC67"/>
+      <c r="AD67"/>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B68" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" s="14">
+        <v>2</v>
+      </c>
+      <c r="D68" s="14">
+        <v>1</v>
+      </c>
+      <c r="I68" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="K67" s="2">
-        <v>1</v>
-      </c>
-      <c r="L67" s="2">
-        <v>1</v>
-      </c>
-      <c r="T67" s="34"/>
-      <c r="U67" s="77">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V67" s="15"/>
-      <c r="X67" s="33"/>
-      <c r="Z67" s="6"/>
-    </row>
-    <row r="68" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="10"/>
-      <c r="B68" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C68" s="14">
-        <v>4</v>
-      </c>
-      <c r="D68" s="14">
-        <v>3</v>
-      </c>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="22"/>
-      <c r="J68" s="36"/>
       <c r="K68" s="2">
         <v>1</v>
       </c>
       <c r="L68" s="2">
-        <v>1</v>
-      </c>
-      <c r="M68" s="20"/>
-      <c r="N68" s="36">
-        <v>1</v>
-      </c>
-      <c r="O68" s="36">
-        <v>1</v>
-      </c>
-      <c r="P68" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="36">
-        <v>1</v>
-      </c>
-      <c r="R68" s="36">
-        <v>1</v>
-      </c>
-      <c r="S68" s="36">
         <v>1</v>
       </c>
       <c r="T68" s="34"/>
       <c r="U68" s="77">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V68" s="15"/>
+      <c r="X68" s="33"/>
+      <c r="Z68" s="6"/>
+    </row>
+    <row r="69" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="10"/>
+      <c r="B69" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="14">
+        <v>4</v>
+      </c>
+      <c r="D69" s="14">
         <v>3</v>
       </c>
-      <c r="V68" s="15"/>
-      <c r="W68" s="3"/>
-      <c r="Z68" s="6"/>
-    </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B69" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="C69" s="14">
-        <v>1</v>
-      </c>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
       <c r="I69" s="22"/>
-      <c r="K69" s="34"/>
-      <c r="L69" s="34"/>
-      <c r="M69" s="36"/>
+      <c r="J69" s="36"/>
+      <c r="K69" s="2">
+        <v>1</v>
+      </c>
+      <c r="L69" s="2">
+        <v>1</v>
+      </c>
+      <c r="M69" s="20"/>
+      <c r="N69" s="36">
+        <v>1</v>
+      </c>
       <c r="O69" s="36">
+        <v>1</v>
+      </c>
+      <c r="P69" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="36">
+        <v>1</v>
+      </c>
+      <c r="R69" s="36">
         <v>1</v>
       </c>
       <c r="S69" s="36">
@@ -5381,47 +5407,25 @@
       </c>
       <c r="T69" s="34"/>
       <c r="U69" s="77">
-        <f t="shared" ref="U69:U72" si="4">SUM(Q69:T69)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="V69" s="15"/>
-      <c r="AA69" s="6"/>
-      <c r="AB69" s="6"/>
-      <c r="AC69" s="6"/>
-      <c r="AD69" s="6"/>
+      <c r="W69" s="3"/>
+      <c r="Z69" s="6"/>
     </row>
     <row r="70" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B70" s="23" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="C70" s="14">
         <v>1</v>
       </c>
-      <c r="D70" s="14">
-        <v>0</v>
-      </c>
-      <c r="I70" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="L70" s="2">
-        <v>0</v>
-      </c>
-      <c r="M70" s="20">
-        <v>1</v>
-      </c>
-      <c r="N70" s="36">
-        <v>1</v>
-      </c>
+      <c r="I70" s="22"/>
+      <c r="K70" s="34"/>
+      <c r="L70" s="34"/>
+      <c r="M70" s="36"/>
       <c r="O70" s="36">
-        <v>1</v>
-      </c>
-      <c r="P70" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q70" s="36">
-        <v>1</v>
-      </c>
-      <c r="R70" s="36">
         <v>1</v>
       </c>
       <c r="S70" s="36">
@@ -5429,35 +5433,34 @@
       </c>
       <c r="T70" s="34"/>
       <c r="U70" s="77">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" ref="U70:U73" si="2">SUM(Q70:T70)</f>
+        <v>1</v>
       </c>
       <c r="V70" s="15"/>
-    </row>
-    <row r="71" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="10"/>
+      <c r="AA70" s="6"/>
+      <c r="AB70" s="6"/>
+      <c r="AC70" s="6"/>
+      <c r="AD70" s="6"/>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B71" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C71" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D71" s="14">
-        <v>1</v>
-      </c>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="22"/>
-      <c r="J71" s="36"/>
-      <c r="K71" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I71" s="22" t="s">
+        <v>91</v>
       </c>
       <c r="L71" s="2">
-        <v>1</v>
-      </c>
-      <c r="M71" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="M71" s="20">
+        <v>1</v>
+      </c>
       <c r="N71" s="36">
         <v>1</v>
       </c>
@@ -5478,135 +5481,150 @@
       </c>
       <c r="T71" s="34"/>
       <c r="U71" s="77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="V71" s="15"/>
-      <c r="W71" s="3"/>
-      <c r="X71"/>
-      <c r="Y71"/>
-      <c r="Z71"/>
-      <c r="AA71"/>
-      <c r="AB71"/>
-      <c r="AC71"/>
-      <c r="AD71"/>
-    </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B72" s="24" t="s">
+    </row>
+    <row r="72" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="10"/>
+      <c r="B72" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C72" s="14">
+        <v>3</v>
+      </c>
+      <c r="D72" s="14">
+        <v>1</v>
+      </c>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="36"/>
+      <c r="K72" s="2">
+        <v>1</v>
+      </c>
+      <c r="L72" s="2">
+        <v>1</v>
+      </c>
+      <c r="M72" s="20"/>
+      <c r="N72" s="36">
+        <v>1</v>
+      </c>
+      <c r="O72" s="36">
+        <v>1</v>
+      </c>
+      <c r="P72" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q72" s="36">
+        <v>1</v>
+      </c>
+      <c r="R72" s="36">
+        <v>1</v>
+      </c>
+      <c r="S72" s="36">
+        <v>1</v>
+      </c>
+      <c r="T72" s="34"/>
+      <c r="U72" s="77">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="V72" s="15"/>
+      <c r="W72" s="3"/>
+      <c r="X72"/>
+      <c r="Y72"/>
+      <c r="Z72"/>
+      <c r="AA72"/>
+      <c r="AB72"/>
+      <c r="AC72"/>
+      <c r="AD72"/>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B73" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C72" s="27">
+      <c r="C73" s="27">
         <v>4</v>
       </c>
-      <c r="D72" s="27">
-        <v>0</v>
-      </c>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
-      <c r="I72" s="29"/>
-      <c r="J72" s="37"/>
-      <c r="K72" s="28">
-        <v>1</v>
-      </c>
-      <c r="L72" s="28">
-        <v>0</v>
-      </c>
-      <c r="M72" s="28"/>
-      <c r="N72" s="37"/>
-      <c r="O72" s="37"/>
-      <c r="P72" s="37">
-        <v>1</v>
-      </c>
-      <c r="Q72" s="37">
-        <v>1</v>
-      </c>
-      <c r="R72" s="37">
-        <v>1</v>
-      </c>
-      <c r="S72" s="37">
-        <v>0</v>
-      </c>
-      <c r="T72" s="37"/>
-      <c r="U72" s="79">
-        <f t="shared" si="4"/>
+      <c r="D73" s="27">
+        <v>0</v>
+      </c>
+      <c r="E73" s="27"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="27"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="37"/>
+      <c r="K73" s="28">
+        <v>1</v>
+      </c>
+      <c r="L73" s="28">
+        <v>0</v>
+      </c>
+      <c r="M73" s="28"/>
+      <c r="N73" s="37"/>
+      <c r="O73" s="37"/>
+      <c r="P73" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="37">
+        <v>1</v>
+      </c>
+      <c r="R73" s="37">
+        <v>1</v>
+      </c>
+      <c r="S73" s="37">
+        <v>0</v>
+      </c>
+      <c r="T73" s="37"/>
+      <c r="U73" s="79">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="V72" s="15"/>
-    </row>
-    <row r="73" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="11"/>
       <c r="V73" s="15"/>
-      <c r="Y73" s="33"/>
-    </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I74" s="64" t="s">
+    </row>
+    <row r="74" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="11"/>
+      <c r="V74" s="15"/>
+      <c r="Y74" s="33"/>
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I75" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="J74" s="85"/>
-      <c r="K74" s="65"/>
-      <c r="L74" s="65"/>
-      <c r="M74" s="65"/>
-      <c r="N74" s="65"/>
-      <c r="O74" s="65"/>
-      <c r="P74" s="65"/>
-      <c r="Q74" s="65">
-        <f t="array" ref="Q74">SUM($C2:$C72*(Q2:Q72&gt;=0.9)*($U2:$U72&gt;=$W$12))</f>
+      <c r="J75" s="85"/>
+      <c r="K75" s="65"/>
+      <c r="L75" s="65"/>
+      <c r="M75" s="65"/>
+      <c r="N75" s="65"/>
+      <c r="O75" s="65"/>
+      <c r="P75" s="65"/>
+      <c r="Q75" s="65">
+        <f t="array" ref="Q75">SUM($C2:$C73*(Q2:Q73&gt;=0.9)*($U2:$U73&gt;=$W$12))</f>
         <v>185</v>
       </c>
-      <c r="R74" s="65">
-        <f t="array" ref="R74">SUM($C2:$C72*(R2:R72&gt;=0.9)*($U2:$U72&gt;=$W$12))</f>
+      <c r="R75" s="65">
+        <f t="array" ref="R75">SUM($C2:$C73*(R2:R73&gt;=0.9)*($U2:$U73&gt;=$W$12))</f>
         <v>193</v>
       </c>
-      <c r="S74" s="65">
-        <f t="array" ref="S74">SUM($C2:$C72*(S2:S72&gt;=0.9)*($U2:$U72&gt;=$W$12))</f>
-        <v>191</v>
-      </c>
-      <c r="T74" s="66"/>
-      <c r="V74" s="15"/>
-      <c r="AA74" s="6"/>
-      <c r="AB74" s="6"/>
-      <c r="AC74" s="6"/>
-      <c r="AD74" s="6"/>
-    </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I75" s="67" t="s">
+      <c r="S75" s="65">
+        <f t="array" ref="S75">SUM($C2:$C73*(S2:S73&gt;=0.9)*($U2:$U73&gt;=$W$12))</f>
+        <v>195</v>
+      </c>
+      <c r="T75" s="66"/>
+      <c r="V75" s="15"/>
+      <c r="AA75" s="6"/>
+      <c r="AB75" s="6"/>
+      <c r="AC75" s="6"/>
+      <c r="AD75" s="6"/>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I76" s="67" t="s">
         <v>100</v>
-      </c>
-      <c r="J75" s="86"/>
-      <c r="K75" s="68"/>
-      <c r="L75" s="68"/>
-      <c r="M75" s="68"/>
-      <c r="N75" s="68"/>
-      <c r="O75" s="68"/>
-      <c r="P75" s="68"/>
-      <c r="Q75" s="68">
-        <f t="array" ref="Q75">SUM($C2:$C72*Q2:Q72*($U2:$U72&gt;=$W$12))</f>
-        <v>192</v>
-      </c>
-      <c r="R75" s="68">
-        <f t="array" ref="R75">SUM($C2:$C72*R2:R72*($U2:$U72&gt;=$W$12))</f>
-        <v>212.6</v>
-      </c>
-      <c r="S75" s="68">
-        <f t="array" ref="S75">SUM($C2:$C72*S2:S72*($U2:$U72&gt;=$W$12))</f>
-        <v>204.23</v>
-      </c>
-      <c r="T75" s="69"/>
-      <c r="V75" s="15"/>
-    </row>
-    <row r="76" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="10"/>
-      <c r="B76" s="23"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="67" t="s">
-        <v>99</v>
       </c>
       <c r="J76" s="86"/>
       <c r="K76" s="68"/>
@@ -5616,32 +5634,31 @@
       <c r="O76" s="68"/>
       <c r="P76" s="68"/>
       <c r="Q76" s="68">
-        <f t="array" ref="Q76">SUM($C$2:$C$72*(Q$2:Q$72&gt;=0.1)*($U$2:$U$72&gt;=$W$12))</f>
-        <v>199</v>
+        <f t="array" ref="Q76">SUM($C2:$C73*Q2:Q73*($U2:$U73&gt;=$W$12))</f>
+        <v>192</v>
       </c>
       <c r="R76" s="68">
-        <f t="array" ref="R76">SUM($C$2:$C$72*(R$2:R$72&gt;=0.1)*($U$2:$U$72&gt;=$W$12))</f>
-        <v>222</v>
+        <f t="array" ref="R76">SUM($C2:$C73*R2:R73*($U2:$U73&gt;=$W$12))</f>
+        <v>212.6</v>
       </c>
       <c r="S76" s="68">
-        <f t="array" ref="S76">SUM($C$2:$C$72*(S$2:S$72&gt;=0.1)*($U$2:$U$72&gt;=$W$12))</f>
-        <v>214</v>
+        <f t="array" ref="S76">SUM($C2:$C73*S2:S73*($U2:$U73&gt;=$W$12))</f>
+        <v>208.23</v>
       </c>
       <c r="T76" s="69"/>
-      <c r="U76" s="3"/>
       <c r="V76" s="15"/>
-      <c r="W76" s="3"/>
-      <c r="X76"/>
-      <c r="Y76"/>
-      <c r="Z76"/>
-      <c r="AA76"/>
-      <c r="AB76"/>
-      <c r="AC76"/>
-      <c r="AD76"/>
-    </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="10"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
       <c r="I77" s="67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J77" s="86"/>
       <c r="K77" s="68"/>
@@ -5651,92 +5668,118 @@
       <c r="O77" s="68"/>
       <c r="P77" s="68"/>
       <c r="Q77" s="68">
-        <f t="shared" ref="Q77:S77" si="5">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>233</v>
+        <f t="array" ref="Q77">SUM($C$2:$C$73*(Q$2:Q$73&gt;=0.1)*($U$2:$U$73&gt;=$W$12))</f>
+        <v>199</v>
       </c>
       <c r="R77" s="68">
-        <f t="shared" si="5"/>
-        <v>233</v>
+        <f t="array" ref="R77">SUM($C$2:$C$73*(R$2:R$73&gt;=0.1)*($U$2:$U$73&gt;=$W$12))</f>
+        <v>222</v>
       </c>
       <c r="S77" s="68">
-        <f t="shared" si="5"/>
-        <v>233</v>
+        <f t="array" ref="S77">SUM($C$2:$C$73*(S$2:S$73&gt;=0.1)*($U$2:$U$73&gt;=$W$12))</f>
+        <v>218</v>
       </c>
       <c r="T77" s="69"/>
+      <c r="U77" s="3"/>
       <c r="V77" s="15"/>
-      <c r="AA77" s="6"/>
-      <c r="AB77" s="6"/>
-      <c r="AC77" s="6"/>
-      <c r="AD77" s="6"/>
+      <c r="W77" s="3"/>
+      <c r="X77"/>
+      <c r="Y77"/>
+      <c r="Z77"/>
+      <c r="AA77"/>
+      <c r="AB77"/>
+      <c r="AC77"/>
+      <c r="AD77"/>
     </row>
     <row r="78" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I78" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="J78" s="86"/>
+      <c r="K78" s="68"/>
+      <c r="L78" s="68"/>
+      <c r="M78" s="68"/>
+      <c r="N78" s="68"/>
+      <c r="O78" s="68"/>
+      <c r="P78" s="68"/>
+      <c r="Q78" s="68">
+        <f t="shared" ref="Q78:S78" si="3">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>237</v>
+      </c>
+      <c r="R78" s="68">
+        <f t="shared" si="3"/>
+        <v>237</v>
+      </c>
+      <c r="S78" s="68">
+        <f t="shared" si="3"/>
+        <v>237</v>
+      </c>
+      <c r="T78" s="69"/>
+      <c r="V78" s="15"/>
+      <c r="AA78" s="6"/>
+      <c r="AB78" s="6"/>
+      <c r="AC78" s="6"/>
+      <c r="AD78" s="6"/>
+    </row>
+    <row r="79" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I79" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="J78" s="86"/>
-      <c r="K78" s="70"/>
-      <c r="L78" s="70"/>
-      <c r="M78" s="70"/>
-      <c r="N78" s="70"/>
-      <c r="O78" s="70"/>
-      <c r="P78" s="70"/>
-      <c r="Q78" s="70">
-        <f t="shared" ref="Q78:S78" si="6">Q75/Q77</f>
-        <v>0.82403433476394849</v>
-      </c>
-      <c r="R78" s="70">
-        <f t="shared" si="6"/>
-        <v>0.9124463519313305</v>
-      </c>
-      <c r="S78" s="70">
-        <f t="shared" si="6"/>
-        <v>0.87652360515021455</v>
-      </c>
-      <c r="T78" s="71"/>
-      <c r="V78" s="15"/>
-    </row>
-    <row r="79" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C79" s="33"/>
-      <c r="I79" s="72" t="s">
+      <c r="J79" s="86"/>
+      <c r="K79" s="70"/>
+      <c r="L79" s="70"/>
+      <c r="M79" s="70"/>
+      <c r="N79" s="70"/>
+      <c r="O79" s="70"/>
+      <c r="P79" s="70"/>
+      <c r="Q79" s="70">
+        <f t="shared" ref="Q79:S79" si="4">Q76/Q78</f>
+        <v>0.810126582278481</v>
+      </c>
+      <c r="R79" s="70">
+        <f t="shared" si="4"/>
+        <v>0.89704641350210967</v>
+      </c>
+      <c r="S79" s="70">
+        <f t="shared" si="4"/>
+        <v>0.87860759493670881</v>
+      </c>
+      <c r="T79" s="71"/>
+      <c r="V79" s="15"/>
+    </row>
+    <row r="80" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C80" s="33"/>
+      <c r="I80" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="J79" s="87"/>
-      <c r="K79" s="73"/>
-      <c r="L79" s="73"/>
-      <c r="M79" s="73"/>
-      <c r="N79" s="73"/>
-      <c r="O79" s="73"/>
-      <c r="P79" s="73"/>
-      <c r="Q79" s="73">
-        <f t="shared" ref="Q79:S79" si="7">Q77-Q75</f>
-        <v>41</v>
-      </c>
-      <c r="R79" s="73">
-        <f t="shared" si="7"/>
-        <v>20.400000000000006</v>
-      </c>
-      <c r="S79" s="73">
-        <f t="shared" si="7"/>
+      <c r="J80" s="87"/>
+      <c r="K80" s="73"/>
+      <c r="L80" s="73"/>
+      <c r="M80" s="73"/>
+      <c r="N80" s="73"/>
+      <c r="O80" s="73"/>
+      <c r="P80" s="73"/>
+      <c r="Q80" s="73">
+        <f t="shared" ref="Q80:S80" si="5">Q78-Q76</f>
+        <v>45</v>
+      </c>
+      <c r="R80" s="73">
+        <f t="shared" si="5"/>
+        <v>24.400000000000006</v>
+      </c>
+      <c r="S80" s="73">
+        <f t="shared" si="5"/>
         <v>28.77000000000001</v>
       </c>
-      <c r="T79" s="74"/>
-      <c r="V79" s="15"/>
-      <c r="AA79" s="6"/>
-      <c r="AB79" s="6"/>
-      <c r="AC79" s="6"/>
-      <c r="AD79" s="6"/>
-    </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="C80" s="33"/>
+      <c r="T80" s="74"/>
       <c r="V80" s="15"/>
+      <c r="AA80" s="6"/>
+      <c r="AB80" s="6"/>
+      <c r="AC80" s="6"/>
+      <c r="AD80" s="6"/>
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C81" s="33"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="14"/>
-      <c r="K81" s="14"/>
-      <c r="L81" s="14"/>
-      <c r="N81" s="14"/>
       <c r="V81" s="15"/>
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.3">
@@ -5749,6 +5792,7 @@
       <c r="V82" s="15"/>
     </row>
     <row r="83" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C83" s="33"/>
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
       <c r="K83" s="14"/>
@@ -5763,7 +5807,6 @@
       <c r="L84" s="14"/>
       <c r="N84" s="14"/>
       <c r="V84" s="15"/>
-      <c r="Z84" s="33"/>
     </row>
     <row r="85" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I85" s="14"/>
@@ -5772,6 +5815,7 @@
       <c r="L85" s="14"/>
       <c r="N85" s="14"/>
       <c r="V85" s="15"/>
+      <c r="Z85" s="33"/>
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I86" s="14"/>
@@ -5779,6 +5823,7 @@
       <c r="K86" s="14"/>
       <c r="L86" s="14"/>
       <c r="N86" s="14"/>
+      <c r="V86" s="15"/>
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I87" s="14"/>
@@ -5794,64 +5839,71 @@
       <c r="L88" s="14"/>
       <c r="N88" s="14"/>
     </row>
-    <row r="89" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="10"/>
-      <c r="B89" s="23"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="20"/>
-      <c r="J89" s="36"/>
-      <c r="K89" s="2"/>
-      <c r="L89" s="2"/>
-      <c r="M89" s="20"/>
-      <c r="N89" s="36"/>
-      <c r="O89" s="36"/>
-      <c r="P89" s="36"/>
-      <c r="Q89" s="36"/>
-      <c r="R89" s="36"/>
-      <c r="S89" s="36"/>
-      <c r="T89" s="2"/>
-      <c r="U89" s="3"/>
-      <c r="V89" s="3"/>
-      <c r="W89" s="3"/>
-      <c r="X89"/>
-      <c r="Y89"/>
-      <c r="Z89"/>
-      <c r="AA89"/>
-      <c r="AB89"/>
-      <c r="AC89"/>
-      <c r="AD89"/>
-    </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA92" s="6"/>
-      <c r="AB92" s="6"/>
-      <c r="AC92" s="6"/>
-      <c r="AD92" s="6"/>
-    </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA96" s="6"/>
-      <c r="AB96" s="6"/>
-      <c r="AC96" s="6"/>
-      <c r="AD96" s="6"/>
-    </row>
-    <row r="101" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA101" s="6"/>
-      <c r="AB101" s="6"/>
-      <c r="AC101" s="6"/>
-      <c r="AD101" s="6"/>
-    </row>
-    <row r="114" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA114" s="33"/>
-      <c r="AB114" s="33"/>
-      <c r="AC114" s="33"/>
-      <c r="AD114" s="33"/>
+    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
+      <c r="N89" s="14"/>
+    </row>
+    <row r="90" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="10"/>
+      <c r="B90" s="23"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="20"/>
+      <c r="J90" s="36"/>
+      <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
+      <c r="M90" s="20"/>
+      <c r="N90" s="36"/>
+      <c r="O90" s="36"/>
+      <c r="P90" s="36"/>
+      <c r="Q90" s="36"/>
+      <c r="R90" s="36"/>
+      <c r="S90" s="36"/>
+      <c r="T90" s="2"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
+      <c r="W90" s="3"/>
+      <c r="X90"/>
+      <c r="Y90"/>
+      <c r="Z90"/>
+      <c r="AA90"/>
+      <c r="AB90"/>
+      <c r="AC90"/>
+      <c r="AD90"/>
+    </row>
+    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA93" s="6"/>
+      <c r="AB93" s="6"/>
+      <c r="AC93" s="6"/>
+      <c r="AD93" s="6"/>
+    </row>
+    <row r="97" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA97" s="6"/>
+      <c r="AB97" s="6"/>
+      <c r="AC97" s="6"/>
+      <c r="AD97" s="6"/>
+    </row>
+    <row r="102" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA102" s="6"/>
+      <c r="AB102" s="6"/>
+      <c r="AC102" s="6"/>
+      <c r="AD102" s="6"/>
+    </row>
+    <row r="115" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA115" s="33"/>
+      <c r="AB115" s="33"/>
+      <c r="AC115" s="33"/>
+      <c r="AD115" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U72">
+  <conditionalFormatting sqref="B2:U73">
     <cfRule type="expression" dxfId="2" priority="37" stopIfTrue="1">
       <formula>$U2&gt;=(0.5+$W$12)</formula>
     </cfRule>

</xml_diff>

<commit_message>
New Lab: Drag Force and Terminal Velocity
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="200">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -781,6 +781,9 @@
   </si>
   <si>
     <t>Tangential Acceleration and Centripetal Acceleration</t>
+  </si>
+  <si>
+    <t>Drag Force and Terminal Velocity [coffee filters]</t>
   </si>
 </sst>
 </file>
@@ -1995,10 +1998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD115"/>
+  <dimension ref="A1:AD116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2202,7 +2205,7 @@
       </c>
       <c r="T3" s="60"/>
       <c r="U3" s="76">
-        <f t="shared" ref="U3:U69" si="0">SUM(Q3:T3)</f>
+        <f t="shared" ref="U3:U70" si="0">SUM(Q3:T3)</f>
         <v>3</v>
       </c>
       <c r="V3" s="80"/>
@@ -3103,16 +3106,16 @@
         <v>0</v>
       </c>
       <c r="X23" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W23,C$2:C$74)</f>
-        <v>307</v>
+        <f t="shared" ref="X23:X31" si="1">SUMIF(U$2:U$75,"&gt;=" &amp; W23,C$2:C$75)</f>
+        <v>310</v>
       </c>
       <c r="Y23" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W23,D$2:D$74)</f>
+        <f t="shared" ref="Y23:Y31" si="2">SUMIF(U$2:U$75,"&gt;=" &amp; W23,D$2:D$75)</f>
         <v>11</v>
       </c>
       <c r="Z23" s="8">
-        <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
-        <v>28.145000000000003</v>
+        <f t="shared" ref="Z23:Z31" si="3">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
+        <v>28.340000000000003</v>
       </c>
       <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
@@ -3179,16 +3182,16 @@
         <v>0.5</v>
       </c>
       <c r="X24" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W24,C$2:C$74)</f>
-        <v>277</v>
+        <f t="shared" si="1"/>
+        <v>280</v>
       </c>
       <c r="Y24" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W24,D$2:D$74)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z24" s="8">
-        <f t="shared" si="1"/>
-        <v>25.805000000000003</v>
+        <f t="shared" si="3"/>
+        <v>26</v>
       </c>
       <c r="AA24" s="33"/>
       <c r="AB24" s="33"/>
@@ -3239,16 +3242,16 @@
         <v>1</v>
       </c>
       <c r="X25" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W25,C$2:C$74)</f>
-        <v>237</v>
+        <f t="shared" si="1"/>
+        <v>240</v>
       </c>
       <c r="Y25" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W25,D$2:D$74)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z25" s="8">
-        <f t="shared" si="1"/>
-        <v>23.205000000000002</v>
+        <f t="shared" si="3"/>
+        <v>23.400000000000002</v>
       </c>
       <c r="AA25" s="33"/>
       <c r="AB25" s="33"/>
@@ -3309,16 +3312,16 @@
         <v>1.5</v>
       </c>
       <c r="X26" s="31">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W26,C$2:C$74)</f>
-        <v>221</v>
+        <f t="shared" si="1"/>
+        <v>227</v>
       </c>
       <c r="Y26" s="31">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W26,D$2:D$74)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z26" s="8">
-        <f t="shared" si="1"/>
-        <v>22.165000000000003</v>
+        <f t="shared" si="3"/>
+        <v>22.555000000000003</v>
       </c>
       <c r="AA26" s="33"/>
       <c r="AB26" s="33"/>
@@ -3387,16 +3390,16 @@
         <v>2</v>
       </c>
       <c r="X27" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W27,C$2:C$74)</f>
-        <v>204</v>
+        <f t="shared" si="1"/>
+        <v>210</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W27,D$2:D$74)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z27" s="8">
-        <f t="shared" si="1"/>
-        <v>21.060000000000006</v>
+        <f t="shared" si="3"/>
+        <v>21.45</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
@@ -3450,16 +3453,16 @@
         <v>2.5</v>
       </c>
       <c r="X28" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W28,C$2:C$74)</f>
-        <v>162</v>
+        <f t="shared" si="1"/>
+        <v>168</v>
       </c>
       <c r="Y28" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W28,D$2:D$74)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z28" s="8">
-        <f t="shared" si="1"/>
-        <v>18.330000000000002</v>
+        <f t="shared" si="3"/>
+        <v>18.720000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
@@ -3492,16 +3495,16 @@
         <v>3</v>
       </c>
       <c r="X29" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W29,C$2:C$74)</f>
-        <v>149</v>
+        <f t="shared" si="1"/>
+        <v>155</v>
       </c>
       <c r="Y29" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W29,D$2:D$74)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="Z29" s="8">
-        <f t="shared" si="1"/>
-        <v>17.094999999999999</v>
+        <f t="shared" si="3"/>
+        <v>17.484999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
@@ -3553,15 +3556,15 @@
         <v>3.5</v>
       </c>
       <c r="X30" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W30,C$2:C$74)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y30" s="6">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W30,D$2:D$74)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z30" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -3593,15 +3596,15 @@
         <v>4</v>
       </c>
       <c r="X31" s="47">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W31,C$2:C$74)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y31" s="47">
-        <f>SUMIF(U$2:U$74,"&gt;=" &amp; W31,D$2:D$74)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z31" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -3785,84 +3788,66 @@
       <c r="V35" s="15"/>
       <c r="W35" s="84"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
       <c r="B36" s="23" t="s">
-        <v>148</v>
+        <v>199</v>
       </c>
       <c r="C36" s="14">
-        <v>5</v>
-      </c>
-      <c r="E36" s="14">
-        <v>19</v>
-      </c>
-      <c r="G36" s="14">
-        <v>15</v>
-      </c>
-      <c r="H36" s="14">
-        <v>15</v>
-      </c>
-      <c r="I36" s="22"/>
-      <c r="K36" s="34">
-        <v>1</v>
-      </c>
-      <c r="L36" s="34">
-        <v>1</v>
-      </c>
-      <c r="M36" s="36">
-        <v>1</v>
-      </c>
-      <c r="N36" s="36">
-        <v>1</v>
-      </c>
-      <c r="O36" s="36">
-        <v>1</v>
-      </c>
-      <c r="P36" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="36">
-        <v>1</v>
-      </c>
-      <c r="R36" s="36">
-        <v>0.75</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="J36" s="36"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36"/>
+      <c r="R36" s="36"/>
       <c r="S36" s="36">
-        <v>0</v>
-      </c>
-      <c r="T36" s="34"/>
+        <v>1</v>
+      </c>
+      <c r="T36" s="34">
+        <v>2</v>
+      </c>
       <c r="U36" s="77">
         <f t="shared" si="0"/>
-        <v>1.75</v>
+        <v>3</v>
       </c>
       <c r="V36" s="15"/>
       <c r="W36" s="84"/>
     </row>
-    <row r="37" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C37" s="14">
-        <v>8</v>
-      </c>
-      <c r="D37" s="14"/>
+        <v>5</v>
+      </c>
       <c r="E37" s="14">
-        <v>20</v>
-      </c>
-      <c r="F37" s="14"/>
+        <v>19</v>
+      </c>
       <c r="G37" s="14">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H37" s="14">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I37" s="22"/>
-      <c r="J37" s="36"/>
       <c r="K37" s="34">
         <v>1</v>
       </c>
       <c r="L37" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M37" s="36">
         <v>1</v>
@@ -3880,76 +3865,107 @@
         <v>1</v>
       </c>
       <c r="R37" s="36">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="S37" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T37" s="34"/>
       <c r="U37" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1.75</v>
       </c>
       <c r="V37" s="15"/>
       <c r="W37" s="84"/>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
       <c r="B38" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C38" s="14">
-        <v>4</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14">
+        <v>20</v>
+      </c>
+      <c r="F38" s="14"/>
       <c r="G38" s="14">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H38" s="14">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I38" s="22"/>
-      <c r="J38" s="36">
+      <c r="J38" s="36"/>
+      <c r="K38" s="34">
+        <v>1</v>
+      </c>
+      <c r="L38" s="34">
         <v>0.5</v>
       </c>
-      <c r="K38" s="34"/>
-      <c r="L38" s="34">
-        <v>0.8</v>
-      </c>
       <c r="M38" s="36">
         <v>1</v>
       </c>
       <c r="N38" s="36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O38" s="36">
         <v>1</v>
       </c>
+      <c r="P38" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="36">
+        <v>1</v>
+      </c>
       <c r="R38" s="36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S38" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T38" s="34"/>
       <c r="U38" s="77">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="V38" s="15"/>
       <c r="W38" s="84"/>
-      <c r="Z38" s="6"/>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B39" s="23" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
       <c r="C39" s="14">
         <v>4</v>
       </c>
-      <c r="I39" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="P39" s="36">
-        <v>1</v>
+      <c r="G39" s="14">
+        <v>17</v>
+      </c>
+      <c r="H39" s="14">
+        <v>17</v>
+      </c>
+      <c r="I39" s="22"/>
+      <c r="J39" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34">
+        <v>0.8</v>
+      </c>
+      <c r="M39" s="36">
+        <v>1</v>
+      </c>
+      <c r="N39" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="O39" s="36">
+        <v>1</v>
+      </c>
+      <c r="R39" s="36">
+        <v>0.5</v>
       </c>
       <c r="S39" s="36">
         <v>0</v>
@@ -3957,155 +3973,118 @@
       <c r="T39" s="34"/>
       <c r="U39" s="77">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V39" s="15"/>
+      <c r="W39" s="84"/>
+      <c r="Z39" s="6"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
+      <c r="B40" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C40" s="14">
+        <v>4</v>
+      </c>
+      <c r="I40" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="P40" s="36">
+        <v>1</v>
+      </c>
+      <c r="S40" s="36">
+        <v>0</v>
+      </c>
+      <c r="T40" s="34"/>
+      <c r="U40" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V40" s="15"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B41" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="C40" s="13">
+      <c r="C41" s="13">
         <v>7</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D41" s="13">
         <v>2</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E41" s="13">
         <v>21</v>
       </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13">
+      <c r="F41" s="13"/>
+      <c r="G41" s="13">
         <v>18</v>
       </c>
-      <c r="H40" s="13">
+      <c r="H41" s="13">
         <v>18</v>
       </c>
-      <c r="I40" s="21"/>
-      <c r="J40" s="35">
-        <v>1</v>
-      </c>
-      <c r="K40" s="12">
-        <v>1</v>
-      </c>
-      <c r="L40" s="12">
-        <v>1</v>
-      </c>
-      <c r="M40" s="12">
-        <v>1</v>
-      </c>
-      <c r="N40" s="35">
-        <v>1</v>
-      </c>
-      <c r="O40" s="35">
-        <v>1</v>
-      </c>
-      <c r="P40" s="35">
-        <v>1</v>
-      </c>
-      <c r="Q40" s="35">
-        <v>1</v>
-      </c>
-      <c r="R40" s="35">
-        <v>1</v>
-      </c>
-      <c r="S40" s="35">
-        <v>1</v>
-      </c>
-      <c r="T40" s="35"/>
-      <c r="U40" s="78">
+      <c r="I41" s="21"/>
+      <c r="J41" s="35">
+        <v>1</v>
+      </c>
+      <c r="K41" s="12">
+        <v>1</v>
+      </c>
+      <c r="L41" s="12">
+        <v>1</v>
+      </c>
+      <c r="M41" s="12">
+        <v>1</v>
+      </c>
+      <c r="N41" s="35">
+        <v>1</v>
+      </c>
+      <c r="O41" s="35">
+        <v>1</v>
+      </c>
+      <c r="P41" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="35">
+        <v>1</v>
+      </c>
+      <c r="R41" s="35">
+        <v>1</v>
+      </c>
+      <c r="S41" s="35">
+        <v>1</v>
+      </c>
+      <c r="T41" s="35"/>
+      <c r="U41" s="78">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="V40" s="15"/>
-      <c r="W40" s="15"/>
-      <c r="X40" s="6"/>
-    </row>
-    <row r="41" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="30"/>
-      <c r="B41" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="14">
-        <v>6</v>
-      </c>
-      <c r="D41" s="14">
-        <v>1</v>
-      </c>
-      <c r="E41" s="14">
-        <v>22</v>
-      </c>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14">
-        <v>19</v>
-      </c>
-      <c r="H41" s="14">
-        <v>19</v>
-      </c>
-      <c r="I41" s="22"/>
-      <c r="J41" s="36">
-        <v>1</v>
-      </c>
-      <c r="K41" s="36">
-        <v>1</v>
-      </c>
-      <c r="L41" s="36">
-        <v>0.75</v>
-      </c>
-      <c r="M41" s="36">
-        <v>1</v>
-      </c>
-      <c r="N41" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="O41" s="36">
-        <v>1</v>
-      </c>
-      <c r="P41" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="36">
-        <v>1</v>
-      </c>
-      <c r="R41" s="36">
-        <v>1</v>
-      </c>
-      <c r="S41" s="36">
-        <v>1</v>
-      </c>
-      <c r="T41" s="36"/>
-      <c r="U41" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
       <c r="V41" s="15"/>
-      <c r="W41" s="3"/>
-      <c r="X41"/>
-      <c r="Y41"/>
-      <c r="AA41"/>
-      <c r="AB41"/>
-      <c r="AC41"/>
-      <c r="AD41"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W41" s="15"/>
+      <c r="X41" s="6"/>
+    </row>
+    <row r="42" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="30"/>
       <c r="B42" s="31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C42" s="14">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="D42" s="14">
+        <v>1</v>
       </c>
       <c r="E42" s="14">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F42" s="14"/>
       <c r="G42" s="14">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H42" s="14">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I42" s="22"/>
       <c r="J42" s="36">
@@ -4115,7 +4094,7 @@
         <v>1</v>
       </c>
       <c r="L42" s="36">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="M42" s="36">
         <v>1</v>
@@ -4144,122 +4123,133 @@
         <v>3</v>
       </c>
       <c r="V42" s="15"/>
-      <c r="AA42" s="6"/>
-      <c r="AB42" s="6"/>
-      <c r="AC42" s="6"/>
-      <c r="AD42" s="6"/>
+      <c r="W42" s="3"/>
+      <c r="X42"/>
+      <c r="Y42"/>
+      <c r="AA42"/>
+      <c r="AB42"/>
+      <c r="AC42"/>
+      <c r="AD42"/>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A43" s="30"/>
       <c r="B43" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C43" s="14">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E43" s="14">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="G43" s="14">
+        <v>20</v>
+      </c>
+      <c r="H43" s="14">
+        <v>20</v>
       </c>
       <c r="I43" s="22"/>
-      <c r="K43" s="36"/>
+      <c r="J43" s="36">
+        <v>1</v>
+      </c>
+      <c r="K43" s="36">
+        <v>1</v>
+      </c>
       <c r="L43" s="36">
-        <v>1</v>
-      </c>
-      <c r="M43" s="36"/>
+        <v>0.5</v>
+      </c>
+      <c r="M43" s="36">
+        <v>1</v>
+      </c>
+      <c r="N43" s="36">
+        <v>0.5</v>
+      </c>
       <c r="O43" s="36">
         <v>1</v>
       </c>
+      <c r="P43" s="36">
+        <v>1</v>
+      </c>
       <c r="Q43" s="36">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="R43" s="36">
+        <v>1</v>
       </c>
       <c r="S43" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T43" s="36"/>
       <c r="U43" s="77">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="V43" s="15"/>
-      <c r="Z43" s="6"/>
+      <c r="AA43" s="6"/>
+      <c r="AB43" s="6"/>
+      <c r="AC43" s="6"/>
+      <c r="AD43" s="6"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A44" s="30"/>
       <c r="B44" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C44" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E44" s="14">
-        <v>25</v>
-      </c>
-      <c r="G44" s="14">
-        <v>21</v>
-      </c>
-      <c r="H44" s="14">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I44" s="22"/>
-      <c r="J44" s="36">
-        <v>1</v>
-      </c>
-      <c r="K44" s="36">
-        <v>1</v>
-      </c>
+      <c r="K44" s="36"/>
       <c r="L44" s="36">
-        <v>0</v>
-      </c>
-      <c r="M44" s="36">
-        <v>1</v>
-      </c>
-      <c r="N44" s="36">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M44" s="36"/>
       <c r="O44" s="36">
         <v>1</v>
       </c>
-      <c r="P44" s="36">
-        <v>1</v>
-      </c>
-      <c r="R44" s="36">
-        <v>1</v>
+      <c r="Q44" s="36">
+        <v>0.5</v>
       </c>
       <c r="S44" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T44" s="36"/>
       <c r="U44" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="6"/>
+      <c r="Z44" s="6"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A45" s="30"/>
       <c r="B45" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C45" s="14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E45" s="14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G45" s="14">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H45" s="14">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I45" s="22"/>
+      <c r="J45" s="36">
+        <v>1</v>
+      </c>
       <c r="K45" s="36">
         <v>1</v>
       </c>
       <c r="L45" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45" s="36">
         <v>1</v>
@@ -4271,9 +4261,6 @@
         <v>1</v>
       </c>
       <c r="P45" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q45" s="36">
         <v>1</v>
       </c>
       <c r="R45" s="36">
@@ -4285,37 +4272,35 @@
       <c r="T45" s="36"/>
       <c r="U45" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V45" s="15"/>
-      <c r="Y45" s="6"/>
-    </row>
-    <row r="46" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="W45" s="15"/>
+      <c r="X45" s="6"/>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A46" s="30"/>
       <c r="B46" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C46" s="14">
-        <v>4</v>
-      </c>
-      <c r="D46" s="14"/>
+        <v>6</v>
+      </c>
       <c r="E46" s="14">
-        <v>27</v>
-      </c>
-      <c r="F46" s="14"/>
+        <v>26</v>
+      </c>
       <c r="G46" s="14">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H46" s="14">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I46" s="22"/>
-      <c r="J46" s="36"/>
       <c r="K46" s="36">
         <v>1</v>
       </c>
       <c r="L46" s="36">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="M46" s="36">
         <v>1</v>
@@ -4344,41 +4329,34 @@
         <v>3</v>
       </c>
       <c r="V46" s="15"/>
-      <c r="W46" s="3"/>
-      <c r="X46"/>
-      <c r="Y46"/>
-      <c r="Z46"/>
-      <c r="AA46"/>
-      <c r="AB46"/>
-      <c r="AC46"/>
-      <c r="AD46"/>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y46" s="6"/>
+    </row>
+    <row r="47" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30"/>
       <c r="B47" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C47" s="14">
-        <v>7</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D47" s="14"/>
       <c r="E47" s="14">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F47" s="14"/>
       <c r="G47" s="14">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H47" s="14">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I47" s="22"/>
-      <c r="J47" s="36">
-        <v>1</v>
-      </c>
+      <c r="J47" s="36"/>
       <c r="K47" s="36">
         <v>1</v>
       </c>
       <c r="L47" s="36">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="M47" s="36">
         <v>1</v>
@@ -4407,31 +4385,41 @@
         <v>3</v>
       </c>
       <c r="V47" s="15"/>
+      <c r="W47" s="3"/>
+      <c r="X47"/>
+      <c r="Y47"/>
+      <c r="Z47"/>
+      <c r="AA47"/>
+      <c r="AB47"/>
+      <c r="AC47"/>
+      <c r="AD47"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A48" s="30"/>
       <c r="B48" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C48" s="14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E48" s="14">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G48" s="14">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H48" s="14">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I48" s="22"/>
       <c r="J48" s="36">
         <v>1</v>
       </c>
-      <c r="K48" s="36"/>
+      <c r="K48" s="36">
+        <v>1</v>
+      </c>
       <c r="L48" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M48" s="36">
         <v>1</v>
@@ -4443,7 +4431,7 @@
         <v>1</v>
       </c>
       <c r="P48" s="36">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="Q48" s="36">
         <v>1</v>
@@ -4461,440 +4449,462 @@
       </c>
       <c r="V48" s="15"/>
     </row>
-    <row r="49" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="10"/>
-      <c r="B49" s="23" t="s">
-        <v>160</v>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A49" s="30"/>
+      <c r="B49" s="31" t="s">
+        <v>159</v>
       </c>
       <c r="C49" s="14">
-        <v>5</v>
-      </c>
-      <c r="D49" s="14"/>
+        <v>6</v>
+      </c>
       <c r="E49" s="14">
-        <v>30</v>
-      </c>
-      <c r="F49" s="14"/>
+        <v>29</v>
+      </c>
       <c r="G49" s="14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H49" s="14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I49" s="22"/>
       <c r="J49" s="36">
         <v>1</v>
       </c>
-      <c r="K49" s="2">
+      <c r="K49" s="36"/>
+      <c r="L49" s="36">
+        <v>0</v>
+      </c>
+      <c r="M49" s="36">
+        <v>1</v>
+      </c>
+      <c r="N49" s="36">
+        <v>1</v>
+      </c>
+      <c r="O49" s="36">
+        <v>1</v>
+      </c>
+      <c r="P49" s="36">
+        <v>0.75</v>
+      </c>
+      <c r="Q49" s="36">
+        <v>1</v>
+      </c>
+      <c r="R49" s="36">
+        <v>1</v>
+      </c>
+      <c r="S49" s="36">
+        <v>1</v>
+      </c>
+      <c r="T49" s="36"/>
+      <c r="U49" s="77">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V49" s="15"/>
+    </row>
+    <row r="50" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="10"/>
+      <c r="B50" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="14">
+        <v>5</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14">
+        <v>30</v>
+      </c>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14">
+        <v>26</v>
+      </c>
+      <c r="H50" s="14">
+        <v>26</v>
+      </c>
+      <c r="I50" s="22"/>
+      <c r="J50" s="36">
+        <v>1</v>
+      </c>
+      <c r="K50" s="2">
         <v>0.5</v>
       </c>
-      <c r="L49" s="2">
-        <v>1</v>
-      </c>
-      <c r="M49" s="20">
-        <v>1</v>
-      </c>
-      <c r="N49" s="36">
+      <c r="L50" s="2">
+        <v>1</v>
+      </c>
+      <c r="M50" s="20">
+        <v>1</v>
+      </c>
+      <c r="N50" s="36">
         <v>0.5</v>
       </c>
-      <c r="O49" s="36">
-        <v>1</v>
-      </c>
-      <c r="P49" s="36">
+      <c r="O50" s="36">
+        <v>1</v>
+      </c>
+      <c r="P50" s="36">
         <v>0.5</v>
       </c>
-      <c r="Q49" s="36">
+      <c r="Q50" s="36">
         <v>0.5</v>
       </c>
-      <c r="R49" s="36">
+      <c r="R50" s="36">
         <v>0.5</v>
       </c>
-      <c r="S49" s="36">
-        <v>1</v>
-      </c>
-      <c r="T49" s="34"/>
-      <c r="U49" s="77">
+      <c r="S50" s="36">
+        <v>1</v>
+      </c>
+      <c r="T50" s="34"/>
+      <c r="U50" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="V49" s="15"/>
-      <c r="W49" s="15"/>
-      <c r="Z49"/>
-      <c r="AA49"/>
-      <c r="AB49"/>
-      <c r="AC49"/>
-      <c r="AD49"/>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A50" s="11" t="s">
+      <c r="V50" s="15"/>
+      <c r="W50" s="15"/>
+      <c r="Z50"/>
+      <c r="AA50"/>
+      <c r="AB50"/>
+      <c r="AC50"/>
+      <c r="AD50"/>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A51" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="26" t="s">
+      <c r="B51" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="C50" s="13">
+      <c r="C51" s="13">
         <v>2</v>
       </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13">
+      <c r="D51" s="13"/>
+      <c r="E51" s="13">
         <v>31</v>
       </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13">
+      <c r="F51" s="13"/>
+      <c r="G51" s="13">
         <v>27</v>
       </c>
-      <c r="H50" s="13">
+      <c r="H51" s="13">
         <v>27</v>
       </c>
-      <c r="I50" s="21"/>
-      <c r="J50" s="35">
-        <v>1</v>
-      </c>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12">
-        <v>0</v>
-      </c>
-      <c r="M50" s="12">
-        <v>1</v>
-      </c>
-      <c r="N50" s="35">
+      <c r="I51" s="21"/>
+      <c r="J51" s="35">
+        <v>1</v>
+      </c>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12">
+        <v>0</v>
+      </c>
+      <c r="M51" s="12">
+        <v>1</v>
+      </c>
+      <c r="N51" s="35">
         <v>0.5</v>
       </c>
-      <c r="O50" s="35">
-        <v>1</v>
-      </c>
-      <c r="P50" s="35"/>
-      <c r="Q50" s="35"/>
-      <c r="R50" s="35">
+      <c r="O51" s="35">
+        <v>1</v>
+      </c>
+      <c r="P51" s="35"/>
+      <c r="Q51" s="35"/>
+      <c r="R51" s="35">
         <v>0.5</v>
       </c>
-      <c r="S50" s="35">
-        <v>0</v>
-      </c>
-      <c r="T50" s="35"/>
-      <c r="U50" s="78">
+      <c r="S51" s="35">
+        <v>0</v>
+      </c>
+      <c r="T51" s="35"/>
+      <c r="U51" s="78">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="V50" s="15"/>
-      <c r="AA50" s="33"/>
-      <c r="AB50" s="6"/>
-      <c r="AC50" s="6"/>
-      <c r="AD50" s="6"/>
-    </row>
-    <row r="51" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C51" s="14">
-        <v>7</v>
-      </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14">
-        <v>32</v>
-      </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14">
-        <v>28</v>
-      </c>
-      <c r="H51" s="14">
-        <v>28</v>
-      </c>
-      <c r="I51" s="22"/>
-      <c r="J51" s="36">
-        <v>1</v>
-      </c>
-      <c r="K51" s="2">
-        <v>1</v>
-      </c>
-      <c r="L51" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="M51" s="20">
-        <v>1</v>
-      </c>
-      <c r="N51" s="36">
-        <v>1</v>
-      </c>
-      <c r="O51" s="36">
-        <v>1</v>
-      </c>
-      <c r="P51" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q51" s="36">
-        <v>1</v>
-      </c>
-      <c r="R51" s="36">
-        <v>1</v>
-      </c>
-      <c r="S51" s="36">
-        <v>1</v>
-      </c>
-      <c r="T51" s="34"/>
-      <c r="U51" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
       <c r="V51" s="15"/>
-      <c r="W51" s="3"/>
-      <c r="X51"/>
-      <c r="Y51"/>
-      <c r="Z51"/>
       <c r="AA51" s="33"/>
-      <c r="AB51"/>
-      <c r="AC51"/>
-      <c r="AD51"/>
+      <c r="AB51" s="6"/>
+      <c r="AC51" s="6"/>
+      <c r="AD51" s="6"/>
     </row>
     <row r="52" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="23" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="C52" s="14">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
+      <c r="E52" s="14">
+        <v>32</v>
+      </c>
       <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="J52" s="36"/>
-      <c r="K52" s="34"/>
-      <c r="L52" s="34"/>
-      <c r="M52" s="36"/>
-      <c r="N52" s="36"/>
-      <c r="O52" s="36"/>
-      <c r="P52" s="36"/>
-      <c r="Q52" s="36"/>
-      <c r="R52" s="36"/>
+      <c r="G52" s="14">
+        <v>28</v>
+      </c>
+      <c r="H52" s="14">
+        <v>28</v>
+      </c>
+      <c r="I52" s="22"/>
+      <c r="J52" s="36">
+        <v>1</v>
+      </c>
+      <c r="K52" s="2">
+        <v>1</v>
+      </c>
+      <c r="L52" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="M52" s="20">
+        <v>1</v>
+      </c>
+      <c r="N52" s="36">
+        <v>1</v>
+      </c>
+      <c r="O52" s="36">
+        <v>1</v>
+      </c>
+      <c r="P52" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="36">
+        <v>1</v>
+      </c>
+      <c r="R52" s="36">
+        <v>1</v>
+      </c>
       <c r="S52" s="36">
         <v>1</v>
       </c>
       <c r="T52" s="34"/>
       <c r="U52" s="77">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V52" s="15"/>
       <c r="W52" s="3"/>
-      <c r="X52" s="33"/>
-      <c r="Y52" s="33"/>
-      <c r="Z52" s="33"/>
+      <c r="X52"/>
+      <c r="Y52"/>
+      <c r="Z52"/>
       <c r="AA52" s="33"/>
-      <c r="AB52" s="33"/>
-      <c r="AC52" s="33"/>
-      <c r="AD52" s="33"/>
-    </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AB52"/>
+      <c r="AC52"/>
+      <c r="AD52"/>
+    </row>
+    <row r="53" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="10"/>
       <c r="B53" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="C53" s="14">
+        <v>2</v>
+      </c>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="J53" s="36"/>
+      <c r="K53" s="34"/>
+      <c r="L53" s="34"/>
+      <c r="M53" s="36"/>
+      <c r="N53" s="36"/>
+      <c r="O53" s="36"/>
+      <c r="P53" s="36"/>
+      <c r="Q53" s="36"/>
+      <c r="R53" s="36"/>
+      <c r="S53" s="36">
+        <v>1</v>
+      </c>
+      <c r="T53" s="34">
+        <v>2</v>
+      </c>
+      <c r="U53" s="77">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V53" s="15"/>
+      <c r="W53" s="3"/>
+      <c r="X53" s="33"/>
+      <c r="Y53" s="33"/>
+      <c r="Z53" s="33"/>
+      <c r="AA53" s="33"/>
+      <c r="AB53" s="33"/>
+      <c r="AC53" s="33"/>
+      <c r="AD53" s="33"/>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B54" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C54" s="14">
         <v>4</v>
       </c>
-      <c r="E53" s="14">
+      <c r="E54" s="14">
         <v>33</v>
       </c>
-      <c r="G53" s="14">
+      <c r="G54" s="14">
         <v>29</v>
       </c>
-      <c r="H53" s="14">
+      <c r="H54" s="14">
         <v>29</v>
       </c>
-      <c r="I53" s="22"/>
-      <c r="J53" s="36">
-        <v>1</v>
-      </c>
-      <c r="K53" s="2">
-        <v>1</v>
-      </c>
-      <c r="L53" s="2">
-        <v>1</v>
-      </c>
-      <c r="M53" s="20">
-        <v>1</v>
-      </c>
-      <c r="N53" s="36">
-        <v>1</v>
-      </c>
-      <c r="O53" s="36">
-        <v>1</v>
-      </c>
-      <c r="P53" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q53" s="36">
-        <v>1</v>
-      </c>
-      <c r="R53" s="36">
-        <v>1</v>
-      </c>
-      <c r="S53" s="36">
-        <v>1</v>
-      </c>
-      <c r="T53" s="34"/>
-      <c r="U53" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V53" s="15"/>
-      <c r="AA53" s="33"/>
-    </row>
-    <row r="54" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10"/>
-      <c r="B54" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="C54" s="14">
-        <v>3</v>
-      </c>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
       <c r="I54" s="22"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="2"/>
+      <c r="J54" s="36">
+        <v>1</v>
+      </c>
+      <c r="K54" s="2">
+        <v>1</v>
+      </c>
       <c r="L54" s="2">
-        <v>0</v>
-      </c>
-      <c r="M54" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="M54" s="20">
+        <v>1</v>
+      </c>
       <c r="N54" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="O54" s="36"/>
-      <c r="P54" s="36"/>
-      <c r="Q54" s="36"/>
-      <c r="R54" s="36"/>
+        <v>1</v>
+      </c>
+      <c r="O54" s="36">
+        <v>1</v>
+      </c>
+      <c r="P54" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="36">
+        <v>1</v>
+      </c>
+      <c r="R54" s="36">
+        <v>1</v>
+      </c>
       <c r="S54" s="36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T54" s="34"/>
       <c r="U54" s="77">
         <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V54" s="15"/>
+      <c r="AA54" s="33"/>
+    </row>
+    <row r="55" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="10"/>
+      <c r="B55" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" s="14">
+        <v>3</v>
+      </c>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2">
+        <v>0</v>
+      </c>
+      <c r="M55" s="20"/>
+      <c r="N55" s="36">
         <v>0.5</v>
       </c>
-      <c r="V54" s="15"/>
-      <c r="W54" s="3"/>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B55" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="C55" s="14">
-        <v>1</v>
-      </c>
-      <c r="I55" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="K55" s="34"/>
-      <c r="L55" s="34"/>
-      <c r="M55" s="36"/>
+      <c r="O55" s="36"/>
+      <c r="P55" s="36"/>
+      <c r="Q55" s="36"/>
+      <c r="R55" s="36"/>
       <c r="S55" s="36">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="T55" s="34"/>
       <c r="U55" s="77">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="V55" s="15"/>
-      <c r="AA55" s="33"/>
-    </row>
-    <row r="56" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="10"/>
+      <c r="W55" s="3"/>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B56" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56" s="14">
+        <v>1</v>
+      </c>
+      <c r="I56" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="K56" s="34"/>
+      <c r="L56" s="34"/>
+      <c r="M56" s="36"/>
+      <c r="S56" s="36">
+        <v>1</v>
+      </c>
+      <c r="T56" s="34">
+        <v>2</v>
+      </c>
+      <c r="U56" s="77">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V56" s="15"/>
+      <c r="AA56" s="33"/>
+    </row>
+    <row r="57" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="10"/>
+      <c r="B57" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="C56" s="14">
+      <c r="C57" s="14">
         <v>4</v>
       </c>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="22"/>
-      <c r="J56" s="36"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2">
-        <v>0</v>
-      </c>
-      <c r="M56" s="20"/>
-      <c r="N56" s="36"/>
-      <c r="O56" s="36"/>
-      <c r="P56" s="36"/>
-      <c r="Q56" s="36"/>
-      <c r="R56" s="36"/>
-      <c r="S56" s="36">
-        <v>0</v>
-      </c>
-      <c r="T56" s="34"/>
-      <c r="U56" s="77">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V56" s="15"/>
-      <c r="W56" s="3"/>
-    </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B57" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="C57" s="14">
-        <v>3</v>
-      </c>
-      <c r="D57" s="14">
-        <v>0</v>
-      </c>
-      <c r="I57" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="K57" s="34"/>
-      <c r="L57" s="34"/>
-      <c r="M57" s="36"/>
-      <c r="R57" s="36">
-        <v>0.7</v>
-      </c>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="36"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2">
+        <v>0</v>
+      </c>
+      <c r="M57" s="20"/>
+      <c r="N57" s="36"/>
+      <c r="O57" s="36"/>
+      <c r="P57" s="36"/>
+      <c r="Q57" s="36"/>
+      <c r="R57" s="36"/>
       <c r="S57" s="36">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="T57" s="34"/>
       <c r="U57" s="77">
         <f t="shared" si="0"/>
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="V57" s="15"/>
-      <c r="Y57" s="6"/>
-      <c r="AA57" s="33"/>
+      <c r="W57" s="3"/>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="C58" s="14">
-        <v>6</v>
-      </c>
-      <c r="E58" s="14">
-        <v>34</v>
-      </c>
-      <c r="H58" s="14">
-        <v>30</v>
-      </c>
-      <c r="I58" s="22"/>
-      <c r="L58" s="2">
+        <v>3</v>
+      </c>
+      <c r="D58" s="14">
+        <v>0</v>
+      </c>
+      <c r="I58" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="K58" s="34"/>
+      <c r="L58" s="34"/>
+      <c r="M58" s="36"/>
+      <c r="R58" s="36">
         <v>0.7</v>
-      </c>
-      <c r="P58" s="36">
-        <v>1</v>
-      </c>
-      <c r="R58" s="36">
-        <v>1</v>
       </c>
       <c r="S58" s="36">
         <v>0.7</v>
@@ -4902,194 +4912,171 @@
       <c r="T58" s="34"/>
       <c r="U58" s="77">
         <f t="shared" si="0"/>
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="V58" s="15"/>
+      <c r="Y58" s="6"/>
       <c r="AA58" s="33"/>
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B59" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C59" s="14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E59" s="14">
-        <v>35</v>
-      </c>
-      <c r="G59" s="14">
+        <v>34</v>
+      </c>
+      <c r="H59" s="14">
         <v>30</v>
       </c>
-      <c r="H59" s="14">
-        <v>31</v>
-      </c>
       <c r="I59" s="22"/>
-      <c r="J59" s="36">
-        <v>1</v>
-      </c>
-      <c r="K59" s="2">
-        <v>1</v>
-      </c>
       <c r="L59" s="2">
-        <v>1</v>
-      </c>
-      <c r="M59" s="20">
-        <v>1</v>
-      </c>
-      <c r="N59" s="36">
-        <v>1</v>
-      </c>
-      <c r="O59" s="36">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="P59" s="36">
         <v>1</v>
       </c>
-      <c r="Q59" s="36">
-        <v>1</v>
-      </c>
       <c r="R59" s="36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S59" s="36">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="T59" s="34"/>
       <c r="U59" s="77">
         <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="V59" s="15"/>
+      <c r="AA59" s="33"/>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B60" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C60" s="14">
+        <v>3</v>
+      </c>
+      <c r="E60" s="14">
+        <v>35</v>
+      </c>
+      <c r="G60" s="14">
+        <v>30</v>
+      </c>
+      <c r="H60" s="14">
+        <v>31</v>
+      </c>
+      <c r="I60" s="22"/>
+      <c r="J60" s="36">
+        <v>1</v>
+      </c>
+      <c r="K60" s="2">
+        <v>1</v>
+      </c>
+      <c r="L60" s="2">
+        <v>1</v>
+      </c>
+      <c r="M60" s="20">
+        <v>1</v>
+      </c>
+      <c r="N60" s="36">
+        <v>1</v>
+      </c>
+      <c r="O60" s="36">
+        <v>1</v>
+      </c>
+      <c r="P60" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="36">
+        <v>1</v>
+      </c>
+      <c r="R60" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="S60" s="36">
+        <v>1</v>
+      </c>
+      <c r="T60" s="34"/>
+      <c r="U60" s="77">
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="V59" s="15"/>
-      <c r="Z59" s="6"/>
-      <c r="AA59" s="33"/>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A60" s="11" t="s">
+      <c r="V60" s="15"/>
+      <c r="Z60" s="6"/>
+      <c r="AA60" s="33"/>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A61" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B60" s="26" t="s">
+      <c r="B61" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="C60" s="13">
+      <c r="C61" s="13">
         <v>2</v>
       </c>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13">
+      <c r="D61" s="13"/>
+      <c r="E61" s="13">
         <v>36</v>
       </c>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13">
+      <c r="F61" s="13"/>
+      <c r="G61" s="13">
         <v>31</v>
       </c>
-      <c r="H60" s="13">
+      <c r="H61" s="13">
         <v>32</v>
       </c>
-      <c r="I60" s="21"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="12"/>
-      <c r="L60" s="12">
-        <v>1</v>
-      </c>
-      <c r="M60" s="12">
-        <v>1</v>
-      </c>
-      <c r="N60" s="35">
-        <v>1</v>
-      </c>
-      <c r="O60" s="35">
-        <v>1</v>
-      </c>
-      <c r="P60" s="35"/>
-      <c r="Q60" s="35">
-        <v>1</v>
-      </c>
-      <c r="R60" s="35">
-        <v>1</v>
-      </c>
-      <c r="S60" s="35">
+      <c r="I61" s="21"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12">
+        <v>1</v>
+      </c>
+      <c r="M61" s="12">
+        <v>1</v>
+      </c>
+      <c r="N61" s="35">
+        <v>1</v>
+      </c>
+      <c r="O61" s="35">
+        <v>1</v>
+      </c>
+      <c r="P61" s="35"/>
+      <c r="Q61" s="35">
+        <v>1</v>
+      </c>
+      <c r="R61" s="35">
+        <v>1</v>
+      </c>
+      <c r="S61" s="35">
         <v>0.5</v>
       </c>
-      <c r="T60" s="35"/>
-      <c r="U60" s="78">
+      <c r="T61" s="35"/>
+      <c r="U61" s="78">
         <f t="shared" si="0"/>
         <v>2.5</v>
-      </c>
-      <c r="V60" s="15"/>
-      <c r="AA60" s="33"/>
-    </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B61" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="C61" s="14">
-        <v>7</v>
-      </c>
-      <c r="E61" s="14">
-        <v>37</v>
-      </c>
-      <c r="G61" s="14">
-        <v>32</v>
-      </c>
-      <c r="H61" s="14">
-        <v>33</v>
-      </c>
-      <c r="I61" s="22"/>
-      <c r="J61" s="36">
-        <v>1</v>
-      </c>
-      <c r="K61" s="2">
-        <v>1</v>
-      </c>
-      <c r="L61" s="2">
-        <v>1</v>
-      </c>
-      <c r="M61" s="20">
-        <v>1</v>
-      </c>
-      <c r="N61" s="36">
-        <v>1</v>
-      </c>
-      <c r="O61" s="36">
-        <v>1</v>
-      </c>
-      <c r="P61" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q61" s="36">
-        <v>1</v>
-      </c>
-      <c r="R61" s="36">
-        <v>1</v>
-      </c>
-      <c r="S61" s="36">
-        <v>1</v>
-      </c>
-      <c r="T61" s="34"/>
-      <c r="U61" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
       </c>
       <c r="V61" s="15"/>
       <c r="AA61" s="33"/>
-      <c r="AB61" s="6"/>
-      <c r="AC61" s="6"/>
-      <c r="AD61" s="6"/>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C62" s="14">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E62" s="14">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G62" s="14">
+        <v>32</v>
+      </c>
+      <c r="H62" s="14">
         <v>33</v>
-      </c>
-      <c r="H62" s="14">
-        <v>34</v>
       </c>
       <c r="I62" s="22"/>
       <c r="J62" s="36">
@@ -5113,231 +5100,235 @@
       <c r="P62" s="36">
         <v>1</v>
       </c>
+      <c r="Q62" s="36">
+        <v>1</v>
+      </c>
       <c r="R62" s="36">
         <v>1</v>
       </c>
       <c r="S62" s="36">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="T62" s="34"/>
       <c r="U62" s="77">
         <f t="shared" si="0"/>
-        <v>1.9</v>
+        <v>3</v>
       </c>
       <c r="V62" s="15"/>
       <c r="AA62" s="33"/>
+      <c r="AB62" s="6"/>
+      <c r="AC62" s="6"/>
+      <c r="AD62" s="6"/>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B63" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C63" s="14">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E63" s="14">
+        <v>38</v>
+      </c>
+      <c r="G63" s="14">
+        <v>33</v>
+      </c>
+      <c r="H63" s="14">
+        <v>34</v>
       </c>
       <c r="I63" s="22"/>
+      <c r="J63" s="36">
+        <v>1</v>
+      </c>
+      <c r="K63" s="2">
+        <v>1</v>
+      </c>
       <c r="L63" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="M63" s="20">
+        <v>1</v>
+      </c>
+      <c r="N63" s="36">
+        <v>1</v>
+      </c>
+      <c r="O63" s="36">
+        <v>1</v>
+      </c>
+      <c r="P63" s="36">
+        <v>1</v>
+      </c>
+      <c r="R63" s="36">
+        <v>1</v>
       </c>
       <c r="S63" s="36">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="T63" s="34"/>
       <c r="U63" s="77">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="V63" s="15"/>
-      <c r="Z63" s="6"/>
       <c r="AA63" s="33"/>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A64" s="11" t="s">
+      <c r="B64" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="C64" s="14">
+        <v>3</v>
+      </c>
+      <c r="I64" s="22"/>
+      <c r="L64" s="2">
+        <v>0</v>
+      </c>
+      <c r="S64" s="36">
+        <v>0</v>
+      </c>
+      <c r="T64" s="34"/>
+      <c r="U64" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V64" s="15"/>
+      <c r="Z64" s="6"/>
+      <c r="AA64" s="33"/>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A65" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B64" s="26" t="s">
+      <c r="B65" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="C64" s="13">
+      <c r="C65" s="13">
         <v>4</v>
       </c>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13">
+      <c r="D65" s="13"/>
+      <c r="E65" s="13">
         <v>39</v>
       </c>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="21"/>
-      <c r="J64" s="35">
-        <v>1</v>
-      </c>
-      <c r="K64" s="12"/>
-      <c r="L64" s="12">
-        <v>0</v>
-      </c>
-      <c r="M64" s="12"/>
-      <c r="N64" s="35">
-        <v>1</v>
-      </c>
-      <c r="O64" s="35"/>
-      <c r="P64" s="35"/>
-      <c r="Q64" s="35">
-        <v>1</v>
-      </c>
-      <c r="R64" s="35"/>
-      <c r="S64" s="35">
-        <v>0</v>
-      </c>
-      <c r="T64" s="35"/>
-      <c r="U64" s="78">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V64" s="15"/>
-      <c r="AA64" s="33"/>
-    </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B65" s="23" t="s">
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="35">
+        <v>1</v>
+      </c>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12">
+        <v>0</v>
+      </c>
+      <c r="M65" s="12"/>
+      <c r="N65" s="35">
+        <v>1</v>
+      </c>
+      <c r="O65" s="35"/>
+      <c r="P65" s="35"/>
+      <c r="Q65" s="35">
+        <v>1</v>
+      </c>
+      <c r="R65" s="35"/>
+      <c r="S65" s="35">
+        <v>0</v>
+      </c>
+      <c r="T65" s="35"/>
+      <c r="U65" s="78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V65" s="15"/>
+      <c r="AA65" s="33"/>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B66" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="C65" s="14">
+      <c r="C66" s="14">
         <v>3</v>
       </c>
-      <c r="E65" s="14">
+      <c r="E66" s="14">
         <v>40</v>
       </c>
-      <c r="I65" s="22"/>
-      <c r="J65" s="36">
-        <v>1</v>
-      </c>
-      <c r="L65" s="2">
-        <v>0</v>
-      </c>
-      <c r="N65" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q65" s="36">
-        <v>1</v>
-      </c>
-      <c r="S65" s="36">
-        <v>0</v>
-      </c>
-      <c r="T65" s="34"/>
-      <c r="U65" s="77">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V65" s="15"/>
-    </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A66" s="11" t="s">
+      <c r="I66" s="22"/>
+      <c r="J66" s="36">
+        <v>1</v>
+      </c>
+      <c r="L66" s="2">
+        <v>0</v>
+      </c>
+      <c r="N66" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="36">
+        <v>1</v>
+      </c>
+      <c r="S66" s="36">
+        <v>0</v>
+      </c>
+      <c r="T66" s="34"/>
+      <c r="U66" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V66" s="15"/>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A67" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B66" s="26" t="s">
+      <c r="B67" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C66" s="13">
+      <c r="C67" s="13">
         <v>2</v>
       </c>
-      <c r="D66" s="13">
-        <v>0</v>
-      </c>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="21"/>
-      <c r="J66" s="35"/>
-      <c r="K66" s="12">
-        <v>1</v>
-      </c>
-      <c r="L66" s="12">
-        <v>1</v>
-      </c>
-      <c r="M66" s="12"/>
-      <c r="N66" s="35">
-        <v>1</v>
-      </c>
-      <c r="O66" s="35">
-        <v>1</v>
-      </c>
-      <c r="P66" s="35">
-        <v>1</v>
-      </c>
-      <c r="Q66" s="35">
-        <v>1</v>
-      </c>
-      <c r="R66" s="35">
-        <v>1</v>
-      </c>
-      <c r="S66" s="35">
+      <c r="D67" s="13">
+        <v>0</v>
+      </c>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="35"/>
+      <c r="K67" s="12">
+        <v>1</v>
+      </c>
+      <c r="L67" s="12">
+        <v>1</v>
+      </c>
+      <c r="M67" s="12"/>
+      <c r="N67" s="35">
+        <v>1</v>
+      </c>
+      <c r="O67" s="35">
+        <v>1</v>
+      </c>
+      <c r="P67" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="35">
+        <v>1</v>
+      </c>
+      <c r="R67" s="35">
+        <v>1</v>
+      </c>
+      <c r="S67" s="35">
         <v>0.9</v>
       </c>
-      <c r="T66" s="35"/>
-      <c r="U66" s="78">
+      <c r="T67" s="35"/>
+      <c r="U67" s="78">
         <f t="shared" si="0"/>
         <v>2.9</v>
       </c>
-      <c r="V66" s="15"/>
-    </row>
-    <row r="67" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="30"/>
-      <c r="B67" s="31" t="s">
+      <c r="V67" s="15"/>
+    </row>
+    <row r="68" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="30"/>
+      <c r="B68" s="31" t="s">
         <v>82</v>
-      </c>
-      <c r="C67" s="14">
-        <v>2</v>
-      </c>
-      <c r="D67" s="14">
-        <v>1</v>
-      </c>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="36"/>
-      <c r="K67" s="20"/>
-      <c r="L67" s="20">
-        <v>1</v>
-      </c>
-      <c r="M67" s="20"/>
-      <c r="N67" s="36">
-        <v>1</v>
-      </c>
-      <c r="O67" s="36">
-        <v>1</v>
-      </c>
-      <c r="P67" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q67" s="36">
-        <v>1</v>
-      </c>
-      <c r="R67" s="36">
-        <v>1</v>
-      </c>
-      <c r="S67" s="36">
-        <v>1</v>
-      </c>
-      <c r="T67" s="36"/>
-      <c r="U67" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V67" s="15"/>
-      <c r="W67" s="3"/>
-      <c r="X67"/>
-      <c r="Y67"/>
-      <c r="Z67"/>
-      <c r="AA67"/>
-      <c r="AB67"/>
-      <c r="AC67"/>
-      <c r="AD67"/>
-    </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B68" s="23" t="s">
-        <v>93</v>
       </c>
       <c r="C68" s="14">
         <v>2</v>
@@ -5345,87 +5336,115 @@
       <c r="D68" s="14">
         <v>1</v>
       </c>
-      <c r="I68" s="22" t="s">
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="22"/>
+      <c r="J68" s="36"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="20">
+        <v>1</v>
+      </c>
+      <c r="M68" s="20"/>
+      <c r="N68" s="36">
+        <v>1</v>
+      </c>
+      <c r="O68" s="36">
+        <v>1</v>
+      </c>
+      <c r="P68" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="36">
+        <v>1</v>
+      </c>
+      <c r="R68" s="36">
+        <v>1</v>
+      </c>
+      <c r="S68" s="36">
+        <v>1</v>
+      </c>
+      <c r="T68" s="36"/>
+      <c r="U68" s="77">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V68" s="15"/>
+      <c r="W68" s="3"/>
+      <c r="X68"/>
+      <c r="Y68"/>
+      <c r="Z68"/>
+      <c r="AA68"/>
+      <c r="AB68"/>
+      <c r="AC68"/>
+      <c r="AD68"/>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B69" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" s="14">
+        <v>2</v>
+      </c>
+      <c r="D69" s="14">
+        <v>1</v>
+      </c>
+      <c r="I69" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="K68" s="2">
-        <v>1</v>
-      </c>
-      <c r="L68" s="2">
-        <v>1</v>
-      </c>
-      <c r="T68" s="34"/>
-      <c r="U68" s="77">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V68" s="15"/>
-      <c r="X68" s="33"/>
-      <c r="Z68" s="6"/>
-    </row>
-    <row r="69" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="10"/>
-      <c r="B69" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69" s="14">
-        <v>4</v>
-      </c>
-      <c r="D69" s="14">
-        <v>3</v>
-      </c>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="22"/>
-      <c r="J69" s="36"/>
       <c r="K69" s="2">
         <v>1</v>
       </c>
       <c r="L69" s="2">
-        <v>1</v>
-      </c>
-      <c r="M69" s="20"/>
-      <c r="N69" s="36">
-        <v>1</v>
-      </c>
-      <c r="O69" s="36">
-        <v>1</v>
-      </c>
-      <c r="P69" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q69" s="36">
-        <v>1</v>
-      </c>
-      <c r="R69" s="36">
-        <v>1</v>
-      </c>
-      <c r="S69" s="36">
         <v>1</v>
       </c>
       <c r="T69" s="34"/>
       <c r="U69" s="77">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V69" s="15"/>
+      <c r="X69" s="33"/>
+      <c r="Z69" s="6"/>
+    </row>
+    <row r="70" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="10"/>
+      <c r="B70" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="14">
+        <v>4</v>
+      </c>
+      <c r="D70" s="14">
         <v>3</v>
       </c>
-      <c r="V69" s="15"/>
-      <c r="W69" s="3"/>
-      <c r="Z69" s="6"/>
-    </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B70" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="C70" s="14">
-        <v>1</v>
-      </c>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
       <c r="I70" s="22"/>
-      <c r="K70" s="34"/>
-      <c r="L70" s="34"/>
-      <c r="M70" s="36"/>
+      <c r="J70" s="36"/>
+      <c r="K70" s="2">
+        <v>1</v>
+      </c>
+      <c r="L70" s="2">
+        <v>1</v>
+      </c>
+      <c r="M70" s="20"/>
+      <c r="N70" s="36">
+        <v>1</v>
+      </c>
       <c r="O70" s="36">
+        <v>1</v>
+      </c>
+      <c r="P70" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q70" s="36">
+        <v>1</v>
+      </c>
+      <c r="R70" s="36">
         <v>1</v>
       </c>
       <c r="S70" s="36">
@@ -5433,47 +5452,25 @@
       </c>
       <c r="T70" s="34"/>
       <c r="U70" s="77">
-        <f t="shared" ref="U70:U73" si="2">SUM(Q70:T70)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="V70" s="15"/>
-      <c r="AA70" s="6"/>
-      <c r="AB70" s="6"/>
-      <c r="AC70" s="6"/>
-      <c r="AD70" s="6"/>
+      <c r="W70" s="3"/>
+      <c r="Z70" s="6"/>
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B71" s="23" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="C71" s="14">
         <v>1</v>
       </c>
-      <c r="D71" s="14">
-        <v>0</v>
-      </c>
-      <c r="I71" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="L71" s="2">
-        <v>0</v>
-      </c>
-      <c r="M71" s="20">
-        <v>1</v>
-      </c>
-      <c r="N71" s="36">
-        <v>1</v>
-      </c>
+      <c r="I71" s="22"/>
+      <c r="K71" s="34"/>
+      <c r="L71" s="34"/>
+      <c r="M71" s="36"/>
       <c r="O71" s="36">
-        <v>1</v>
-      </c>
-      <c r="P71" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q71" s="36">
-        <v>1</v>
-      </c>
-      <c r="R71" s="36">
         <v>1</v>
       </c>
       <c r="S71" s="36">
@@ -5481,35 +5478,34 @@
       </c>
       <c r="T71" s="34"/>
       <c r="U71" s="77">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" ref="U71:U74" si="4">SUM(Q71:T71)</f>
+        <v>1</v>
       </c>
       <c r="V71" s="15"/>
-    </row>
-    <row r="72" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="10"/>
+      <c r="AA71" s="6"/>
+      <c r="AB71" s="6"/>
+      <c r="AC71" s="6"/>
+      <c r="AD71" s="6"/>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B72" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C72" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D72" s="14">
-        <v>1</v>
-      </c>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="22"/>
-      <c r="J72" s="36"/>
-      <c r="K72" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I72" s="22" t="s">
+        <v>91</v>
       </c>
       <c r="L72" s="2">
-        <v>1</v>
-      </c>
-      <c r="M72" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="M72" s="20">
+        <v>1</v>
+      </c>
       <c r="N72" s="36">
         <v>1</v>
       </c>
@@ -5530,135 +5526,150 @@
       </c>
       <c r="T72" s="34"/>
       <c r="U72" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="V72" s="15"/>
-      <c r="W72" s="3"/>
-      <c r="X72"/>
-      <c r="Y72"/>
-      <c r="Z72"/>
-      <c r="AA72"/>
-      <c r="AB72"/>
-      <c r="AC72"/>
-      <c r="AD72"/>
-    </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B73" s="24" t="s">
+    </row>
+    <row r="73" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="10"/>
+      <c r="B73" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" s="14">
+        <v>3</v>
+      </c>
+      <c r="D73" s="14">
+        <v>1</v>
+      </c>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="36"/>
+      <c r="K73" s="2">
+        <v>1</v>
+      </c>
+      <c r="L73" s="2">
+        <v>1</v>
+      </c>
+      <c r="M73" s="20"/>
+      <c r="N73" s="36">
+        <v>1</v>
+      </c>
+      <c r="O73" s="36">
+        <v>1</v>
+      </c>
+      <c r="P73" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="36">
+        <v>1</v>
+      </c>
+      <c r="R73" s="36">
+        <v>1</v>
+      </c>
+      <c r="S73" s="36">
+        <v>1</v>
+      </c>
+      <c r="T73" s="34"/>
+      <c r="U73" s="77">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="V73" s="15"/>
+      <c r="W73" s="3"/>
+      <c r="X73"/>
+      <c r="Y73"/>
+      <c r="Z73"/>
+      <c r="AA73"/>
+      <c r="AB73"/>
+      <c r="AC73"/>
+      <c r="AD73"/>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B74" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C73" s="27">
+      <c r="C74" s="27">
         <v>4</v>
       </c>
-      <c r="D73" s="27">
-        <v>0</v>
-      </c>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="27"/>
-      <c r="H73" s="27"/>
-      <c r="I73" s="29"/>
-      <c r="J73" s="37"/>
-      <c r="K73" s="28">
-        <v>1</v>
-      </c>
-      <c r="L73" s="28">
-        <v>0</v>
-      </c>
-      <c r="M73" s="28"/>
-      <c r="N73" s="37"/>
-      <c r="O73" s="37"/>
-      <c r="P73" s="37">
-        <v>1</v>
-      </c>
-      <c r="Q73" s="37">
-        <v>1</v>
-      </c>
-      <c r="R73" s="37">
-        <v>1</v>
-      </c>
-      <c r="S73" s="37">
-        <v>0</v>
-      </c>
-      <c r="T73" s="37"/>
-      <c r="U73" s="79">
-        <f t="shared" si="2"/>
+      <c r="D74" s="27">
+        <v>0</v>
+      </c>
+      <c r="E74" s="27"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="27"/>
+      <c r="H74" s="27"/>
+      <c r="I74" s="29"/>
+      <c r="J74" s="37"/>
+      <c r="K74" s="28">
+        <v>1</v>
+      </c>
+      <c r="L74" s="28">
+        <v>0</v>
+      </c>
+      <c r="M74" s="28"/>
+      <c r="N74" s="37"/>
+      <c r="O74" s="37"/>
+      <c r="P74" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="37">
+        <v>1</v>
+      </c>
+      <c r="R74" s="37">
+        <v>1</v>
+      </c>
+      <c r="S74" s="37">
+        <v>0</v>
+      </c>
+      <c r="T74" s="37"/>
+      <c r="U74" s="79">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="V73" s="15"/>
-    </row>
-    <row r="74" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="11"/>
       <c r="V74" s="15"/>
-      <c r="Y74" s="33"/>
-    </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I75" s="64" t="s">
+    </row>
+    <row r="75" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="11"/>
+      <c r="V75" s="15"/>
+      <c r="Y75" s="33"/>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I76" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="J75" s="85"/>
-      <c r="K75" s="65"/>
-      <c r="L75" s="65"/>
-      <c r="M75" s="65"/>
-      <c r="N75" s="65"/>
-      <c r="O75" s="65"/>
-      <c r="P75" s="65"/>
-      <c r="Q75" s="65">
-        <f t="array" ref="Q75">SUM($C2:$C73*(Q2:Q73&gt;=0.9)*($U2:$U73&gt;=$W$12))</f>
+      <c r="J76" s="85"/>
+      <c r="K76" s="65"/>
+      <c r="L76" s="65"/>
+      <c r="M76" s="65"/>
+      <c r="N76" s="65"/>
+      <c r="O76" s="65"/>
+      <c r="P76" s="65"/>
+      <c r="Q76" s="65">
+        <f t="array" ref="Q76">SUM($C2:$C74*(Q2:Q74&gt;=0.9)*($U2:$U74&gt;=$W$12))</f>
         <v>185</v>
       </c>
-      <c r="R75" s="65">
-        <f t="array" ref="R75">SUM($C2:$C73*(R2:R73&gt;=0.9)*($U2:$U73&gt;=$W$12))</f>
+      <c r="R76" s="65">
+        <f t="array" ref="R76">SUM($C2:$C74*(R2:R74&gt;=0.9)*($U2:$U74&gt;=$W$12))</f>
         <v>193</v>
       </c>
-      <c r="S75" s="65">
-        <f t="array" ref="S75">SUM($C2:$C73*(S2:S73&gt;=0.9)*($U2:$U73&gt;=$W$12))</f>
-        <v>195</v>
-      </c>
-      <c r="T75" s="66"/>
-      <c r="V75" s="15"/>
-      <c r="AA75" s="6"/>
-      <c r="AB75" s="6"/>
-      <c r="AC75" s="6"/>
-      <c r="AD75" s="6"/>
-    </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I76" s="67" t="s">
+      <c r="S76" s="65">
+        <f t="array" ref="S76">SUM($C2:$C74*(S2:S74&gt;=0.9)*($U2:$U74&gt;=$W$12))</f>
+        <v>198</v>
+      </c>
+      <c r="T76" s="66"/>
+      <c r="V76" s="15"/>
+      <c r="AA76" s="6"/>
+      <c r="AB76" s="6"/>
+      <c r="AC76" s="6"/>
+      <c r="AD76" s="6"/>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I77" s="67" t="s">
         <v>100</v>
-      </c>
-      <c r="J76" s="86"/>
-      <c r="K76" s="68"/>
-      <c r="L76" s="68"/>
-      <c r="M76" s="68"/>
-      <c r="N76" s="68"/>
-      <c r="O76" s="68"/>
-      <c r="P76" s="68"/>
-      <c r="Q76" s="68">
-        <f t="array" ref="Q76">SUM($C2:$C73*Q2:Q73*($U2:$U73&gt;=$W$12))</f>
-        <v>192</v>
-      </c>
-      <c r="R76" s="68">
-        <f t="array" ref="R76">SUM($C2:$C73*R2:R73*($U2:$U73&gt;=$W$12))</f>
-        <v>212.6</v>
-      </c>
-      <c r="S76" s="68">
-        <f t="array" ref="S76">SUM($C2:$C73*S2:S73*($U2:$U73&gt;=$W$12))</f>
-        <v>208.23</v>
-      </c>
-      <c r="T76" s="69"/>
-      <c r="V76" s="15"/>
-    </row>
-    <row r="77" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="10"/>
-      <c r="B77" s="23"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="67" t="s">
-        <v>99</v>
       </c>
       <c r="J77" s="86"/>
       <c r="K77" s="68"/>
@@ -5668,32 +5679,31 @@
       <c r="O77" s="68"/>
       <c r="P77" s="68"/>
       <c r="Q77" s="68">
-        <f t="array" ref="Q77">SUM($C$2:$C$73*(Q$2:Q$73&gt;=0.1)*($U$2:$U$73&gt;=$W$12))</f>
-        <v>199</v>
+        <f t="array" ref="Q77">SUM($C2:$C74*Q2:Q74*($U2:$U74&gt;=$W$12))</f>
+        <v>192</v>
       </c>
       <c r="R77" s="68">
-        <f t="array" ref="R77">SUM($C$2:$C$73*(R$2:R$73&gt;=0.1)*($U$2:$U$73&gt;=$W$12))</f>
-        <v>222</v>
+        <f t="array" ref="R77">SUM($C2:$C74*R2:R74*($U2:$U74&gt;=$W$12))</f>
+        <v>212.6</v>
       </c>
       <c r="S77" s="68">
-        <f t="array" ref="S77">SUM($C$2:$C$73*(S$2:S$73&gt;=0.1)*($U$2:$U$73&gt;=$W$12))</f>
-        <v>218</v>
+        <f t="array" ref="S77">SUM($C2:$C74*S2:S74*($U2:$U74&gt;=$W$12))</f>
+        <v>211.23</v>
       </c>
       <c r="T77" s="69"/>
-      <c r="U77" s="3"/>
       <c r="V77" s="15"/>
-      <c r="W77" s="3"/>
-      <c r="X77"/>
-      <c r="Y77"/>
-      <c r="Z77"/>
-      <c r="AA77"/>
-      <c r="AB77"/>
-      <c r="AC77"/>
-      <c r="AD77"/>
-    </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="10"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
       <c r="I78" s="67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J78" s="86"/>
       <c r="K78" s="68"/>
@@ -5703,92 +5713,118 @@
       <c r="O78" s="68"/>
       <c r="P78" s="68"/>
       <c r="Q78" s="68">
-        <f t="shared" ref="Q78:S78" si="3">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>237</v>
+        <f t="array" ref="Q78">SUM($C$2:$C$74*(Q$2:Q$74&gt;=0.1)*($U$2:$U$74&gt;=$W$12))</f>
+        <v>199</v>
       </c>
       <c r="R78" s="68">
-        <f t="shared" si="3"/>
-        <v>237</v>
+        <f t="array" ref="R78">SUM($C$2:$C$74*(R$2:R$74&gt;=0.1)*($U$2:$U$74&gt;=$W$12))</f>
+        <v>222</v>
       </c>
       <c r="S78" s="68">
-        <f t="shared" si="3"/>
-        <v>237</v>
+        <f t="array" ref="S78">SUM($C$2:$C$74*(S$2:S$74&gt;=0.1)*($U$2:$U$74&gt;=$W$12))</f>
+        <v>221</v>
       </c>
       <c r="T78" s="69"/>
+      <c r="U78" s="3"/>
       <c r="V78" s="15"/>
-      <c r="AA78" s="6"/>
-      <c r="AB78" s="6"/>
-      <c r="AC78" s="6"/>
-      <c r="AD78" s="6"/>
+      <c r="W78" s="3"/>
+      <c r="X78"/>
+      <c r="Y78"/>
+      <c r="Z78"/>
+      <c r="AA78"/>
+      <c r="AB78"/>
+      <c r="AC78"/>
+      <c r="AD78"/>
     </row>
     <row r="79" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I79" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="J79" s="86"/>
+      <c r="K79" s="68"/>
+      <c r="L79" s="68"/>
+      <c r="M79" s="68"/>
+      <c r="N79" s="68"/>
+      <c r="O79" s="68"/>
+      <c r="P79" s="68"/>
+      <c r="Q79" s="68">
+        <f t="shared" ref="Q79:S79" si="5">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>240</v>
+      </c>
+      <c r="R79" s="68">
+        <f t="shared" si="5"/>
+        <v>240</v>
+      </c>
+      <c r="S79" s="68">
+        <f t="shared" si="5"/>
+        <v>240</v>
+      </c>
+      <c r="T79" s="69"/>
+      <c r="V79" s="15"/>
+      <c r="AA79" s="6"/>
+      <c r="AB79" s="6"/>
+      <c r="AC79" s="6"/>
+      <c r="AD79" s="6"/>
+    </row>
+    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I80" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="J79" s="86"/>
-      <c r="K79" s="70"/>
-      <c r="L79" s="70"/>
-      <c r="M79" s="70"/>
-      <c r="N79" s="70"/>
-      <c r="O79" s="70"/>
-      <c r="P79" s="70"/>
-      <c r="Q79" s="70">
-        <f t="shared" ref="Q79:S79" si="4">Q76/Q78</f>
-        <v>0.810126582278481</v>
-      </c>
-      <c r="R79" s="70">
-        <f t="shared" si="4"/>
-        <v>0.89704641350210967</v>
-      </c>
-      <c r="S79" s="70">
-        <f t="shared" si="4"/>
-        <v>0.87860759493670881</v>
-      </c>
-      <c r="T79" s="71"/>
-      <c r="V79" s="15"/>
-    </row>
-    <row r="80" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C80" s="33"/>
-      <c r="I80" s="72" t="s">
+      <c r="J80" s="86"/>
+      <c r="K80" s="70"/>
+      <c r="L80" s="70"/>
+      <c r="M80" s="70"/>
+      <c r="N80" s="70"/>
+      <c r="O80" s="70"/>
+      <c r="P80" s="70"/>
+      <c r="Q80" s="70">
+        <f t="shared" ref="Q80:S80" si="6">Q77/Q79</f>
+        <v>0.8</v>
+      </c>
+      <c r="R80" s="70">
+        <f t="shared" si="6"/>
+        <v>0.88583333333333336</v>
+      </c>
+      <c r="S80" s="70">
+        <f t="shared" si="6"/>
+        <v>0.88012499999999994</v>
+      </c>
+      <c r="T80" s="71"/>
+      <c r="V80" s="15"/>
+    </row>
+    <row r="81" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C81" s="33"/>
+      <c r="I81" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="J80" s="87"/>
-      <c r="K80" s="73"/>
-      <c r="L80" s="73"/>
-      <c r="M80" s="73"/>
-      <c r="N80" s="73"/>
-      <c r="O80" s="73"/>
-      <c r="P80" s="73"/>
-      <c r="Q80" s="73">
-        <f t="shared" ref="Q80:S80" si="5">Q78-Q76</f>
-        <v>45</v>
-      </c>
-      <c r="R80" s="73">
-        <f t="shared" si="5"/>
-        <v>24.400000000000006</v>
-      </c>
-      <c r="S80" s="73">
-        <f t="shared" si="5"/>
+      <c r="J81" s="87"/>
+      <c r="K81" s="73"/>
+      <c r="L81" s="73"/>
+      <c r="M81" s="73"/>
+      <c r="N81" s="73"/>
+      <c r="O81" s="73"/>
+      <c r="P81" s="73"/>
+      <c r="Q81" s="73">
+        <f t="shared" ref="Q81:S81" si="7">Q79-Q77</f>
+        <v>48</v>
+      </c>
+      <c r="R81" s="73">
+        <f t="shared" si="7"/>
+        <v>27.400000000000006</v>
+      </c>
+      <c r="S81" s="73">
+        <f t="shared" si="7"/>
         <v>28.77000000000001</v>
       </c>
-      <c r="T80" s="74"/>
-      <c r="V80" s="15"/>
-      <c r="AA80" s="6"/>
-      <c r="AB80" s="6"/>
-      <c r="AC80" s="6"/>
-      <c r="AD80" s="6"/>
-    </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="C81" s="33"/>
+      <c r="T81" s="74"/>
       <c r="V81" s="15"/>
+      <c r="AA81" s="6"/>
+      <c r="AB81" s="6"/>
+      <c r="AC81" s="6"/>
+      <c r="AD81" s="6"/>
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C82" s="33"/>
-      <c r="I82" s="14"/>
-      <c r="J82" s="14"/>
-      <c r="K82" s="14"/>
-      <c r="L82" s="14"/>
-      <c r="N82" s="14"/>
       <c r="V82" s="15"/>
     </row>
     <row r="83" spans="1:30" x14ac:dyDescent="0.3">
@@ -5801,6 +5837,7 @@
       <c r="V83" s="15"/>
     </row>
     <row r="84" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C84" s="33"/>
       <c r="I84" s="14"/>
       <c r="J84" s="14"/>
       <c r="K84" s="14"/>
@@ -5815,7 +5852,6 @@
       <c r="L85" s="14"/>
       <c r="N85" s="14"/>
       <c r="V85" s="15"/>
-      <c r="Z85" s="33"/>
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I86" s="14"/>
@@ -5824,6 +5860,7 @@
       <c r="L86" s="14"/>
       <c r="N86" s="14"/>
       <c r="V86" s="15"/>
+      <c r="Z86" s="33"/>
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I87" s="14"/>
@@ -5831,6 +5868,7 @@
       <c r="K87" s="14"/>
       <c r="L87" s="14"/>
       <c r="N87" s="14"/>
+      <c r="V87" s="15"/>
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I88" s="14"/>
@@ -5846,64 +5884,71 @@
       <c r="L89" s="14"/>
       <c r="N89" s="14"/>
     </row>
-    <row r="90" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="10"/>
-      <c r="B90" s="23"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="20"/>
-      <c r="J90" s="36"/>
-      <c r="K90" s="2"/>
-      <c r="L90" s="2"/>
-      <c r="M90" s="20"/>
-      <c r="N90" s="36"/>
-      <c r="O90" s="36"/>
-      <c r="P90" s="36"/>
-      <c r="Q90" s="36"/>
-      <c r="R90" s="36"/>
-      <c r="S90" s="36"/>
-      <c r="T90" s="2"/>
-      <c r="U90" s="3"/>
-      <c r="V90" s="3"/>
-      <c r="W90" s="3"/>
-      <c r="X90"/>
-      <c r="Y90"/>
-      <c r="Z90"/>
-      <c r="AA90"/>
-      <c r="AB90"/>
-      <c r="AC90"/>
-      <c r="AD90"/>
-    </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA93" s="6"/>
-      <c r="AB93" s="6"/>
-      <c r="AC93" s="6"/>
-      <c r="AD93" s="6"/>
-    </row>
-    <row r="97" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA97" s="6"/>
-      <c r="AB97" s="6"/>
-      <c r="AC97" s="6"/>
-      <c r="AD97" s="6"/>
-    </row>
-    <row r="102" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA102" s="6"/>
-      <c r="AB102" s="6"/>
-      <c r="AC102" s="6"/>
-      <c r="AD102" s="6"/>
-    </row>
-    <row r="115" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA115" s="33"/>
-      <c r="AB115" s="33"/>
-      <c r="AC115" s="33"/>
-      <c r="AD115" s="33"/>
+    <row r="90" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
+      <c r="N90" s="14"/>
+    </row>
+    <row r="91" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="10"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="20"/>
+      <c r="J91" s="36"/>
+      <c r="K91" s="2"/>
+      <c r="L91" s="2"/>
+      <c r="M91" s="20"/>
+      <c r="N91" s="36"/>
+      <c r="O91" s="36"/>
+      <c r="P91" s="36"/>
+      <c r="Q91" s="36"/>
+      <c r="R91" s="36"/>
+      <c r="S91" s="36"/>
+      <c r="T91" s="2"/>
+      <c r="U91" s="3"/>
+      <c r="V91" s="3"/>
+      <c r="W91" s="3"/>
+      <c r="X91"/>
+      <c r="Y91"/>
+      <c r="Z91"/>
+      <c r="AA91"/>
+      <c r="AB91"/>
+      <c r="AC91"/>
+      <c r="AD91"/>
+    </row>
+    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA94" s="6"/>
+      <c r="AB94" s="6"/>
+      <c r="AC94" s="6"/>
+      <c r="AD94" s="6"/>
+    </row>
+    <row r="98" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA98" s="6"/>
+      <c r="AB98" s="6"/>
+      <c r="AC98" s="6"/>
+      <c r="AD98" s="6"/>
+    </row>
+    <row r="103" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA103" s="6"/>
+      <c r="AB103" s="6"/>
+      <c r="AC103" s="6"/>
+      <c r="AD103" s="6"/>
+    </row>
+    <row r="116" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA116" s="33"/>
+      <c r="AB116" s="33"/>
+      <c r="AC116" s="33"/>
+      <c r="AD116" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U73">
+  <conditionalFormatting sqref="B2:U74">
     <cfRule type="expression" dxfId="2" priority="37" stopIfTrue="1">
       <formula>$U2&gt;=(0.5+$W$12)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Switched order of two labs
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
@@ -2000,8 +2000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3106,15 +3106,15 @@
         <v>0</v>
       </c>
       <c r="X23" s="6">
-        <f t="shared" ref="X23:X31" si="1">SUMIF(U$2:U$75,"&gt;=" &amp; W23,C$2:C$75)</f>
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W23,C$2:C$75)</f>
         <v>310</v>
       </c>
       <c r="Y23" s="6">
-        <f t="shared" ref="Y23:Y31" si="2">SUMIF(U$2:U$75,"&gt;=" &amp; W23,D$2:D$75)</f>
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W23,D$2:D$75)</f>
         <v>11</v>
       </c>
       <c r="Z23" s="8">
-        <f t="shared" ref="Z23:Z31" si="3">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
+        <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
         <v>28.340000000000003</v>
       </c>
       <c r="AA23" s="33"/>
@@ -3182,15 +3182,15 @@
         <v>0.5</v>
       </c>
       <c r="X24" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W24,C$2:C$75)</f>
+        <v>280</v>
+      </c>
+      <c r="Y24" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W24,D$2:D$75)</f>
+        <v>10</v>
+      </c>
+      <c r="Z24" s="8">
         <f t="shared" si="1"/>
-        <v>280</v>
-      </c>
-      <c r="Y24" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z24" s="8">
-        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="AA24" s="33"/>
@@ -3242,15 +3242,15 @@
         <v>1</v>
       </c>
       <c r="X25" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W25,C$2:C$75)</f>
+        <v>240</v>
+      </c>
+      <c r="Y25" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W25,D$2:D$75)</f>
+        <v>10</v>
+      </c>
+      <c r="Z25" s="8">
         <f t="shared" si="1"/>
-        <v>240</v>
-      </c>
-      <c r="Y25" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z25" s="8">
-        <f t="shared" si="3"/>
         <v>23.400000000000002</v>
       </c>
       <c r="AA25" s="33"/>
@@ -3312,15 +3312,15 @@
         <v>1.5</v>
       </c>
       <c r="X26" s="31">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W26,C$2:C$75)</f>
+        <v>227</v>
+      </c>
+      <c r="Y26" s="31">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W26,D$2:D$75)</f>
+        <v>10</v>
+      </c>
+      <c r="Z26" s="8">
         <f t="shared" si="1"/>
-        <v>227</v>
-      </c>
-      <c r="Y26" s="31">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z26" s="8">
-        <f t="shared" si="3"/>
         <v>22.555000000000003</v>
       </c>
       <c r="AA26" s="33"/>
@@ -3390,15 +3390,15 @@
         <v>2</v>
       </c>
       <c r="X27" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W27,C$2:C$75)</f>
+        <v>210</v>
+      </c>
+      <c r="Y27" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W27,D$2:D$75)</f>
+        <v>10</v>
+      </c>
+      <c r="Z27" s="8">
         <f t="shared" si="1"/>
-        <v>210</v>
-      </c>
-      <c r="Y27" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z27" s="8">
-        <f t="shared" si="3"/>
         <v>21.45</v>
       </c>
     </row>
@@ -3453,15 +3453,15 @@
         <v>2.5</v>
       </c>
       <c r="X28" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W28,C$2:C$75)</f>
+        <v>168</v>
+      </c>
+      <c r="Y28" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W28,D$2:D$75)</f>
+        <v>10</v>
+      </c>
+      <c r="Z28" s="8">
         <f t="shared" si="1"/>
-        <v>168</v>
-      </c>
-      <c r="Y28" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z28" s="8">
-        <f t="shared" si="3"/>
         <v>18.720000000000002</v>
       </c>
     </row>
@@ -3495,15 +3495,15 @@
         <v>3</v>
       </c>
       <c r="X29" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W29,C$2:C$75)</f>
+        <v>155</v>
+      </c>
+      <c r="Y29" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W29,D$2:D$75)</f>
+        <v>9</v>
+      </c>
+      <c r="Z29" s="8">
         <f t="shared" si="1"/>
-        <v>155</v>
-      </c>
-      <c r="Y29" s="6">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="Z29" s="8">
-        <f t="shared" si="3"/>
         <v>17.484999999999999</v>
       </c>
     </row>
@@ -3556,15 +3556,15 @@
         <v>3.5</v>
       </c>
       <c r="X30" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W30,C$2:C$75)</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="6">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W30,D$2:D$75)</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y30" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z30" s="8">
-        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -3596,15 +3596,15 @@
         <v>4</v>
       </c>
       <c r="X31" s="47">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W31,C$2:C$75)</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="47">
+        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W31,D$2:D$75)</f>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y31" s="47">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z31" s="9">
-        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -4734,122 +4734,122 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B54" s="23" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="C54" s="14">
-        <v>4</v>
-      </c>
-      <c r="E54" s="14">
-        <v>33</v>
-      </c>
-      <c r="G54" s="14">
-        <v>29</v>
-      </c>
-      <c r="H54" s="14">
-        <v>29</v>
-      </c>
-      <c r="I54" s="22"/>
-      <c r="J54" s="36">
-        <v>1</v>
-      </c>
-      <c r="K54" s="2">
-        <v>1</v>
-      </c>
-      <c r="L54" s="2">
-        <v>1</v>
-      </c>
-      <c r="M54" s="20">
-        <v>1</v>
-      </c>
-      <c r="N54" s="36">
-        <v>1</v>
-      </c>
-      <c r="O54" s="36">
-        <v>1</v>
-      </c>
-      <c r="P54" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q54" s="36">
-        <v>1</v>
-      </c>
-      <c r="R54" s="36">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I54" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="K54" s="34"/>
+      <c r="L54" s="34"/>
+      <c r="M54" s="36"/>
       <c r="S54" s="36">
         <v>1</v>
       </c>
-      <c r="T54" s="34"/>
+      <c r="T54" s="34">
+        <v>2</v>
+      </c>
       <c r="U54" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(Q54:T54)</f>
         <v>3</v>
       </c>
       <c r="V54" s="15"/>
       <c r="AA54" s="33"/>
     </row>
-    <row r="55" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="10"/>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B55" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C55" s="14">
-        <v>3</v>
-      </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="E55" s="14">
+        <v>33</v>
+      </c>
+      <c r="G55" s="14">
+        <v>29</v>
+      </c>
+      <c r="H55" s="14">
+        <v>29</v>
+      </c>
       <c r="I55" s="22"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="2"/>
+      <c r="J55" s="36">
+        <v>1</v>
+      </c>
+      <c r="K55" s="2">
+        <v>1</v>
+      </c>
       <c r="L55" s="2">
-        <v>0</v>
-      </c>
-      <c r="M55" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="M55" s="20">
+        <v>1</v>
+      </c>
       <c r="N55" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="O55" s="36"/>
-      <c r="P55" s="36"/>
-      <c r="Q55" s="36"/>
-      <c r="R55" s="36"/>
+        <v>1</v>
+      </c>
+      <c r="O55" s="36">
+        <v>1</v>
+      </c>
+      <c r="P55" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="36">
+        <v>1</v>
+      </c>
+      <c r="R55" s="36">
+        <v>1</v>
+      </c>
       <c r="S55" s="36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T55" s="34"/>
       <c r="U55" s="77">
         <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V55" s="15"/>
+      <c r="AA55" s="33"/>
+    </row>
+    <row r="56" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="10"/>
+      <c r="B56" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="14">
+        <v>3</v>
+      </c>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2">
+        <v>0</v>
+      </c>
+      <c r="M56" s="20"/>
+      <c r="N56" s="36">
         <v>0.5</v>
       </c>
-      <c r="V55" s="15"/>
-      <c r="W55" s="3"/>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B56" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="C56" s="14">
-        <v>1</v>
-      </c>
-      <c r="I56" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="K56" s="34"/>
-      <c r="L56" s="34"/>
-      <c r="M56" s="36"/>
+      <c r="O56" s="36"/>
+      <c r="P56" s="36"/>
+      <c r="Q56" s="36"/>
+      <c r="R56" s="36"/>
       <c r="S56" s="36">
-        <v>1</v>
-      </c>
-      <c r="T56" s="34">
-        <v>2</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="T56" s="34"/>
       <c r="U56" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="V56" s="15"/>
-      <c r="AA56" s="33"/>
+      <c r="W56" s="3"/>
     </row>
     <row r="57" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="10"/>
@@ -5478,7 +5478,7 @@
       </c>
       <c r="T71" s="34"/>
       <c r="U71" s="77">
-        <f t="shared" ref="U71:U74" si="4">SUM(Q71:T71)</f>
+        <f t="shared" ref="U71:U74" si="2">SUM(Q71:T71)</f>
         <v>1</v>
       </c>
       <c r="V71" s="15"/>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="T72" s="34"/>
       <c r="U72" s="77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="V72" s="15"/>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="T73" s="34"/>
       <c r="U73" s="77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="V73" s="15"/>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="T74" s="37"/>
       <c r="U74" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="V74" s="15"/>
@@ -5748,15 +5748,15 @@
       <c r="O79" s="68"/>
       <c r="P79" s="68"/>
       <c r="Q79" s="68">
-        <f t="shared" ref="Q79:S79" si="5">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
         <v>240</v>
       </c>
       <c r="R79" s="68">
-        <f t="shared" si="5"/>
+        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
         <v>240</v>
       </c>
       <c r="S79" s="68">
-        <f t="shared" si="5"/>
+        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
         <v>240</v>
       </c>
       <c r="T79" s="69"/>
@@ -5778,15 +5778,15 @@
       <c r="O80" s="70"/>
       <c r="P80" s="70"/>
       <c r="Q80" s="70">
-        <f t="shared" ref="Q80:S80" si="6">Q77/Q79</f>
+        <f t="shared" ref="Q80:S80" si="3">Q77/Q79</f>
         <v>0.8</v>
       </c>
       <c r="R80" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.88583333333333336</v>
       </c>
       <c r="S80" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.88012499999999994</v>
       </c>
       <c r="T80" s="71"/>
@@ -5805,15 +5805,15 @@
       <c r="O81" s="73"/>
       <c r="P81" s="73"/>
       <c r="Q81" s="73">
-        <f t="shared" ref="Q81:S81" si="7">Q79-Q77</f>
+        <f t="shared" ref="Q81:S81" si="4">Q79-Q77</f>
         <v>48</v>
       </c>
       <c r="R81" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>27.400000000000006</v>
       </c>
       <c r="S81" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>28.77000000000001</v>
       </c>
       <c r="T81" s="74"/>

</xml_diff>

<commit_message>
New lab on damped driven oscillators
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="201">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -784,6 +784,9 @@
   </si>
   <si>
     <t>Drag Force and Terminal Velocity [coffee filters]</t>
+  </si>
+  <si>
+    <t>Oscillators with Damping and Driving Forces</t>
   </si>
 </sst>
 </file>
@@ -1998,10 +2001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD116"/>
+  <dimension ref="A1:AD117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S65" sqref="S65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2205,7 +2208,7 @@
       </c>
       <c r="T3" s="60"/>
       <c r="U3" s="76">
-        <f t="shared" ref="U3:U70" si="0">SUM(Q3:T3)</f>
+        <f t="shared" ref="U3:U71" si="0">SUM(Q3:T3)</f>
         <v>3</v>
       </c>
       <c r="V3" s="80"/>
@@ -3106,16 +3109,16 @@
         <v>0</v>
       </c>
       <c r="X23" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W23,C$2:C$75)</f>
-        <v>310</v>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W23,C$2:C$76)</f>
+        <v>316</v>
       </c>
       <c r="Y23" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W23,D$2:D$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W23,D$2:D$76)</f>
         <v>11</v>
       </c>
       <c r="Z23" s="8">
         <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
-        <v>28.340000000000003</v>
+        <v>28.730000000000004</v>
       </c>
       <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
@@ -3182,16 +3185,16 @@
         <v>0.5</v>
       </c>
       <c r="X24" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W24,C$2:C$75)</f>
-        <v>280</v>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W24,C$2:C$76)</f>
+        <v>286</v>
       </c>
       <c r="Y24" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W24,D$2:D$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W24,D$2:D$76)</f>
         <v>10</v>
       </c>
       <c r="Z24" s="8">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>26.39</v>
       </c>
       <c r="AA24" s="33"/>
       <c r="AB24" s="33"/>
@@ -3242,16 +3245,16 @@
         <v>1</v>
       </c>
       <c r="X25" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W25,C$2:C$75)</f>
-        <v>240</v>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W25,C$2:C$76)</f>
+        <v>246</v>
       </c>
       <c r="Y25" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W25,D$2:D$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W25,D$2:D$76)</f>
         <v>10</v>
       </c>
       <c r="Z25" s="8">
         <f t="shared" si="1"/>
-        <v>23.400000000000002</v>
+        <v>23.790000000000003</v>
       </c>
       <c r="AA25" s="33"/>
       <c r="AB25" s="33"/>
@@ -3312,16 +3315,16 @@
         <v>1.5</v>
       </c>
       <c r="X26" s="31">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W26,C$2:C$75)</f>
-        <v>227</v>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W26,C$2:C$76)</f>
+        <v>233</v>
       </c>
       <c r="Y26" s="31">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W26,D$2:D$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W26,D$2:D$76)</f>
         <v>10</v>
       </c>
       <c r="Z26" s="8">
         <f t="shared" si="1"/>
-        <v>22.555000000000003</v>
+        <v>22.945</v>
       </c>
       <c r="AA26" s="33"/>
       <c r="AB26" s="33"/>
@@ -3390,16 +3393,16 @@
         <v>2</v>
       </c>
       <c r="X27" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W27,C$2:C$75)</f>
-        <v>210</v>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W27,C$2:C$76)</f>
+        <v>216</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W27,D$2:D$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W27,D$2:D$76)</f>
         <v>10</v>
       </c>
       <c r="Z27" s="8">
         <f t="shared" si="1"/>
-        <v>21.45</v>
+        <v>21.840000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
@@ -3453,11 +3456,11 @@
         <v>2.5</v>
       </c>
       <c r="X28" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W28,C$2:C$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W28,C$2:C$76)</f>
         <v>168</v>
       </c>
       <c r="Y28" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W28,D$2:D$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W28,D$2:D$76)</f>
         <v>10</v>
       </c>
       <c r="Z28" s="8">
@@ -3495,11 +3498,11 @@
         <v>3</v>
       </c>
       <c r="X29" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W29,C$2:C$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W29,C$2:C$76)</f>
         <v>155</v>
       </c>
       <c r="Y29" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W29,D$2:D$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W29,D$2:D$76)</f>
         <v>9</v>
       </c>
       <c r="Z29" s="8">
@@ -3556,11 +3559,11 @@
         <v>3.5</v>
       </c>
       <c r="X30" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W30,C$2:C$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W30,C$2:C$76)</f>
         <v>0</v>
       </c>
       <c r="Y30" s="6">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W30,D$2:D$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W30,D$2:D$76)</f>
         <v>0</v>
       </c>
       <c r="Z30" s="8">
@@ -3596,11 +3599,11 @@
         <v>4</v>
       </c>
       <c r="X31" s="47">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W31,C$2:C$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W31,C$2:C$76)</f>
         <v>0</v>
       </c>
       <c r="Y31" s="47">
-        <f>SUMIF(U$2:U$75,"&gt;=" &amp; W31,D$2:D$75)</f>
+        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W31,D$2:D$76)</f>
         <v>0</v>
       </c>
       <c r="Z31" s="9">
@@ -5172,217 +5175,201 @@
       <c r="V63" s="15"/>
       <c r="AA63" s="33"/>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
       <c r="B64" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" s="14">
+        <v>6</v>
+      </c>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="J64" s="36"/>
+      <c r="K64" s="34"/>
+      <c r="L64" s="34"/>
+      <c r="M64" s="36"/>
+      <c r="N64" s="36"/>
+      <c r="O64" s="36"/>
+      <c r="P64" s="36"/>
+      <c r="Q64" s="36"/>
+      <c r="R64" s="36"/>
+      <c r="S64" s="36">
+        <v>1</v>
+      </c>
+      <c r="T64" s="34">
+        <v>1</v>
+      </c>
+      <c r="U64" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="V64" s="15"/>
+      <c r="W64" s="3"/>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B65" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="C64" s="14">
+      <c r="C65" s="14">
         <v>3</v>
       </c>
-      <c r="I64" s="22"/>
-      <c r="L64" s="2">
-        <v>0</v>
-      </c>
-      <c r="S64" s="36">
-        <v>0</v>
-      </c>
-      <c r="T64" s="34"/>
-      <c r="U64" s="77">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V64" s="15"/>
-      <c r="Z64" s="6"/>
-      <c r="AA64" s="33"/>
-    </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A65" s="11" t="s">
+      <c r="I65" s="22"/>
+      <c r="L65" s="2">
+        <v>0</v>
+      </c>
+      <c r="S65" s="36">
+        <v>0</v>
+      </c>
+      <c r="T65" s="34"/>
+      <c r="U65" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V65" s="15"/>
+      <c r="Z65" s="6"/>
+      <c r="AA65" s="33"/>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A66" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="26" t="s">
+      <c r="B66" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="C65" s="13">
+      <c r="C66" s="13">
         <v>4</v>
       </c>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13">
+      <c r="D66" s="13"/>
+      <c r="E66" s="13">
         <v>39</v>
       </c>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="21"/>
-      <c r="J65" s="35">
-        <v>1</v>
-      </c>
-      <c r="K65" s="12"/>
-      <c r="L65" s="12">
-        <v>0</v>
-      </c>
-      <c r="M65" s="12"/>
-      <c r="N65" s="35">
-        <v>1</v>
-      </c>
-      <c r="O65" s="35"/>
-      <c r="P65" s="35"/>
-      <c r="Q65" s="35">
-        <v>1</v>
-      </c>
-      <c r="R65" s="35"/>
-      <c r="S65" s="35">
-        <v>0</v>
-      </c>
-      <c r="T65" s="35"/>
-      <c r="U65" s="78">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V65" s="15"/>
-      <c r="AA65" s="33"/>
-    </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B66" s="23" t="s">
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="35">
+        <v>1</v>
+      </c>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12">
+        <v>0</v>
+      </c>
+      <c r="M66" s="12"/>
+      <c r="N66" s="35">
+        <v>1</v>
+      </c>
+      <c r="O66" s="35"/>
+      <c r="P66" s="35"/>
+      <c r="Q66" s="35">
+        <v>1</v>
+      </c>
+      <c r="R66" s="35"/>
+      <c r="S66" s="35">
+        <v>0</v>
+      </c>
+      <c r="T66" s="35"/>
+      <c r="U66" s="78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V66" s="15"/>
+      <c r="AA66" s="33"/>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B67" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C67" s="14">
         <v>3</v>
       </c>
-      <c r="E66" s="14">
+      <c r="E67" s="14">
         <v>40</v>
       </c>
-      <c r="I66" s="22"/>
-      <c r="J66" s="36">
-        <v>1</v>
-      </c>
-      <c r="L66" s="2">
-        <v>0</v>
-      </c>
-      <c r="N66" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q66" s="36">
-        <v>1</v>
-      </c>
-      <c r="S66" s="36">
-        <v>0</v>
-      </c>
-      <c r="T66" s="34"/>
-      <c r="U66" s="77">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V66" s="15"/>
-    </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A67" s="11" t="s">
+      <c r="I67" s="22"/>
+      <c r="J67" s="36">
+        <v>1</v>
+      </c>
+      <c r="L67" s="2">
+        <v>0</v>
+      </c>
+      <c r="N67" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="36">
+        <v>1</v>
+      </c>
+      <c r="S67" s="36">
+        <v>0</v>
+      </c>
+      <c r="T67" s="34"/>
+      <c r="U67" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V67" s="15"/>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A68" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B67" s="26" t="s">
+      <c r="B68" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C67" s="13">
+      <c r="C68" s="13">
         <v>2</v>
       </c>
-      <c r="D67" s="13">
-        <v>0</v>
-      </c>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="21"/>
-      <c r="J67" s="35"/>
-      <c r="K67" s="12">
-        <v>1</v>
-      </c>
-      <c r="L67" s="12">
-        <v>1</v>
-      </c>
-      <c r="M67" s="12"/>
-      <c r="N67" s="35">
-        <v>1</v>
-      </c>
-      <c r="O67" s="35">
-        <v>1</v>
-      </c>
-      <c r="P67" s="35">
-        <v>1</v>
-      </c>
-      <c r="Q67" s="35">
-        <v>1</v>
-      </c>
-      <c r="R67" s="35">
-        <v>1</v>
-      </c>
-      <c r="S67" s="35">
+      <c r="D68" s="13">
+        <v>0</v>
+      </c>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="12">
+        <v>1</v>
+      </c>
+      <c r="L68" s="12">
+        <v>1</v>
+      </c>
+      <c r="M68" s="12"/>
+      <c r="N68" s="35">
+        <v>1</v>
+      </c>
+      <c r="O68" s="35">
+        <v>1</v>
+      </c>
+      <c r="P68" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="35">
+        <v>1</v>
+      </c>
+      <c r="R68" s="35">
+        <v>1</v>
+      </c>
+      <c r="S68" s="35">
         <v>0.9</v>
       </c>
-      <c r="T67" s="35"/>
-      <c r="U67" s="78">
+      <c r="T68" s="35"/>
+      <c r="U68" s="78">
         <f t="shared" si="0"/>
         <v>2.9</v>
       </c>
-      <c r="V67" s="15"/>
-    </row>
-    <row r="68" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="30"/>
-      <c r="B68" s="31" t="s">
+      <c r="V68" s="15"/>
+    </row>
+    <row r="69" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="30"/>
+      <c r="B69" s="31" t="s">
         <v>82</v>
-      </c>
-      <c r="C68" s="14">
-        <v>2</v>
-      </c>
-      <c r="D68" s="14">
-        <v>1</v>
-      </c>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="22"/>
-      <c r="J68" s="36"/>
-      <c r="K68" s="20"/>
-      <c r="L68" s="20">
-        <v>1</v>
-      </c>
-      <c r="M68" s="20"/>
-      <c r="N68" s="36">
-        <v>1</v>
-      </c>
-      <c r="O68" s="36">
-        <v>1</v>
-      </c>
-      <c r="P68" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="36">
-        <v>1</v>
-      </c>
-      <c r="R68" s="36">
-        <v>1</v>
-      </c>
-      <c r="S68" s="36">
-        <v>1</v>
-      </c>
-      <c r="T68" s="36"/>
-      <c r="U68" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V68" s="15"/>
-      <c r="W68" s="3"/>
-      <c r="X68"/>
-      <c r="Y68"/>
-      <c r="Z68"/>
-      <c r="AA68"/>
-      <c r="AB68"/>
-      <c r="AC68"/>
-      <c r="AD68"/>
-    </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B69" s="23" t="s">
-        <v>93</v>
       </c>
       <c r="C69" s="14">
         <v>2</v>
@@ -5390,87 +5377,115 @@
       <c r="D69" s="14">
         <v>1</v>
       </c>
-      <c r="I69" s="22" t="s">
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="36"/>
+      <c r="K69" s="20"/>
+      <c r="L69" s="20">
+        <v>1</v>
+      </c>
+      <c r="M69" s="20"/>
+      <c r="N69" s="36">
+        <v>1</v>
+      </c>
+      <c r="O69" s="36">
+        <v>1</v>
+      </c>
+      <c r="P69" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="36">
+        <v>1</v>
+      </c>
+      <c r="R69" s="36">
+        <v>1</v>
+      </c>
+      <c r="S69" s="36">
+        <v>1</v>
+      </c>
+      <c r="T69" s="36"/>
+      <c r="U69" s="77">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V69" s="15"/>
+      <c r="W69" s="3"/>
+      <c r="X69"/>
+      <c r="Y69"/>
+      <c r="Z69"/>
+      <c r="AA69"/>
+      <c r="AB69"/>
+      <c r="AC69"/>
+      <c r="AD69"/>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B70" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="14">
+        <v>2</v>
+      </c>
+      <c r="D70" s="14">
+        <v>1</v>
+      </c>
+      <c r="I70" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="K69" s="2">
-        <v>1</v>
-      </c>
-      <c r="L69" s="2">
-        <v>1</v>
-      </c>
-      <c r="T69" s="34"/>
-      <c r="U69" s="77">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V69" s="15"/>
-      <c r="X69" s="33"/>
-      <c r="Z69" s="6"/>
-    </row>
-    <row r="70" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="10"/>
-      <c r="B70" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C70" s="14">
-        <v>4</v>
-      </c>
-      <c r="D70" s="14">
-        <v>3</v>
-      </c>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="22"/>
-      <c r="J70" s="36"/>
       <c r="K70" s="2">
         <v>1</v>
       </c>
       <c r="L70" s="2">
-        <v>1</v>
-      </c>
-      <c r="M70" s="20"/>
-      <c r="N70" s="36">
-        <v>1</v>
-      </c>
-      <c r="O70" s="36">
-        <v>1</v>
-      </c>
-      <c r="P70" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q70" s="36">
-        <v>1</v>
-      </c>
-      <c r="R70" s="36">
-        <v>1</v>
-      </c>
-      <c r="S70" s="36">
         <v>1</v>
       </c>
       <c r="T70" s="34"/>
       <c r="U70" s="77">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V70" s="15"/>
+      <c r="X70" s="33"/>
+      <c r="Z70" s="6"/>
+    </row>
+    <row r="71" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="10"/>
+      <c r="B71" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71" s="14">
+        <v>4</v>
+      </c>
+      <c r="D71" s="14">
         <v>3</v>
       </c>
-      <c r="V70" s="15"/>
-      <c r="W70" s="3"/>
-      <c r="Z70" s="6"/>
-    </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B71" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="C71" s="14">
-        <v>1</v>
-      </c>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
       <c r="I71" s="22"/>
-      <c r="K71" s="34"/>
-      <c r="L71" s="34"/>
-      <c r="M71" s="36"/>
+      <c r="J71" s="36"/>
+      <c r="K71" s="2">
+        <v>1</v>
+      </c>
+      <c r="L71" s="2">
+        <v>1</v>
+      </c>
+      <c r="M71" s="20"/>
+      <c r="N71" s="36">
+        <v>1</v>
+      </c>
       <c r="O71" s="36">
+        <v>1</v>
+      </c>
+      <c r="P71" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q71" s="36">
+        <v>1</v>
+      </c>
+      <c r="R71" s="36">
         <v>1</v>
       </c>
       <c r="S71" s="36">
@@ -5478,47 +5493,25 @@
       </c>
       <c r="T71" s="34"/>
       <c r="U71" s="77">
-        <f t="shared" ref="U71:U74" si="2">SUM(Q71:T71)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="V71" s="15"/>
-      <c r="AA71" s="6"/>
-      <c r="AB71" s="6"/>
-      <c r="AC71" s="6"/>
-      <c r="AD71" s="6"/>
+      <c r="W71" s="3"/>
+      <c r="Z71" s="6"/>
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B72" s="23" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="C72" s="14">
         <v>1</v>
       </c>
-      <c r="D72" s="14">
-        <v>0</v>
-      </c>
-      <c r="I72" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="L72" s="2">
-        <v>0</v>
-      </c>
-      <c r="M72" s="20">
-        <v>1</v>
-      </c>
-      <c r="N72" s="36">
-        <v>1</v>
-      </c>
+      <c r="I72" s="22"/>
+      <c r="K72" s="34"/>
+      <c r="L72" s="34"/>
+      <c r="M72" s="36"/>
       <c r="O72" s="36">
-        <v>1</v>
-      </c>
-      <c r="P72" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q72" s="36">
-        <v>1</v>
-      </c>
-      <c r="R72" s="36">
         <v>1</v>
       </c>
       <c r="S72" s="36">
@@ -5526,35 +5519,34 @@
       </c>
       <c r="T72" s="34"/>
       <c r="U72" s="77">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" ref="U72:U75" si="2">SUM(Q72:T72)</f>
+        <v>1</v>
       </c>
       <c r="V72" s="15"/>
-    </row>
-    <row r="73" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="10"/>
+      <c r="AA72" s="6"/>
+      <c r="AB72" s="6"/>
+      <c r="AC72" s="6"/>
+      <c r="AD72" s="6"/>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B73" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C73" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D73" s="14">
-        <v>1</v>
-      </c>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="22"/>
-      <c r="J73" s="36"/>
-      <c r="K73" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I73" s="22" t="s">
+        <v>91</v>
       </c>
       <c r="L73" s="2">
-        <v>1</v>
-      </c>
-      <c r="M73" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="M73" s="20">
+        <v>1</v>
+      </c>
       <c r="N73" s="36">
         <v>1</v>
       </c>
@@ -5579,131 +5571,146 @@
         <v>3</v>
       </c>
       <c r="V73" s="15"/>
-      <c r="W73" s="3"/>
-      <c r="X73"/>
-      <c r="Y73"/>
-      <c r="Z73"/>
-      <c r="AA73"/>
-      <c r="AB73"/>
-      <c r="AC73"/>
-      <c r="AD73"/>
-    </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B74" s="24" t="s">
+    </row>
+    <row r="74" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="10"/>
+      <c r="B74" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="14">
+        <v>3</v>
+      </c>
+      <c r="D74" s="14">
+        <v>1</v>
+      </c>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="36"/>
+      <c r="K74" s="2">
+        <v>1</v>
+      </c>
+      <c r="L74" s="2">
+        <v>1</v>
+      </c>
+      <c r="M74" s="20"/>
+      <c r="N74" s="36">
+        <v>1</v>
+      </c>
+      <c r="O74" s="36">
+        <v>1</v>
+      </c>
+      <c r="P74" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="36">
+        <v>1</v>
+      </c>
+      <c r="R74" s="36">
+        <v>1</v>
+      </c>
+      <c r="S74" s="36">
+        <v>1</v>
+      </c>
+      <c r="T74" s="34"/>
+      <c r="U74" s="77">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="V74" s="15"/>
+      <c r="W74" s="3"/>
+      <c r="X74"/>
+      <c r="Y74"/>
+      <c r="Z74"/>
+      <c r="AA74"/>
+      <c r="AB74"/>
+      <c r="AC74"/>
+      <c r="AD74"/>
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B75" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C74" s="27">
+      <c r="C75" s="27">
         <v>4</v>
       </c>
-      <c r="D74" s="27">
-        <v>0</v>
-      </c>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="27"/>
-      <c r="H74" s="27"/>
-      <c r="I74" s="29"/>
-      <c r="J74" s="37"/>
-      <c r="K74" s="28">
-        <v>1</v>
-      </c>
-      <c r="L74" s="28">
-        <v>0</v>
-      </c>
-      <c r="M74" s="28"/>
-      <c r="N74" s="37"/>
-      <c r="O74" s="37"/>
-      <c r="P74" s="37">
-        <v>1</v>
-      </c>
-      <c r="Q74" s="37">
-        <v>1</v>
-      </c>
-      <c r="R74" s="37">
-        <v>1</v>
-      </c>
-      <c r="S74" s="37">
-        <v>0</v>
-      </c>
-      <c r="T74" s="37"/>
-      <c r="U74" s="79">
+      <c r="D75" s="27">
+        <v>0</v>
+      </c>
+      <c r="E75" s="27"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="27"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="37"/>
+      <c r="K75" s="28">
+        <v>1</v>
+      </c>
+      <c r="L75" s="28">
+        <v>0</v>
+      </c>
+      <c r="M75" s="28"/>
+      <c r="N75" s="37"/>
+      <c r="O75" s="37"/>
+      <c r="P75" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="37">
+        <v>1</v>
+      </c>
+      <c r="R75" s="37">
+        <v>1</v>
+      </c>
+      <c r="S75" s="37">
+        <v>0</v>
+      </c>
+      <c r="T75" s="37"/>
+      <c r="U75" s="79">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="V74" s="15"/>
-    </row>
-    <row r="75" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="11"/>
       <c r="V75" s="15"/>
-      <c r="Y75" s="33"/>
-    </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I76" s="64" t="s">
+    </row>
+    <row r="76" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="11"/>
+      <c r="V76" s="15"/>
+      <c r="Y76" s="33"/>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I77" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="J76" s="85"/>
-      <c r="K76" s="65"/>
-      <c r="L76" s="65"/>
-      <c r="M76" s="65"/>
-      <c r="N76" s="65"/>
-      <c r="O76" s="65"/>
-      <c r="P76" s="65"/>
-      <c r="Q76" s="65">
-        <f t="array" ref="Q76">SUM($C2:$C74*(Q2:Q74&gt;=0.9)*($U2:$U74&gt;=$W$12))</f>
+      <c r="J77" s="85"/>
+      <c r="K77" s="65"/>
+      <c r="L77" s="65"/>
+      <c r="M77" s="65"/>
+      <c r="N77" s="65"/>
+      <c r="O77" s="65"/>
+      <c r="P77" s="65"/>
+      <c r="Q77" s="65">
+        <f t="array" ref="Q77">SUM($C2:$C75*(Q2:Q75&gt;=0.9)*($U2:$U75&gt;=$W$12))</f>
         <v>185</v>
       </c>
-      <c r="R76" s="65">
-        <f t="array" ref="R76">SUM($C2:$C74*(R2:R74&gt;=0.9)*($U2:$U74&gt;=$W$12))</f>
+      <c r="R77" s="65">
+        <f t="array" ref="R77">SUM($C2:$C75*(R2:R75&gt;=0.9)*($U2:$U75&gt;=$W$12))</f>
         <v>193</v>
       </c>
-      <c r="S76" s="65">
-        <f t="array" ref="S76">SUM($C2:$C74*(S2:S74&gt;=0.9)*($U2:$U74&gt;=$W$12))</f>
-        <v>198</v>
-      </c>
-      <c r="T76" s="66"/>
-      <c r="V76" s="15"/>
-      <c r="AA76" s="6"/>
-      <c r="AB76" s="6"/>
-      <c r="AC76" s="6"/>
-      <c r="AD76" s="6"/>
-    </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I77" s="67" t="s">
+      <c r="S77" s="65">
+        <f t="array" ref="S77">SUM($C2:$C75*(S2:S75&gt;=0.9)*($U2:$U75&gt;=$W$12))</f>
+        <v>204</v>
+      </c>
+      <c r="T77" s="66"/>
+      <c r="V77" s="15"/>
+      <c r="AA77" s="6"/>
+      <c r="AB77" s="6"/>
+      <c r="AC77" s="6"/>
+      <c r="AD77" s="6"/>
+    </row>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I78" s="67" t="s">
         <v>100</v>
-      </c>
-      <c r="J77" s="86"/>
-      <c r="K77" s="68"/>
-      <c r="L77" s="68"/>
-      <c r="M77" s="68"/>
-      <c r="N77" s="68"/>
-      <c r="O77" s="68"/>
-      <c r="P77" s="68"/>
-      <c r="Q77" s="68">
-        <f t="array" ref="Q77">SUM($C2:$C74*Q2:Q74*($U2:$U74&gt;=$W$12))</f>
-        <v>192</v>
-      </c>
-      <c r="R77" s="68">
-        <f t="array" ref="R77">SUM($C2:$C74*R2:R74*($U2:$U74&gt;=$W$12))</f>
-        <v>212.6</v>
-      </c>
-      <c r="S77" s="68">
-        <f t="array" ref="S77">SUM($C2:$C74*S2:S74*($U2:$U74&gt;=$W$12))</f>
-        <v>211.23</v>
-      </c>
-      <c r="T77" s="69"/>
-      <c r="V77" s="15"/>
-    </row>
-    <row r="78" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="10"/>
-      <c r="B78" s="23"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="67" t="s">
-        <v>99</v>
       </c>
       <c r="J78" s="86"/>
       <c r="K78" s="68"/>
@@ -5713,32 +5720,31 @@
       <c r="O78" s="68"/>
       <c r="P78" s="68"/>
       <c r="Q78" s="68">
-        <f t="array" ref="Q78">SUM($C$2:$C$74*(Q$2:Q$74&gt;=0.1)*($U$2:$U$74&gt;=$W$12))</f>
-        <v>199</v>
+        <f t="array" ref="Q78">SUM($C2:$C75*Q2:Q75*($U2:$U75&gt;=$W$12))</f>
+        <v>192</v>
       </c>
       <c r="R78" s="68">
-        <f t="array" ref="R78">SUM($C$2:$C$74*(R$2:R$74&gt;=0.1)*($U$2:$U$74&gt;=$W$12))</f>
-        <v>222</v>
+        <f t="array" ref="R78">SUM($C2:$C75*R2:R75*($U2:$U75&gt;=$W$12))</f>
+        <v>212.6</v>
       </c>
       <c r="S78" s="68">
-        <f t="array" ref="S78">SUM($C$2:$C$74*(S$2:S$74&gt;=0.1)*($U$2:$U$74&gt;=$W$12))</f>
-        <v>221</v>
+        <f t="array" ref="S78">SUM($C2:$C75*S2:S75*($U2:$U75&gt;=$W$12))</f>
+        <v>217.23</v>
       </c>
       <c r="T78" s="69"/>
-      <c r="U78" s="3"/>
       <c r="V78" s="15"/>
-      <c r="W78" s="3"/>
-      <c r="X78"/>
-      <c r="Y78"/>
-      <c r="Z78"/>
-      <c r="AA78"/>
-      <c r="AB78"/>
-      <c r="AC78"/>
-      <c r="AD78"/>
-    </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="10"/>
+      <c r="B79" s="23"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
       <c r="I79" s="67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J79" s="86"/>
       <c r="K79" s="68"/>
@@ -5748,92 +5754,118 @@
       <c r="O79" s="68"/>
       <c r="P79" s="68"/>
       <c r="Q79" s="68">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>240</v>
+        <f t="array" ref="Q79">SUM($C$2:$C$75*(Q$2:Q$75&gt;=0.1)*($U$2:$U$75&gt;=$W$12))</f>
+        <v>199</v>
       </c>
       <c r="R79" s="68">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>240</v>
+        <f t="array" ref="R79">SUM($C$2:$C$75*(R$2:R$75&gt;=0.1)*($U$2:$U$75&gt;=$W$12))</f>
+        <v>222</v>
       </c>
       <c r="S79" s="68">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>240</v>
+        <f t="array" ref="S79">SUM($C$2:$C$75*(S$2:S$75&gt;=0.1)*($U$2:$U$75&gt;=$W$12))</f>
+        <v>227</v>
       </c>
       <c r="T79" s="69"/>
+      <c r="U79" s="3"/>
       <c r="V79" s="15"/>
-      <c r="AA79" s="6"/>
-      <c r="AB79" s="6"/>
-      <c r="AC79" s="6"/>
-      <c r="AD79" s="6"/>
+      <c r="W79" s="3"/>
+      <c r="X79"/>
+      <c r="Y79"/>
+      <c r="Z79"/>
+      <c r="AA79"/>
+      <c r="AB79"/>
+      <c r="AC79"/>
+      <c r="AD79"/>
     </row>
     <row r="80" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I80" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="J80" s="86"/>
+      <c r="K80" s="68"/>
+      <c r="L80" s="68"/>
+      <c r="M80" s="68"/>
+      <c r="N80" s="68"/>
+      <c r="O80" s="68"/>
+      <c r="P80" s="68"/>
+      <c r="Q80" s="68">
+        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>246</v>
+      </c>
+      <c r="R80" s="68">
+        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>246</v>
+      </c>
+      <c r="S80" s="68">
+        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>246</v>
+      </c>
+      <c r="T80" s="69"/>
+      <c r="V80" s="15"/>
+      <c r="AA80" s="6"/>
+      <c r="AB80" s="6"/>
+      <c r="AC80" s="6"/>
+      <c r="AD80" s="6"/>
+    </row>
+    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I81" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="J80" s="86"/>
-      <c r="K80" s="70"/>
-      <c r="L80" s="70"/>
-      <c r="M80" s="70"/>
-      <c r="N80" s="70"/>
-      <c r="O80" s="70"/>
-      <c r="P80" s="70"/>
-      <c r="Q80" s="70">
-        <f t="shared" ref="Q80:S80" si="3">Q77/Q79</f>
-        <v>0.8</v>
-      </c>
-      <c r="R80" s="70">
+      <c r="J81" s="86"/>
+      <c r="K81" s="70"/>
+      <c r="L81" s="70"/>
+      <c r="M81" s="70"/>
+      <c r="N81" s="70"/>
+      <c r="O81" s="70"/>
+      <c r="P81" s="70"/>
+      <c r="Q81" s="70">
+        <f t="shared" ref="Q81:S81" si="3">Q78/Q80</f>
+        <v>0.78048780487804881</v>
+      </c>
+      <c r="R81" s="70">
         <f t="shared" si="3"/>
-        <v>0.88583333333333336</v>
-      </c>
-      <c r="S80" s="70">
+        <v>0.86422764227642279</v>
+      </c>
+      <c r="S81" s="70">
         <f t="shared" si="3"/>
-        <v>0.88012499999999994</v>
-      </c>
-      <c r="T80" s="71"/>
-      <c r="V80" s="15"/>
-    </row>
-    <row r="81" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C81" s="33"/>
-      <c r="I81" s="72" t="s">
+        <v>0.88304878048780489</v>
+      </c>
+      <c r="T81" s="71"/>
+      <c r="V81" s="15"/>
+    </row>
+    <row r="82" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C82" s="33"/>
+      <c r="I82" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="J81" s="87"/>
-      <c r="K81" s="73"/>
-      <c r="L81" s="73"/>
-      <c r="M81" s="73"/>
-      <c r="N81" s="73"/>
-      <c r="O81" s="73"/>
-      <c r="P81" s="73"/>
-      <c r="Q81" s="73">
-        <f t="shared" ref="Q81:S81" si="4">Q79-Q77</f>
-        <v>48</v>
-      </c>
-      <c r="R81" s="73">
+      <c r="J82" s="87"/>
+      <c r="K82" s="73"/>
+      <c r="L82" s="73"/>
+      <c r="M82" s="73"/>
+      <c r="N82" s="73"/>
+      <c r="O82" s="73"/>
+      <c r="P82" s="73"/>
+      <c r="Q82" s="73">
+        <f t="shared" ref="Q82:S82" si="4">Q80-Q78</f>
+        <v>54</v>
+      </c>
+      <c r="R82" s="73">
         <f t="shared" si="4"/>
-        <v>27.400000000000006</v>
-      </c>
-      <c r="S81" s="73">
+        <v>33.400000000000006</v>
+      </c>
+      <c r="S82" s="73">
         <f t="shared" si="4"/>
         <v>28.77000000000001</v>
       </c>
-      <c r="T81" s="74"/>
-      <c r="V81" s="15"/>
-      <c r="AA81" s="6"/>
-      <c r="AB81" s="6"/>
-      <c r="AC81" s="6"/>
-      <c r="AD81" s="6"/>
-    </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="C82" s="33"/>
+      <c r="T82" s="74"/>
       <c r="V82" s="15"/>
+      <c r="AA82" s="6"/>
+      <c r="AB82" s="6"/>
+      <c r="AC82" s="6"/>
+      <c r="AD82" s="6"/>
     </row>
     <row r="83" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C83" s="33"/>
-      <c r="I83" s="14"/>
-      <c r="J83" s="14"/>
-      <c r="K83" s="14"/>
-      <c r="L83" s="14"/>
-      <c r="N83" s="14"/>
       <c r="V83" s="15"/>
     </row>
     <row r="84" spans="1:30" x14ac:dyDescent="0.3">
@@ -5846,6 +5878,7 @@
       <c r="V84" s="15"/>
     </row>
     <row r="85" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C85" s="33"/>
       <c r="I85" s="14"/>
       <c r="J85" s="14"/>
       <c r="K85" s="14"/>
@@ -5860,7 +5893,6 @@
       <c r="L86" s="14"/>
       <c r="N86" s="14"/>
       <c r="V86" s="15"/>
-      <c r="Z86" s="33"/>
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I87" s="14"/>
@@ -5869,6 +5901,7 @@
       <c r="L87" s="14"/>
       <c r="N87" s="14"/>
       <c r="V87" s="15"/>
+      <c r="Z87" s="33"/>
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I88" s="14"/>
@@ -5876,6 +5909,7 @@
       <c r="K88" s="14"/>
       <c r="L88" s="14"/>
       <c r="N88" s="14"/>
+      <c r="V88" s="15"/>
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I89" s="14"/>
@@ -5891,64 +5925,71 @@
       <c r="L90" s="14"/>
       <c r="N90" s="14"/>
     </row>
-    <row r="91" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="10"/>
-      <c r="B91" s="23"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14"/>
-      <c r="H91" s="14"/>
-      <c r="I91" s="20"/>
-      <c r="J91" s="36"/>
-      <c r="K91" s="2"/>
-      <c r="L91" s="2"/>
-      <c r="M91" s="20"/>
-      <c r="N91" s="36"/>
-      <c r="O91" s="36"/>
-      <c r="P91" s="36"/>
-      <c r="Q91" s="36"/>
-      <c r="R91" s="36"/>
-      <c r="S91" s="36"/>
-      <c r="T91" s="2"/>
-      <c r="U91" s="3"/>
-      <c r="V91" s="3"/>
-      <c r="W91" s="3"/>
-      <c r="X91"/>
-      <c r="Y91"/>
-      <c r="Z91"/>
-      <c r="AA91"/>
-      <c r="AB91"/>
-      <c r="AC91"/>
-      <c r="AD91"/>
-    </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA94" s="6"/>
-      <c r="AB94" s="6"/>
-      <c r="AC94" s="6"/>
-      <c r="AD94" s="6"/>
-    </row>
-    <row r="98" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA98" s="6"/>
-      <c r="AB98" s="6"/>
-      <c r="AC98" s="6"/>
-      <c r="AD98" s="6"/>
-    </row>
-    <row r="103" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA103" s="6"/>
-      <c r="AB103" s="6"/>
-      <c r="AC103" s="6"/>
-      <c r="AD103" s="6"/>
-    </row>
-    <row r="116" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA116" s="33"/>
-      <c r="AB116" s="33"/>
-      <c r="AC116" s="33"/>
-      <c r="AD116" s="33"/>
+    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
+      <c r="N91" s="14"/>
+    </row>
+    <row r="92" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="10"/>
+      <c r="B92" s="23"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="20"/>
+      <c r="J92" s="36"/>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="20"/>
+      <c r="N92" s="36"/>
+      <c r="O92" s="36"/>
+      <c r="P92" s="36"/>
+      <c r="Q92" s="36"/>
+      <c r="R92" s="36"/>
+      <c r="S92" s="36"/>
+      <c r="T92" s="2"/>
+      <c r="U92" s="3"/>
+      <c r="V92" s="3"/>
+      <c r="W92" s="3"/>
+      <c r="X92"/>
+      <c r="Y92"/>
+      <c r="Z92"/>
+      <c r="AA92"/>
+      <c r="AB92"/>
+      <c r="AC92"/>
+      <c r="AD92"/>
+    </row>
+    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA95" s="6"/>
+      <c r="AB95" s="6"/>
+      <c r="AC95" s="6"/>
+      <c r="AD95" s="6"/>
+    </row>
+    <row r="99" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA99" s="6"/>
+      <c r="AB99" s="6"/>
+      <c r="AC99" s="6"/>
+      <c r="AD99" s="6"/>
+    </row>
+    <row r="104" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA104" s="6"/>
+      <c r="AB104" s="6"/>
+      <c r="AC104" s="6"/>
+      <c r="AD104" s="6"/>
+    </row>
+    <row r="117" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA117" s="33"/>
+      <c r="AB117" s="33"/>
+      <c r="AC117" s="33"/>
+      <c r="AD117" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U74">
+  <conditionalFormatting sqref="B2:U75">
     <cfRule type="expression" dxfId="2" priority="37" stopIfTrue="1">
       <formula>$U2&gt;=(0.5+$W$12)</formula>
     </cfRule>

</xml_diff>

<commit_message>
New lab: exercises in relativity
Activity 1 is a couple of problems related to swimming in a river with current, in preparation for discussing the Michaelson Morley experiment.  Activity 2 has to do with drawing Minkowski diagrams and doing Galilean Transformations.
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="202">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -787,6 +787,9 @@
   </si>
   <si>
     <t>Oscillators with Damping and Driving Forces</t>
+  </si>
+  <si>
+    <t>Exercises in Relativity</t>
   </si>
 </sst>
 </file>
@@ -2001,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD117"/>
+  <dimension ref="A1:AD118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S65" sqref="S65"/>
+    <sheetView tabSelected="1" topLeftCell="H55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W65" sqref="W65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2208,7 +2211,7 @@
       </c>
       <c r="T3" s="60"/>
       <c r="U3" s="76">
-        <f t="shared" ref="U3:U71" si="0">SUM(Q3:T3)</f>
+        <f t="shared" ref="U3:U72" si="0">SUM(Q3:T3)</f>
         <v>3</v>
       </c>
       <c r="V3" s="80"/>
@@ -3109,16 +3112,16 @@
         <v>0</v>
       </c>
       <c r="X23" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W23,C$2:C$76)</f>
-        <v>316</v>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W23,C$2:C$77)</f>
+        <v>319</v>
       </c>
       <c r="Y23" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W23,D$2:D$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W23,D$2:D$77)</f>
         <v>11</v>
       </c>
       <c r="Z23" s="8">
         <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
-        <v>28.730000000000004</v>
+        <v>28.925000000000004</v>
       </c>
       <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
@@ -3185,16 +3188,16 @@
         <v>0.5</v>
       </c>
       <c r="X24" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W24,C$2:C$76)</f>
-        <v>286</v>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W24,C$2:C$77)</f>
+        <v>289</v>
       </c>
       <c r="Y24" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W24,D$2:D$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W24,D$2:D$77)</f>
         <v>10</v>
       </c>
       <c r="Z24" s="8">
         <f t="shared" si="1"/>
-        <v>26.39</v>
+        <v>26.585000000000004</v>
       </c>
       <c r="AA24" s="33"/>
       <c r="AB24" s="33"/>
@@ -3245,16 +3248,16 @@
         <v>1</v>
       </c>
       <c r="X25" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W25,C$2:C$76)</f>
-        <v>246</v>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W25,C$2:C$77)</f>
+        <v>249</v>
       </c>
       <c r="Y25" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W25,D$2:D$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W25,D$2:D$77)</f>
         <v>10</v>
       </c>
       <c r="Z25" s="8">
         <f t="shared" si="1"/>
-        <v>23.790000000000003</v>
+        <v>23.985000000000003</v>
       </c>
       <c r="AA25" s="33"/>
       <c r="AB25" s="33"/>
@@ -3315,11 +3318,11 @@
         <v>1.5</v>
       </c>
       <c r="X26" s="31">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W26,C$2:C$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W26,C$2:C$77)</f>
         <v>233</v>
       </c>
       <c r="Y26" s="31">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W26,D$2:D$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W26,D$2:D$77)</f>
         <v>10</v>
       </c>
       <c r="Z26" s="8">
@@ -3393,11 +3396,11 @@
         <v>2</v>
       </c>
       <c r="X27" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W27,C$2:C$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W27,C$2:C$77)</f>
         <v>216</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W27,D$2:D$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W27,D$2:D$77)</f>
         <v>10</v>
       </c>
       <c r="Z27" s="8">
@@ -3456,11 +3459,11 @@
         <v>2.5</v>
       </c>
       <c r="X28" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W28,C$2:C$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W28,C$2:C$77)</f>
         <v>168</v>
       </c>
       <c r="Y28" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W28,D$2:D$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W28,D$2:D$77)</f>
         <v>10</v>
       </c>
       <c r="Z28" s="8">
@@ -3498,11 +3501,11 @@
         <v>3</v>
       </c>
       <c r="X29" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W29,C$2:C$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W29,C$2:C$77)</f>
         <v>155</v>
       </c>
       <c r="Y29" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W29,D$2:D$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W29,D$2:D$77)</f>
         <v>9</v>
       </c>
       <c r="Z29" s="8">
@@ -3559,11 +3562,11 @@
         <v>3.5</v>
       </c>
       <c r="X30" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W30,C$2:C$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W30,C$2:C$77)</f>
         <v>0</v>
       </c>
       <c r="Y30" s="6">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W30,D$2:D$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W30,D$2:D$77)</f>
         <v>0</v>
       </c>
       <c r="Z30" s="8">
@@ -3599,11 +3602,11 @@
         <v>4</v>
       </c>
       <c r="X31" s="47">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W31,C$2:C$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W31,C$2:C$77)</f>
         <v>0</v>
       </c>
       <c r="Y31" s="47">
-        <f>SUMIF(U$2:U$76,"&gt;=" &amp; W31,D$2:D$76)</f>
+        <f>SUMIF(U$2:U$77,"&gt;=" &amp; W31,D$2:D$77)</f>
         <v>0</v>
       </c>
       <c r="Z31" s="9">
@@ -5315,115 +5318,97 @@
       </c>
       <c r="V67" s="15"/>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A68" s="11" t="s">
+    <row r="68" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="10"/>
+      <c r="B68" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C68" s="14">
+        <v>3</v>
+      </c>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="J68" s="36"/>
+      <c r="K68" s="34"/>
+      <c r="L68" s="34"/>
+      <c r="M68" s="36"/>
+      <c r="N68" s="36"/>
+      <c r="O68" s="36"/>
+      <c r="P68" s="36"/>
+      <c r="Q68" s="36"/>
+      <c r="R68" s="36"/>
+      <c r="S68" s="36">
+        <v>1</v>
+      </c>
+      <c r="T68" s="34"/>
+      <c r="U68" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V68" s="15"/>
+      <c r="W68" s="3"/>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A69" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="26" t="s">
+      <c r="B69" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C68" s="13">
+      <c r="C69" s="13">
         <v>2</v>
       </c>
-      <c r="D68" s="13">
+      <c r="D69" s="13">
         <v>0</v>
       </c>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="21"/>
-      <c r="J68" s="35"/>
-      <c r="K68" s="12">
-        <v>1</v>
-      </c>
-      <c r="L68" s="12">
-        <v>1</v>
-      </c>
-      <c r="M68" s="12"/>
-      <c r="N68" s="35">
-        <v>1</v>
-      </c>
-      <c r="O68" s="35">
-        <v>1</v>
-      </c>
-      <c r="P68" s="35">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="35">
-        <v>1</v>
-      </c>
-      <c r="R68" s="35">
-        <v>1</v>
-      </c>
-      <c r="S68" s="35">
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="12">
+        <v>1</v>
+      </c>
+      <c r="L69" s="12">
+        <v>1</v>
+      </c>
+      <c r="M69" s="12"/>
+      <c r="N69" s="35">
+        <v>1</v>
+      </c>
+      <c r="O69" s="35">
+        <v>1</v>
+      </c>
+      <c r="P69" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="35">
+        <v>1</v>
+      </c>
+      <c r="R69" s="35">
+        <v>1</v>
+      </c>
+      <c r="S69" s="35">
         <v>0.9</v>
       </c>
-      <c r="T68" s="35"/>
-      <c r="U68" s="78">
+      <c r="T69" s="35"/>
+      <c r="U69" s="78">
         <f t="shared" si="0"/>
         <v>2.9</v>
       </c>
-      <c r="V68" s="15"/>
-    </row>
-    <row r="69" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="30"/>
-      <c r="B69" s="31" t="s">
+      <c r="V69" s="15"/>
+    </row>
+    <row r="70" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="30"/>
+      <c r="B70" s="31" t="s">
         <v>82</v>
-      </c>
-      <c r="C69" s="14">
-        <v>2</v>
-      </c>
-      <c r="D69" s="14">
-        <v>1</v>
-      </c>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="22"/>
-      <c r="J69" s="36"/>
-      <c r="K69" s="20"/>
-      <c r="L69" s="20">
-        <v>1</v>
-      </c>
-      <c r="M69" s="20"/>
-      <c r="N69" s="36">
-        <v>1</v>
-      </c>
-      <c r="O69" s="36">
-        <v>1</v>
-      </c>
-      <c r="P69" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q69" s="36">
-        <v>1</v>
-      </c>
-      <c r="R69" s="36">
-        <v>1</v>
-      </c>
-      <c r="S69" s="36">
-        <v>1</v>
-      </c>
-      <c r="T69" s="36"/>
-      <c r="U69" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V69" s="15"/>
-      <c r="W69" s="3"/>
-      <c r="X69"/>
-      <c r="Y69"/>
-      <c r="Z69"/>
-      <c r="AA69"/>
-      <c r="AB69"/>
-      <c r="AC69"/>
-      <c r="AD69"/>
-    </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B70" s="23" t="s">
-        <v>93</v>
       </c>
       <c r="C70" s="14">
         <v>2</v>
@@ -5431,87 +5416,115 @@
       <c r="D70" s="14">
         <v>1</v>
       </c>
-      <c r="I70" s="22" t="s">
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="22"/>
+      <c r="J70" s="36"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="20">
+        <v>1</v>
+      </c>
+      <c r="M70" s="20"/>
+      <c r="N70" s="36">
+        <v>1</v>
+      </c>
+      <c r="O70" s="36">
+        <v>1</v>
+      </c>
+      <c r="P70" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q70" s="36">
+        <v>1</v>
+      </c>
+      <c r="R70" s="36">
+        <v>1</v>
+      </c>
+      <c r="S70" s="36">
+        <v>1</v>
+      </c>
+      <c r="T70" s="36"/>
+      <c r="U70" s="77">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V70" s="15"/>
+      <c r="W70" s="3"/>
+      <c r="X70"/>
+      <c r="Y70"/>
+      <c r="Z70"/>
+      <c r="AA70"/>
+      <c r="AB70"/>
+      <c r="AC70"/>
+      <c r="AD70"/>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B71" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" s="14">
+        <v>2</v>
+      </c>
+      <c r="D71" s="14">
+        <v>1</v>
+      </c>
+      <c r="I71" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="K70" s="2">
-        <v>1</v>
-      </c>
-      <c r="L70" s="2">
-        <v>1</v>
-      </c>
-      <c r="T70" s="34"/>
-      <c r="U70" s="77">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V70" s="15"/>
-      <c r="X70" s="33"/>
-      <c r="Z70" s="6"/>
-    </row>
-    <row r="71" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="10"/>
-      <c r="B71" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C71" s="14">
-        <v>4</v>
-      </c>
-      <c r="D71" s="14">
-        <v>3</v>
-      </c>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="22"/>
-      <c r="J71" s="36"/>
       <c r="K71" s="2">
         <v>1</v>
       </c>
       <c r="L71" s="2">
-        <v>1</v>
-      </c>
-      <c r="M71" s="20"/>
-      <c r="N71" s="36">
-        <v>1</v>
-      </c>
-      <c r="O71" s="36">
-        <v>1</v>
-      </c>
-      <c r="P71" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q71" s="36">
-        <v>1</v>
-      </c>
-      <c r="R71" s="36">
-        <v>1</v>
-      </c>
-      <c r="S71" s="36">
         <v>1</v>
       </c>
       <c r="T71" s="34"/>
       <c r="U71" s="77">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V71" s="15"/>
+      <c r="X71" s="33"/>
+      <c r="Z71" s="6"/>
+    </row>
+    <row r="72" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="10"/>
+      <c r="B72" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="14">
+        <v>4</v>
+      </c>
+      <c r="D72" s="14">
         <v>3</v>
       </c>
-      <c r="V71" s="15"/>
-      <c r="W71" s="3"/>
-      <c r="Z71" s="6"/>
-    </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B72" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="C72" s="14">
-        <v>1</v>
-      </c>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
       <c r="I72" s="22"/>
-      <c r="K72" s="34"/>
-      <c r="L72" s="34"/>
-      <c r="M72" s="36"/>
+      <c r="J72" s="36"/>
+      <c r="K72" s="2">
+        <v>1</v>
+      </c>
+      <c r="L72" s="2">
+        <v>1</v>
+      </c>
+      <c r="M72" s="20"/>
+      <c r="N72" s="36">
+        <v>1</v>
+      </c>
       <c r="O72" s="36">
+        <v>1</v>
+      </c>
+      <c r="P72" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q72" s="36">
+        <v>1</v>
+      </c>
+      <c r="R72" s="36">
         <v>1</v>
       </c>
       <c r="S72" s="36">
@@ -5519,47 +5532,25 @@
       </c>
       <c r="T72" s="34"/>
       <c r="U72" s="77">
-        <f t="shared" ref="U72:U75" si="2">SUM(Q72:T72)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="V72" s="15"/>
-      <c r="AA72" s="6"/>
-      <c r="AB72" s="6"/>
-      <c r="AC72" s="6"/>
-      <c r="AD72" s="6"/>
+      <c r="W72" s="3"/>
+      <c r="Z72" s="6"/>
     </row>
     <row r="73" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B73" s="23" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="C73" s="14">
         <v>1</v>
       </c>
-      <c r="D73" s="14">
-        <v>0</v>
-      </c>
-      <c r="I73" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="L73" s="2">
-        <v>0</v>
-      </c>
-      <c r="M73" s="20">
-        <v>1</v>
-      </c>
-      <c r="N73" s="36">
-        <v>1</v>
-      </c>
+      <c r="I73" s="22"/>
+      <c r="K73" s="34"/>
+      <c r="L73" s="34"/>
+      <c r="M73" s="36"/>
       <c r="O73" s="36">
-        <v>1</v>
-      </c>
-      <c r="P73" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q73" s="36">
-        <v>1</v>
-      </c>
-      <c r="R73" s="36">
         <v>1</v>
       </c>
       <c r="S73" s="36">
@@ -5567,35 +5558,34 @@
       </c>
       <c r="T73" s="34"/>
       <c r="U73" s="77">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" ref="U73:U76" si="2">SUM(Q73:T73)</f>
+        <v>1</v>
       </c>
       <c r="V73" s="15"/>
-    </row>
-    <row r="74" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="10"/>
+      <c r="AA73" s="6"/>
+      <c r="AB73" s="6"/>
+      <c r="AC73" s="6"/>
+      <c r="AD73" s="6"/>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B74" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C74" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D74" s="14">
-        <v>1</v>
-      </c>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="22"/>
-      <c r="J74" s="36"/>
-      <c r="K74" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I74" s="22" t="s">
+        <v>91</v>
       </c>
       <c r="L74" s="2">
-        <v>1</v>
-      </c>
-      <c r="M74" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="M74" s="20">
+        <v>1</v>
+      </c>
       <c r="N74" s="36">
         <v>1</v>
       </c>
@@ -5620,131 +5610,146 @@
         <v>3</v>
       </c>
       <c r="V74" s="15"/>
-      <c r="W74" s="3"/>
-      <c r="X74"/>
-      <c r="Y74"/>
-      <c r="Z74"/>
-      <c r="AA74"/>
-      <c r="AB74"/>
-      <c r="AC74"/>
-      <c r="AD74"/>
-    </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B75" s="24" t="s">
+    </row>
+    <row r="75" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="10"/>
+      <c r="B75" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" s="14">
+        <v>3</v>
+      </c>
+      <c r="D75" s="14">
+        <v>1</v>
+      </c>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="36"/>
+      <c r="K75" s="2">
+        <v>1</v>
+      </c>
+      <c r="L75" s="2">
+        <v>1</v>
+      </c>
+      <c r="M75" s="20"/>
+      <c r="N75" s="36">
+        <v>1</v>
+      </c>
+      <c r="O75" s="36">
+        <v>1</v>
+      </c>
+      <c r="P75" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="36">
+        <v>1</v>
+      </c>
+      <c r="R75" s="36">
+        <v>1</v>
+      </c>
+      <c r="S75" s="36">
+        <v>1</v>
+      </c>
+      <c r="T75" s="34"/>
+      <c r="U75" s="77">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="V75" s="15"/>
+      <c r="W75" s="3"/>
+      <c r="X75"/>
+      <c r="Y75"/>
+      <c r="Z75"/>
+      <c r="AA75"/>
+      <c r="AB75"/>
+      <c r="AC75"/>
+      <c r="AD75"/>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B76" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="27">
+      <c r="C76" s="27">
         <v>4</v>
       </c>
-      <c r="D75" s="27">
+      <c r="D76" s="27">
         <v>0</v>
       </c>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="27"/>
-      <c r="I75" s="29"/>
-      <c r="J75" s="37"/>
-      <c r="K75" s="28">
-        <v>1</v>
-      </c>
-      <c r="L75" s="28">
+      <c r="E76" s="27"/>
+      <c r="F76" s="27"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="27"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="37"/>
+      <c r="K76" s="28">
+        <v>1</v>
+      </c>
+      <c r="L76" s="28">
         <v>0</v>
       </c>
-      <c r="M75" s="28"/>
-      <c r="N75" s="37"/>
-      <c r="O75" s="37"/>
-      <c r="P75" s="37">
-        <v>1</v>
-      </c>
-      <c r="Q75" s="37">
-        <v>1</v>
-      </c>
-      <c r="R75" s="37">
-        <v>1</v>
-      </c>
-      <c r="S75" s="37">
+      <c r="M76" s="28"/>
+      <c r="N76" s="37"/>
+      <c r="O76" s="37"/>
+      <c r="P76" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="37">
+        <v>1</v>
+      </c>
+      <c r="R76" s="37">
+        <v>1</v>
+      </c>
+      <c r="S76" s="37">
         <v>0</v>
       </c>
-      <c r="T75" s="37"/>
-      <c r="U75" s="79">
+      <c r="T76" s="37"/>
+      <c r="U76" s="79">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="V75" s="15"/>
-    </row>
-    <row r="76" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="11"/>
       <c r="V76" s="15"/>
-      <c r="Y76" s="33"/>
-    </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I77" s="64" t="s">
+    </row>
+    <row r="77" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="11"/>
+      <c r="V77" s="15"/>
+      <c r="Y77" s="33"/>
+    </row>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I78" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="J77" s="85"/>
-      <c r="K77" s="65"/>
-      <c r="L77" s="65"/>
-      <c r="M77" s="65"/>
-      <c r="N77" s="65"/>
-      <c r="O77" s="65"/>
-      <c r="P77" s="65"/>
-      <c r="Q77" s="65">
-        <f t="array" ref="Q77">SUM($C2:$C75*(Q2:Q75&gt;=0.9)*($U2:$U75&gt;=$W$12))</f>
+      <c r="J78" s="85"/>
+      <c r="K78" s="65"/>
+      <c r="L78" s="65"/>
+      <c r="M78" s="65"/>
+      <c r="N78" s="65"/>
+      <c r="O78" s="65"/>
+      <c r="P78" s="65"/>
+      <c r="Q78" s="65">
+        <f t="array" ref="Q78">SUM($C2:$C76*(Q2:Q76&gt;=0.9)*($U2:$U76&gt;=$W$12))</f>
         <v>185</v>
       </c>
-      <c r="R77" s="65">
-        <f t="array" ref="R77">SUM($C2:$C75*(R2:R75&gt;=0.9)*($U2:$U75&gt;=$W$12))</f>
+      <c r="R78" s="65">
+        <f t="array" ref="R78">SUM($C2:$C76*(R2:R76&gt;=0.9)*($U2:$U76&gt;=$W$12))</f>
         <v>193</v>
       </c>
-      <c r="S77" s="65">
-        <f t="array" ref="S77">SUM($C2:$C75*(S2:S75&gt;=0.9)*($U2:$U75&gt;=$W$12))</f>
-        <v>204</v>
-      </c>
-      <c r="T77" s="66"/>
-      <c r="V77" s="15"/>
-      <c r="AA77" s="6"/>
-      <c r="AB77" s="6"/>
-      <c r="AC77" s="6"/>
-      <c r="AD77" s="6"/>
-    </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I78" s="67" t="s">
+      <c r="S78" s="65">
+        <f t="array" ref="S78">SUM($C2:$C76*(S2:S76&gt;=0.9)*($U2:$U76&gt;=$W$12))</f>
+        <v>207</v>
+      </c>
+      <c r="T78" s="66"/>
+      <c r="V78" s="15"/>
+      <c r="AA78" s="6"/>
+      <c r="AB78" s="6"/>
+      <c r="AC78" s="6"/>
+      <c r="AD78" s="6"/>
+    </row>
+    <row r="79" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I79" s="67" t="s">
         <v>100</v>
-      </c>
-      <c r="J78" s="86"/>
-      <c r="K78" s="68"/>
-      <c r="L78" s="68"/>
-      <c r="M78" s="68"/>
-      <c r="N78" s="68"/>
-      <c r="O78" s="68"/>
-      <c r="P78" s="68"/>
-      <c r="Q78" s="68">
-        <f t="array" ref="Q78">SUM($C2:$C75*Q2:Q75*($U2:$U75&gt;=$W$12))</f>
-        <v>192</v>
-      </c>
-      <c r="R78" s="68">
-        <f t="array" ref="R78">SUM($C2:$C75*R2:R75*($U2:$U75&gt;=$W$12))</f>
-        <v>212.6</v>
-      </c>
-      <c r="S78" s="68">
-        <f t="array" ref="S78">SUM($C2:$C75*S2:S75*($U2:$U75&gt;=$W$12))</f>
-        <v>217.23</v>
-      </c>
-      <c r="T78" s="69"/>
-      <c r="V78" s="15"/>
-    </row>
-    <row r="79" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="10"/>
-      <c r="B79" s="23"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="67" t="s">
-        <v>99</v>
       </c>
       <c r="J79" s="86"/>
       <c r="K79" s="68"/>
@@ -5754,32 +5759,31 @@
       <c r="O79" s="68"/>
       <c r="P79" s="68"/>
       <c r="Q79" s="68">
-        <f t="array" ref="Q79">SUM($C$2:$C$75*(Q$2:Q$75&gt;=0.1)*($U$2:$U$75&gt;=$W$12))</f>
-        <v>199</v>
+        <f t="array" ref="Q79">SUM($C2:$C76*Q2:Q76*($U2:$U76&gt;=$W$12))</f>
+        <v>192</v>
       </c>
       <c r="R79" s="68">
-        <f t="array" ref="R79">SUM($C$2:$C$75*(R$2:R$75&gt;=0.1)*($U$2:$U$75&gt;=$W$12))</f>
-        <v>222</v>
+        <f t="array" ref="R79">SUM($C2:$C76*R2:R76*($U2:$U76&gt;=$W$12))</f>
+        <v>212.6</v>
       </c>
       <c r="S79" s="68">
-        <f t="array" ref="S79">SUM($C$2:$C$75*(S$2:S$75&gt;=0.1)*($U$2:$U$75&gt;=$W$12))</f>
-        <v>227</v>
+        <f t="array" ref="S79">SUM($C2:$C76*S2:S76*($U2:$U76&gt;=$W$12))</f>
+        <v>220.23</v>
       </c>
       <c r="T79" s="69"/>
-      <c r="U79" s="3"/>
       <c r="V79" s="15"/>
-      <c r="W79" s="3"/>
-      <c r="X79"/>
-      <c r="Y79"/>
-      <c r="Z79"/>
-      <c r="AA79"/>
-      <c r="AB79"/>
-      <c r="AC79"/>
-      <c r="AD79"/>
-    </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="10"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
       <c r="I80" s="67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J80" s="86"/>
       <c r="K80" s="68"/>
@@ -5789,92 +5793,118 @@
       <c r="O80" s="68"/>
       <c r="P80" s="68"/>
       <c r="Q80" s="68">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>246</v>
+        <f t="array" ref="Q80">SUM($C$2:$C$76*(Q$2:Q$76&gt;=0.1)*($U$2:$U$76&gt;=$W$12))</f>
+        <v>199</v>
       </c>
       <c r="R80" s="68">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>246</v>
+        <f t="array" ref="R80">SUM($C$2:$C$76*(R$2:R$76&gt;=0.1)*($U$2:$U$76&gt;=$W$12))</f>
+        <v>222</v>
       </c>
       <c r="S80" s="68">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>246</v>
+        <f t="array" ref="S80">SUM($C$2:$C$76*(S$2:S$76&gt;=0.1)*($U$2:$U$76&gt;=$W$12))</f>
+        <v>230</v>
       </c>
       <c r="T80" s="69"/>
+      <c r="U80" s="3"/>
       <c r="V80" s="15"/>
-      <c r="AA80" s="6"/>
-      <c r="AB80" s="6"/>
-      <c r="AC80" s="6"/>
-      <c r="AD80" s="6"/>
+      <c r="W80" s="3"/>
+      <c r="X80"/>
+      <c r="Y80"/>
+      <c r="Z80"/>
+      <c r="AA80"/>
+      <c r="AB80"/>
+      <c r="AC80"/>
+      <c r="AD80"/>
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I81" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="J81" s="86"/>
+      <c r="K81" s="68"/>
+      <c r="L81" s="68"/>
+      <c r="M81" s="68"/>
+      <c r="N81" s="68"/>
+      <c r="O81" s="68"/>
+      <c r="P81" s="68"/>
+      <c r="Q81" s="68">
+        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>249</v>
+      </c>
+      <c r="R81" s="68">
+        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>249</v>
+      </c>
+      <c r="S81" s="68">
+        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>249</v>
+      </c>
+      <c r="T81" s="69"/>
+      <c r="V81" s="15"/>
+      <c r="AA81" s="6"/>
+      <c r="AB81" s="6"/>
+      <c r="AC81" s="6"/>
+      <c r="AD81" s="6"/>
+    </row>
+    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I82" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="J81" s="86"/>
-      <c r="K81" s="70"/>
-      <c r="L81" s="70"/>
-      <c r="M81" s="70"/>
-      <c r="N81" s="70"/>
-      <c r="O81" s="70"/>
-      <c r="P81" s="70"/>
-      <c r="Q81" s="70">
-        <f t="shared" ref="Q81:S81" si="3">Q78/Q80</f>
-        <v>0.78048780487804881</v>
-      </c>
-      <c r="R81" s="70">
+      <c r="J82" s="86"/>
+      <c r="K82" s="70"/>
+      <c r="L82" s="70"/>
+      <c r="M82" s="70"/>
+      <c r="N82" s="70"/>
+      <c r="O82" s="70"/>
+      <c r="P82" s="70"/>
+      <c r="Q82" s="70">
+        <f t="shared" ref="Q82:S82" si="3">Q79/Q81</f>
+        <v>0.77108433734939763</v>
+      </c>
+      <c r="R82" s="70">
         <f t="shared" si="3"/>
-        <v>0.86422764227642279</v>
-      </c>
-      <c r="S81" s="70">
+        <v>0.85381526104417671</v>
+      </c>
+      <c r="S82" s="70">
         <f t="shared" si="3"/>
-        <v>0.88304878048780489</v>
-      </c>
-      <c r="T81" s="71"/>
-      <c r="V81" s="15"/>
-    </row>
-    <row r="82" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C82" s="33"/>
-      <c r="I82" s="72" t="s">
+        <v>0.8844578313253012</v>
+      </c>
+      <c r="T82" s="71"/>
+      <c r="V82" s="15"/>
+    </row>
+    <row r="83" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C83" s="33"/>
+      <c r="I83" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="J82" s="87"/>
-      <c r="K82" s="73"/>
-      <c r="L82" s="73"/>
-      <c r="M82" s="73"/>
-      <c r="N82" s="73"/>
-      <c r="O82" s="73"/>
-      <c r="P82" s="73"/>
-      <c r="Q82" s="73">
-        <f t="shared" ref="Q82:S82" si="4">Q80-Q78</f>
-        <v>54</v>
-      </c>
-      <c r="R82" s="73">
+      <c r="J83" s="87"/>
+      <c r="K83" s="73"/>
+      <c r="L83" s="73"/>
+      <c r="M83" s="73"/>
+      <c r="N83" s="73"/>
+      <c r="O83" s="73"/>
+      <c r="P83" s="73"/>
+      <c r="Q83" s="73">
+        <f t="shared" ref="Q83:S83" si="4">Q81-Q79</f>
+        <v>57</v>
+      </c>
+      <c r="R83" s="73">
         <f t="shared" si="4"/>
-        <v>33.400000000000006</v>
-      </c>
-      <c r="S82" s="73">
+        <v>36.400000000000006</v>
+      </c>
+      <c r="S83" s="73">
         <f t="shared" si="4"/>
         <v>28.77000000000001</v>
       </c>
-      <c r="T82" s="74"/>
-      <c r="V82" s="15"/>
-      <c r="AA82" s="6"/>
-      <c r="AB82" s="6"/>
-      <c r="AC82" s="6"/>
-      <c r="AD82" s="6"/>
-    </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="C83" s="33"/>
+      <c r="T83" s="74"/>
       <c r="V83" s="15"/>
+      <c r="AA83" s="6"/>
+      <c r="AB83" s="6"/>
+      <c r="AC83" s="6"/>
+      <c r="AD83" s="6"/>
     </row>
     <row r="84" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C84" s="33"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="14"/>
-      <c r="K84" s="14"/>
-      <c r="L84" s="14"/>
-      <c r="N84" s="14"/>
       <c r="V84" s="15"/>
     </row>
     <row r="85" spans="1:30" x14ac:dyDescent="0.3">
@@ -5887,6 +5917,7 @@
       <c r="V85" s="15"/>
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C86" s="33"/>
       <c r="I86" s="14"/>
       <c r="J86" s="14"/>
       <c r="K86" s="14"/>
@@ -5901,7 +5932,6 @@
       <c r="L87" s="14"/>
       <c r="N87" s="14"/>
       <c r="V87" s="15"/>
-      <c r="Z87" s="33"/>
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I88" s="14"/>
@@ -5910,6 +5940,7 @@
       <c r="L88" s="14"/>
       <c r="N88" s="14"/>
       <c r="V88" s="15"/>
+      <c r="Z88" s="33"/>
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I89" s="14"/>
@@ -5917,6 +5948,7 @@
       <c r="K89" s="14"/>
       <c r="L89" s="14"/>
       <c r="N89" s="14"/>
+      <c r="V89" s="15"/>
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I90" s="14"/>
@@ -5932,64 +5964,71 @@
       <c r="L91" s="14"/>
       <c r="N91" s="14"/>
     </row>
-    <row r="92" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="10"/>
-      <c r="B92" s="23"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="20"/>
-      <c r="J92" s="36"/>
-      <c r="K92" s="2"/>
-      <c r="L92" s="2"/>
-      <c r="M92" s="20"/>
-      <c r="N92" s="36"/>
-      <c r="O92" s="36"/>
-      <c r="P92" s="36"/>
-      <c r="Q92" s="36"/>
-      <c r="R92" s="36"/>
-      <c r="S92" s="36"/>
-      <c r="T92" s="2"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-      <c r="W92" s="3"/>
-      <c r="X92"/>
-      <c r="Y92"/>
-      <c r="Z92"/>
-      <c r="AA92"/>
-      <c r="AB92"/>
-      <c r="AC92"/>
-      <c r="AD92"/>
-    </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA95" s="6"/>
-      <c r="AB95" s="6"/>
-      <c r="AC95" s="6"/>
-      <c r="AD95" s="6"/>
-    </row>
-    <row r="99" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA99" s="6"/>
-      <c r="AB99" s="6"/>
-      <c r="AC99" s="6"/>
-      <c r="AD99" s="6"/>
-    </row>
-    <row r="104" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA104" s="6"/>
-      <c r="AB104" s="6"/>
-      <c r="AC104" s="6"/>
-      <c r="AD104" s="6"/>
-    </row>
-    <row r="117" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA117" s="33"/>
-      <c r="AB117" s="33"/>
-      <c r="AC117" s="33"/>
-      <c r="AD117" s="33"/>
+    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
+      <c r="L92" s="14"/>
+      <c r="N92" s="14"/>
+    </row>
+    <row r="93" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="10"/>
+      <c r="B93" s="23"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="20"/>
+      <c r="J93" s="36"/>
+      <c r="K93" s="2"/>
+      <c r="L93" s="2"/>
+      <c r="M93" s="20"/>
+      <c r="N93" s="36"/>
+      <c r="O93" s="36"/>
+      <c r="P93" s="36"/>
+      <c r="Q93" s="36"/>
+      <c r="R93" s="36"/>
+      <c r="S93" s="36"/>
+      <c r="T93" s="2"/>
+      <c r="U93" s="3"/>
+      <c r="V93" s="3"/>
+      <c r="W93" s="3"/>
+      <c r="X93"/>
+      <c r="Y93"/>
+      <c r="Z93"/>
+      <c r="AA93"/>
+      <c r="AB93"/>
+      <c r="AC93"/>
+      <c r="AD93"/>
+    </row>
+    <row r="96" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA96" s="6"/>
+      <c r="AB96" s="6"/>
+      <c r="AC96" s="6"/>
+      <c r="AD96" s="6"/>
+    </row>
+    <row r="100" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA100" s="6"/>
+      <c r="AB100" s="6"/>
+      <c r="AC100" s="6"/>
+      <c r="AD100" s="6"/>
+    </row>
+    <row r="105" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA105" s="6"/>
+      <c r="AB105" s="6"/>
+      <c r="AC105" s="6"/>
+      <c r="AD105" s="6"/>
+    </row>
+    <row r="118" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA118" s="33"/>
+      <c r="AB118" s="33"/>
+      <c r="AC118" s="33"/>
+      <c r="AD118" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U75">
+  <conditionalFormatting sqref="B2:U76">
     <cfRule type="expression" dxfId="2" priority="37" stopIfTrue="1">
       <formula>$U2&gt;=(0.5+$W$12)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update 131 lab list for 2020spring.xlsx
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
@@ -1,37 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\131\StudentGuideModule1\what_labs_to_include\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsubrama/Documents/Github/131/StudentGuideModule1/what_labs_to_include/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D94580-7BFB-CD42-882E-7FF97452CBAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="192" windowWidth="22980" windowHeight="9408" tabRatio="539"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="49100" windowHeight="26720" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Matt Trawick</author>
   </authors>
   <commentList>
-    <comment ref="W1" authorId="0" shapeId="0">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -40,25 +49,91 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-In the table on the left:
-Write "1" if you will use the lab.  
-Leave blank or write "0" if you will not use the lab.  
-Write "0.5" for maybe, or any other probability between 0 and 1 for "probably yes" or "probably no".</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">In the table on the left:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Write "1" if you will use the lab.  
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Leave blank or write "0" if you will not use the lab.  
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Write "0.5" for maybe, or any other probability between 0 and 1 for "probably yes" or "probably no".</t>
         </r>
       </text>
     </comment>
-    <comment ref="X11" authorId="0" shapeId="0">
+    <comment ref="Y11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -67,17 +142,45 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-In the past we have used 1.5 (one "yes", one "maybe") as the minimum number of votes needed to include a lab in the manual.  
-Remember, if a lab is not in the manual, it's VERY easy to generate a PDF file of a single lab to give your class.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">In the past we have used 1.5 (one "yes", one "maybe") as the minimum number of votes needed to include a lab in the manual.  
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Remember, if a lab is not in the manual, it's VERY easy to generate a PDF file of a single lab to give your class.</t>
         </r>
       </text>
     </comment>
-    <comment ref="Y19" authorId="0" shapeId="0">
+    <comment ref="Z19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -102,13 +205,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="W22" authorId="0" shapeId="0">
+    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -117,16 +220,25 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-This is kind of a "what if" table.  What if we set the cutoff at 2 people using a particular lab for whether to include that lab in the manual?  For each possible cutoff, this table shows how long the manual would be and how much it would cost.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is kind of a "what if" table.  What if we set the cutoff at 2 people using a particular lab for whether to include that lab in the manual?  For each possible cutoff, this table shows how long the manual would be and how much it would cost.</t>
         </r>
       </text>
     </comment>
-    <comment ref="X22" authorId="0" shapeId="0">
+    <comment ref="Y22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -150,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z22" authorId="0" shapeId="0">
+    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S61" authorId="0" shapeId="0">
+    <comment ref="R61" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -204,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="207">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -786,9 +898,6 @@
     <t>2019 fall Jerry</t>
   </si>
   <si>
-    <t>2019 fall Mariama</t>
-  </si>
-  <si>
     <t>2019 fall Matt</t>
   </si>
   <si>
@@ -826,16 +935,22 @@
   </si>
   <si>
     <t>added by Matt, 2019</t>
+  </si>
+  <si>
+    <t>2020 spr Mariama</t>
+  </si>
+  <si>
+    <t>2020 spr Barti</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -981,6 +1096,19 @@
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1457,7 +1585,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1638,8 +1766,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1829,6 +1955,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1864,6 +2007,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2039,34 +2199,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD121"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+      <selection activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.33203125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="14" customWidth="1"/>
-    <col min="4" max="8" width="5.88671875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="36" customWidth="1"/>
-    <col min="11" max="12" width="8.77734375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.77734375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="10.21875" style="36" customWidth="1"/>
-    <col min="15" max="19" width="8.77734375" style="36" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="11" style="3" customWidth="1"/>
-    <col min="22" max="22" width="2.44140625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="10.33203125" style="3" customWidth="1"/>
-    <col min="25" max="25" width="9.5546875" customWidth="1"/>
-    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="14" customWidth="1"/>
+    <col min="4" max="8" width="5.83203125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="28.5" style="20" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" style="36" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="20" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" style="36" customWidth="1"/>
+    <col min="15" max="20" width="8.83203125" style="36" customWidth="1"/>
+    <col min="21" max="21" width="8.83203125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="11" style="3" customWidth="1"/>
+    <col min="23" max="23" width="2.5" style="3" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" style="3" customWidth="1"/>
+    <col min="26" max="26" width="9.5" customWidth="1"/>
+    <col min="27" max="27" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="48" t="s">
         <v>73</v>
       </c>
@@ -2122,25 +2282,28 @@
         <v>192</v>
       </c>
       <c r="S1" s="49" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="T1" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="U1" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="V1" s="52" t="s">
         <v>184</v>
       </c>
-      <c r="V1" s="32"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="33"/>
       <c r="Y1" s="32"/>
       <c r="Z1" s="32"/>
-      <c r="AA1" s="33"/>
+      <c r="AA1" s="32"/>
       <c r="AB1" s="33"/>
       <c r="AC1" s="33"/>
       <c r="AD1" s="33"/>
-    </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE1" s="33"/>
+    </row>
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>86</v>
       </c>
@@ -2168,24 +2331,25 @@
       <c r="Q2" s="59"/>
       <c r="R2" s="59"/>
       <c r="S2" s="59"/>
-      <c r="T2" s="55">
+      <c r="T2" s="59"/>
+      <c r="U2" s="55">
         <v>3</v>
       </c>
-      <c r="U2" s="75">
-        <f>SUM(Q2:T2)</f>
+      <c r="V2" s="75">
+        <f>SUM(Q2:U2)</f>
         <v>3</v>
       </c>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80"/>
-      <c r="X2" s="80"/>
-      <c r="Y2" s="80"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="33"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="32"/>
       <c r="AB2" s="33"/>
       <c r="AC2" s="33"/>
       <c r="AD2" s="33"/>
-    </row>
-    <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE2" s="33"/>
+    </row>
+    <row r="3" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="48"/>
       <c r="B3" s="54" t="s">
         <v>88</v>
@@ -2211,24 +2375,25 @@
       <c r="Q3" s="60"/>
       <c r="R3" s="60"/>
       <c r="S3" s="60"/>
-      <c r="T3" s="60">
+      <c r="T3" s="60"/>
+      <c r="U3" s="60">
         <v>3</v>
       </c>
-      <c r="U3" s="76">
-        <f t="shared" ref="U3:U75" si="0">SUM(Q3:T3)</f>
+      <c r="V3" s="76">
+        <f>SUM(Q3:U3)</f>
         <v>3</v>
       </c>
-      <c r="V3" s="80"/>
-      <c r="W3" s="80"/>
-      <c r="X3" s="80"/>
-      <c r="Y3" s="80"/>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="33"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="78"/>
+      <c r="Z3" s="78"/>
+      <c r="AA3" s="32"/>
       <c r="AB3" s="33"/>
       <c r="AC3" s="33"/>
       <c r="AD3" s="33"/>
-    </row>
-    <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE3" s="33"/>
+    </row>
+    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>110</v>
       </c>
@@ -2269,27 +2434,30 @@
       <c r="P4" s="36"/>
       <c r="Q4" s="36"/>
       <c r="R4" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="S4" s="36">
         <v>0.5</v>
       </c>
-      <c r="S4" s="36">
-        <v>0.2</v>
-      </c>
-      <c r="T4" s="36"/>
-      <c r="U4" s="77">
-        <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="V4" s="5"/>
+      <c r="T4" s="36">
+        <v>0</v>
+      </c>
+      <c r="U4" s="36"/>
+      <c r="V4" s="77">
+        <f>SUM(S4:U4)</f>
+        <v>0.5</v>
+      </c>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="33"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="15"/>
       <c r="AB4" s="33"/>
       <c r="AC4" s="33"/>
       <c r="AD4" s="33"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE4" s="33"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
         <v>120</v>
       </c>
@@ -2303,25 +2471,28 @@
       <c r="L5" s="2">
         <v>0.75</v>
       </c>
-      <c r="S5" s="36">
-        <v>0</v>
-      </c>
-      <c r="T5" s="34"/>
-      <c r="U5" s="77">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V5" s="5"/>
+      <c r="R5" s="36">
+        <v>0</v>
+      </c>
+      <c r="T5" s="36">
+        <v>0</v>
+      </c>
+      <c r="U5" s="34"/>
+      <c r="V5" s="77">
+        <f t="shared" ref="V5:V68" si="0">SUM(S5:U5)</f>
+        <v>0</v>
+      </c>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="33"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="15"/>
       <c r="AB5" s="33"/>
       <c r="AC5" s="33"/>
       <c r="AD5" s="33"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE5" s="33"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
       <c r="B6" s="31" t="s">
         <v>121</v>
@@ -2335,25 +2506,28 @@
         <v>0</v>
       </c>
       <c r="M6" s="36"/>
-      <c r="S6" s="36">
-        <v>0</v>
-      </c>
-      <c r="T6" s="36"/>
-      <c r="U6" s="77">
+      <c r="R6" s="36">
+        <v>0</v>
+      </c>
+      <c r="T6" s="36">
+        <v>0</v>
+      </c>
+      <c r="U6" s="36"/>
+      <c r="V6" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V6" s="5"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="33"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="15"/>
       <c r="AB6" s="33"/>
       <c r="AC6" s="33"/>
       <c r="AD6" s="33"/>
-    </row>
-    <row r="7" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE6" s="33"/>
+    </row>
+    <row r="7" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="23" t="s">
         <v>122</v>
@@ -2377,22 +2551,25 @@
       <c r="O7" s="36"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="36">
-        <v>0</v>
-      </c>
-      <c r="T7" s="34"/>
-      <c r="U7" s="77">
+      <c r="R7" s="36">
+        <v>0</v>
+      </c>
+      <c r="S7" s="36"/>
+      <c r="T7" s="36">
+        <v>0</v>
+      </c>
+      <c r="U7" s="34"/>
+      <c r="V7" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
-      <c r="Z7" s="15"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="15"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B8" s="23" t="s">
         <v>123</v>
       </c>
@@ -2403,25 +2580,28 @@
       <c r="L8" s="2">
         <v>0</v>
       </c>
-      <c r="S8" s="36">
-        <v>0</v>
-      </c>
-      <c r="T8" s="34"/>
-      <c r="U8" s="77">
+      <c r="R8" s="36">
+        <v>0</v>
+      </c>
+      <c r="T8" s="36">
+        <v>0</v>
+      </c>
+      <c r="U8" s="34"/>
+      <c r="V8" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V8" s="5"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="33"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="15"/>
       <c r="AB8" s="33"/>
       <c r="AC8" s="33"/>
       <c r="AD8" s="33"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE8" s="33"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B9" s="23" t="s">
         <v>124</v>
       </c>
@@ -2468,22 +2648,25 @@
       <c r="S9" s="36">
         <v>1</v>
       </c>
-      <c r="T9" s="34"/>
-      <c r="U9" s="77">
+      <c r="T9" s="36">
+        <v>1</v>
+      </c>
+      <c r="U9" s="34"/>
+      <c r="V9" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V9" s="5"/>
+        <v>2</v>
+      </c>
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="33"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="15"/>
       <c r="AB9" s="33"/>
       <c r="AC9" s="33"/>
       <c r="AD9" s="33"/>
-    </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE9" s="33"/>
+    </row>
+    <row r="10" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>125</v>
       </c>
@@ -2530,22 +2713,25 @@
       <c r="S10" s="36">
         <v>1</v>
       </c>
-      <c r="T10" s="34"/>
-      <c r="U10" s="77">
+      <c r="T10" s="36">
+        <v>1</v>
+      </c>
+      <c r="U10" s="34"/>
+      <c r="V10" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V10" s="5"/>
+        <v>2</v>
+      </c>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="33"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="15"/>
       <c r="AB10" s="33"/>
       <c r="AC10" s="33"/>
       <c r="AD10" s="33"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE10" s="33"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B11" s="23" t="s">
         <v>126</v>
       </c>
@@ -2589,24 +2775,27 @@
       <c r="S11" s="36">
         <v>1</v>
       </c>
-      <c r="T11" s="34"/>
-      <c r="U11" s="77">
+      <c r="T11" s="36">
+        <v>1</v>
+      </c>
+      <c r="U11" s="34"/>
+      <c r="V11" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V11" s="5"/>
-      <c r="W11" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="W11" s="5"/>
+      <c r="X11" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="33"/>
+      <c r="Y11" s="43"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="15"/>
       <c r="AB11" s="33"/>
       <c r="AC11" s="33"/>
       <c r="AD11" s="33"/>
-    </row>
-    <row r="12" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE11" s="33"/>
+    </row>
+    <row r="12" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>127</v>
       </c>
@@ -2619,27 +2808,30 @@
         <v>0</v>
       </c>
       <c r="M12" s="36"/>
-      <c r="S12" s="36">
-        <v>0</v>
-      </c>
-      <c r="T12" s="34"/>
-      <c r="U12" s="77">
+      <c r="R12" s="36">
+        <v>0</v>
+      </c>
+      <c r="T12" s="36">
+        <v>0</v>
+      </c>
+      <c r="U12" s="34"/>
+      <c r="V12" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V12" s="15"/>
-      <c r="W12" s="44">
-        <v>1</v>
-      </c>
-      <c r="X12" s="45"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="33"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="45"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="15"/>
       <c r="AB12" s="33"/>
       <c r="AC12" s="33"/>
       <c r="AD12" s="33"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE12" s="33"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
         <v>175</v>
       </c>
@@ -2680,22 +2872,25 @@
       <c r="S13" s="36">
         <v>1</v>
       </c>
-      <c r="T13" s="34"/>
-      <c r="U13" s="77">
+      <c r="T13" s="36">
+        <v>1</v>
+      </c>
+      <c r="U13" s="34"/>
+      <c r="V13" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="V13" s="5"/>
-      <c r="W13" s="33"/>
+      <c r="W13" s="5"/>
       <c r="X13" s="33"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="33"/>
+      <c r="Y13" s="33"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="15"/>
       <c r="AB13" s="33"/>
       <c r="AC13" s="33"/>
       <c r="AD13" s="33"/>
-    </row>
-    <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE13" s="33"/>
+    </row>
+    <row r="14" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>128</v>
       </c>
@@ -2739,23 +2934,26 @@
       <c r="S14" s="36">
         <v>1</v>
       </c>
-      <c r="T14" s="34"/>
-      <c r="U14" s="77">
+      <c r="T14" s="36">
+        <v>1</v>
+      </c>
+      <c r="U14" s="34"/>
+      <c r="V14" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V14" s="5"/>
-      <c r="W14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="W14" s="5"/>
+      <c r="X14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Y14" s="33"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="33"/>
+      <c r="Z14" s="33"/>
+      <c r="AA14" s="15"/>
       <c r="AB14" s="33"/>
       <c r="AC14" s="33"/>
       <c r="AD14" s="33"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE14" s="33"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>174</v>
       </c>
@@ -2772,31 +2970,34 @@
       </c>
       <c r="M15" s="36"/>
       <c r="R15" s="36">
+        <v>0</v>
+      </c>
+      <c r="S15" s="36">
         <v>0.5</v>
       </c>
-      <c r="S15" s="36">
-        <v>0</v>
-      </c>
-      <c r="T15" s="34"/>
-      <c r="U15" s="77">
+      <c r="T15" s="36">
+        <v>0</v>
+      </c>
+      <c r="U15" s="34"/>
+      <c r="V15" s="77">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="V15" s="5"/>
-      <c r="W15" s="17" t="s">
+      <c r="W15" s="5"/>
+      <c r="X15" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="X15" s="38"/>
-      <c r="Y15" s="16">
+      <c r="Y15" s="38"/>
+      <c r="Z15" s="16">
         <v>0.05</v>
       </c>
-      <c r="Z15" s="33"/>
       <c r="AA15" s="33"/>
       <c r="AB15" s="33"/>
       <c r="AC15" s="33"/>
       <c r="AD15" s="33"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE15" s="33"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
         <v>129</v>
       </c>
@@ -2813,31 +3014,34 @@
         <v>1</v>
       </c>
       <c r="R16" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="S16" s="36">
         <v>0.5</v>
       </c>
-      <c r="S16" s="36">
-        <v>0.01</v>
-      </c>
-      <c r="T16" s="34"/>
-      <c r="U16" s="77">
+      <c r="T16" s="36">
+        <v>0</v>
+      </c>
+      <c r="U16" s="34"/>
+      <c r="V16" s="77">
         <f t="shared" si="0"/>
-        <v>0.51</v>
-      </c>
-      <c r="V16" s="5"/>
-      <c r="W16" s="18" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="W16" s="5"/>
+      <c r="X16" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="8">
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="8">
         <v>0.3</v>
       </c>
-      <c r="Z16" s="33"/>
       <c r="AA16" s="33"/>
       <c r="AB16" s="33"/>
       <c r="AC16" s="33"/>
       <c r="AD16" s="33"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE16" s="33"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
         <v>130</v>
       </c>
@@ -2871,31 +3075,34 @@
         <v>1</v>
       </c>
       <c r="R17" s="36">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="S17" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="T17" s="34"/>
-      <c r="U17" s="77">
+        <v>1</v>
+      </c>
+      <c r="T17" s="36">
+        <v>0</v>
+      </c>
+      <c r="U17" s="34"/>
+      <c r="V17" s="77">
         <f t="shared" si="0"/>
-        <v>2.8</v>
-      </c>
-      <c r="V17" s="5"/>
-      <c r="W17" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="W17" s="5"/>
+      <c r="X17" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="8">
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="8">
         <v>3</v>
       </c>
-      <c r="Z17" s="33"/>
       <c r="AA17" s="33"/>
       <c r="AB17" s="33"/>
       <c r="AC17" s="33"/>
       <c r="AD17" s="33"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE17" s="33"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B18" s="23" t="s">
         <v>131</v>
       </c>
@@ -2937,31 +3144,34 @@
         <v>1</v>
       </c>
       <c r="R18" s="36">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="S18" s="36">
-        <v>0.01</v>
-      </c>
-      <c r="T18" s="34"/>
-      <c r="U18" s="77">
+        <v>1</v>
+      </c>
+      <c r="T18" s="36">
+        <v>1</v>
+      </c>
+      <c r="U18" s="34"/>
+      <c r="V18" s="77">
         <f t="shared" si="0"/>
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="V18" s="5"/>
-      <c r="W18" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="W18" s="5"/>
+      <c r="X18" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="X18" s="5"/>
-      <c r="Y18" s="39">
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="39">
         <v>0.25</v>
       </c>
-      <c r="Z18" s="33"/>
       <c r="AA18" s="33"/>
       <c r="AB18" s="33"/>
       <c r="AC18" s="33"/>
       <c r="AD18" s="33"/>
-    </row>
-    <row r="19" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE18" s="33"/>
+    </row>
+    <row r="19" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="23" t="s">
         <v>132</v>
       </c>
@@ -2974,29 +3184,32 @@
         <v>0</v>
       </c>
       <c r="M19" s="36"/>
-      <c r="S19" s="36">
-        <v>0</v>
-      </c>
-      <c r="T19" s="34"/>
-      <c r="U19" s="77">
+      <c r="R19" s="36">
+        <v>0</v>
+      </c>
+      <c r="T19" s="36">
+        <v>0</v>
+      </c>
+      <c r="U19" s="34"/>
+      <c r="V19" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V19" s="15"/>
-      <c r="W19" s="19" t="s">
+      <c r="W19" s="15"/>
+      <c r="X19" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="X19" s="40"/>
-      <c r="Y19" s="41">
+      <c r="Y19" s="40"/>
+      <c r="Z19" s="41">
         <v>0.05</v>
       </c>
-      <c r="Z19" s="33"/>
       <c r="AA19" s="33"/>
       <c r="AB19" s="33"/>
       <c r="AC19" s="33"/>
       <c r="AD19" s="33"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE19" s="33"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B20" s="23" t="s">
         <v>133</v>
       </c>
@@ -3009,22 +3222,25 @@
         <v>0</v>
       </c>
       <c r="M20" s="36"/>
-      <c r="S20" s="36">
+      <c r="R20" s="36">
         <v>0.5</v>
       </c>
-      <c r="T20" s="34"/>
-      <c r="U20" s="77">
+      <c r="T20" s="36">
+        <v>0</v>
+      </c>
+      <c r="U20" s="34"/>
+      <c r="V20" s="77">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="V20" s="15"/>
-      <c r="Z20" s="33"/>
+        <v>0</v>
+      </c>
+      <c r="W20" s="15"/>
       <c r="AA20" s="33"/>
       <c r="AB20" s="33"/>
       <c r="AC20" s="33"/>
       <c r="AD20" s="33"/>
-    </row>
-    <row r="21" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE20" s="33"/>
+    </row>
+    <row r="21" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
         <v>134</v>
       </c>
@@ -3037,25 +3253,28 @@
         <v>0</v>
       </c>
       <c r="M21" s="36"/>
-      <c r="S21" s="36">
-        <v>0</v>
-      </c>
-      <c r="T21" s="34"/>
-      <c r="U21" s="77">
+      <c r="R21" s="36">
+        <v>0</v>
+      </c>
+      <c r="T21" s="36">
+        <v>0</v>
+      </c>
+      <c r="U21" s="34"/>
+      <c r="V21" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V21" s="15"/>
       <c r="W21" s="15"/>
-      <c r="X21" s="6"/>
+      <c r="X21" s="15"/>
       <c r="Y21" s="6"/>
-      <c r="Z21" s="33"/>
+      <c r="Z21" s="6"/>
       <c r="AA21" s="33"/>
       <c r="AB21" s="33"/>
       <c r="AC21" s="33"/>
       <c r="AD21" s="33"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE21" s="33"/>
+    </row>
+    <row r="22" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="23" t="s">
         <v>135</v>
       </c>
@@ -3066,33 +3285,36 @@
       <c r="L22" s="2">
         <v>0</v>
       </c>
-      <c r="S22" s="36">
+      <c r="R22" s="36">
         <v>0.1</v>
       </c>
-      <c r="T22" s="34"/>
-      <c r="U22" s="77">
+      <c r="T22" s="36">
+        <v>0</v>
+      </c>
+      <c r="U22" s="34"/>
+      <c r="V22" s="77">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="V22" s="15"/>
-      <c r="W22" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="W22" s="15"/>
+      <c r="X22" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="X22" s="4" t="s">
+      <c r="Y22" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="Y22" s="4" t="s">
+      <c r="Z22" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="Z22" s="7" t="s">
+      <c r="AA22" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="AA22" s="33"/>
       <c r="AB22" s="33"/>
       <c r="AC22" s="33"/>
       <c r="AD22" s="33"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE22" s="33"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B23" s="23" t="s">
         <v>136</v>
       </c>
@@ -3103,36 +3325,39 @@
       <c r="L23" s="2">
         <v>0</v>
       </c>
-      <c r="S23" s="36">
-        <v>0</v>
-      </c>
-      <c r="T23" s="34"/>
-      <c r="U23" s="77">
+      <c r="R23" s="36">
+        <v>0</v>
+      </c>
+      <c r="T23" s="36">
+        <v>0</v>
+      </c>
+      <c r="U23" s="34"/>
+      <c r="V23" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V23" s="15"/>
-      <c r="W23" s="81">
-        <v>0</v>
-      </c>
-      <c r="X23" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W23,C$2:C$80)</f>
+      <c r="W23" s="15"/>
+      <c r="X23" s="79">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X23,C$2:C$80)</f>
         <v>327</v>
       </c>
-      <c r="Y23" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W23,D$2:D$80)</f>
+      <c r="Z23" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X23,D$2:D$80)</f>
         <v>11</v>
       </c>
-      <c r="Z23" s="8">
-        <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
+      <c r="AA23" s="8">
+        <f t="shared" ref="AA23:AA31" si="1">($Z$17 + $Z$15*Y23+$Z$16*Z23)*(1+Z$18+Z$19)</f>
         <v>29.445000000000004</v>
       </c>
-      <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
       <c r="AC23" s="33"/>
       <c r="AD23" s="33"/>
-    </row>
-    <row r="24" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE23" s="33"/>
+    </row>
+    <row r="24" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="23" t="s">
         <v>137</v>
@@ -3182,33 +3407,36 @@
       <c r="S24" s="36">
         <v>1</v>
       </c>
-      <c r="T24" s="34"/>
-      <c r="U24" s="77">
+      <c r="T24" s="36">
+        <v>1</v>
+      </c>
+      <c r="U24" s="34"/>
+      <c r="V24" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V24" s="15"/>
-      <c r="W24" s="81">
+        <v>2</v>
+      </c>
+      <c r="W24" s="15"/>
+      <c r="X24" s="79">
         <v>0.5</v>
       </c>
-      <c r="X24" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W24,C$2:C$80)</f>
-        <v>297</v>
-      </c>
       <c r="Y24" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W24,D$2:D$80)</f>
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X24,C$2:C$80)</f>
+        <v>277</v>
+      </c>
+      <c r="Z24" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X24,D$2:D$80)</f>
         <v>10</v>
       </c>
-      <c r="Z24" s="8">
+      <c r="AA24" s="8">
         <f t="shared" si="1"/>
-        <v>27.105000000000004</v>
-      </c>
-      <c r="AA24" s="33"/>
+        <v>25.805000000000003</v>
+      </c>
       <c r="AB24" s="33"/>
       <c r="AC24" s="33"/>
       <c r="AD24" s="33"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE24" s="33"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B25" s="23" t="s">
         <v>138</v>
       </c>
@@ -3237,38 +3465,41 @@
         <v>1</v>
       </c>
       <c r="R25" s="36">
+        <v>1</v>
+      </c>
+      <c r="S25" s="36">
         <v>0.75</v>
       </c>
-      <c r="S25" s="36">
-        <v>1</v>
-      </c>
-      <c r="T25" s="34"/>
-      <c r="U25" s="77">
+      <c r="T25" s="36">
+        <v>1</v>
+      </c>
+      <c r="U25" s="34"/>
+      <c r="V25" s="77">
         <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
-      <c r="V25" s="15"/>
-      <c r="W25" s="81">
-        <v>1</v>
-      </c>
-      <c r="X25" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W25,C$2:C$80)</f>
-        <v>257</v>
+      <c r="W25" s="15"/>
+      <c r="X25" s="79">
+        <v>1</v>
       </c>
       <c r="Y25" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W25,D$2:D$80)</f>
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X25,C$2:C$80)</f>
+        <v>260</v>
+      </c>
+      <c r="Z25" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X25,D$2:D$80)</f>
         <v>10</v>
       </c>
-      <c r="Z25" s="8">
+      <c r="AA25" s="8">
         <f t="shared" si="1"/>
-        <v>24.505000000000003</v>
-      </c>
-      <c r="AA25" s="33"/>
+        <v>24.7</v>
+      </c>
       <c r="AB25" s="33"/>
       <c r="AC25" s="33"/>
       <c r="AD25" s="33"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE25" s="33"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B26" s="23" t="s">
         <v>139</v>
       </c>
@@ -3307,38 +3538,41 @@
         <v>1</v>
       </c>
       <c r="R26" s="36">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="S26" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="T26" s="34"/>
-      <c r="U26" s="77">
+        <v>1</v>
+      </c>
+      <c r="T26" s="36">
+        <v>1</v>
+      </c>
+      <c r="U26" s="34"/>
+      <c r="V26" s="77">
         <f t="shared" si="0"/>
-        <v>2.1</v>
-      </c>
-      <c r="V26" s="15"/>
-      <c r="W26" s="82">
+        <v>2</v>
+      </c>
+      <c r="W26" s="15"/>
+      <c r="X26" s="80">
         <v>1.5</v>
       </c>
-      <c r="X26" s="31">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W26,C$2:C$80)</f>
-        <v>248</v>
-      </c>
       <c r="Y26" s="31">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W26,D$2:D$80)</f>
-        <v>10</v>
-      </c>
-      <c r="Z26" s="8">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X26,C$2:C$80)</f>
+        <v>221</v>
+      </c>
+      <c r="Z26" s="31">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X26,D$2:D$80)</f>
+        <v>9</v>
+      </c>
+      <c r="AA26" s="8">
         <f t="shared" si="1"/>
-        <v>23.919999999999998</v>
-      </c>
-      <c r="AA26" s="33"/>
+        <v>21.775000000000002</v>
+      </c>
       <c r="AB26" s="33"/>
       <c r="AC26" s="33"/>
       <c r="AD26" s="33"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE26" s="33"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>117</v>
       </c>
@@ -3390,29 +3624,32 @@
       <c r="S27" s="35">
         <v>1</v>
       </c>
-      <c r="T27" s="35"/>
-      <c r="U27" s="78">
+      <c r="T27" s="35">
+        <v>1</v>
+      </c>
+      <c r="U27" s="35"/>
+      <c r="V27" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V27" s="15"/>
-      <c r="W27" s="81">
         <v>2</v>
       </c>
-      <c r="X27" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W27,C$2:C$80)</f>
-        <v>229</v>
+      <c r="W27" s="15"/>
+      <c r="X27" s="79">
+        <v>2</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W27,D$2:D$80)</f>
-        <v>10</v>
-      </c>
-      <c r="Z27" s="8">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X27,C$2:C$80)</f>
+        <v>190</v>
+      </c>
+      <c r="Z27" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X27,D$2:D$80)</f>
+        <v>9</v>
+      </c>
+      <c r="AA27" s="8">
         <f t="shared" si="1"/>
-        <v>22.685000000000006</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+        <v>19.759999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B28" s="23" t="s">
         <v>141</v>
       </c>
@@ -3453,29 +3690,32 @@
       <c r="S28" s="36">
         <v>1</v>
       </c>
-      <c r="T28" s="34"/>
-      <c r="U28" s="77">
+      <c r="T28" s="36">
+        <v>1</v>
+      </c>
+      <c r="U28" s="34"/>
+      <c r="V28" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V28" s="15"/>
-      <c r="W28" s="81">
+        <v>2</v>
+      </c>
+      <c r="W28" s="15"/>
+      <c r="X28" s="79">
         <v>2.5</v>
       </c>
-      <c r="X28" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W28,C$2:C$80)</f>
-        <v>166</v>
-      </c>
       <c r="Y28" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W28,D$2:D$80)</f>
-        <v>10</v>
-      </c>
-      <c r="Z28" s="8">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X28,C$2:C$80)</f>
+        <v>8</v>
+      </c>
+      <c r="Z28" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X28,D$2:D$80)</f>
+        <v>1</v>
+      </c>
+      <c r="AA28" s="8">
         <f t="shared" si="1"/>
-        <v>18.59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B29" s="23" t="s">
         <v>142</v>
       </c>
@@ -3490,34 +3730,37 @@
         <v>0.7</v>
       </c>
       <c r="R29" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="S29" s="36">
         <v>0.75</v>
       </c>
-      <c r="S29" s="36">
-        <v>0.01</v>
-      </c>
-      <c r="T29" s="34"/>
-      <c r="U29" s="77">
+      <c r="T29" s="36">
+        <v>0.75</v>
+      </c>
+      <c r="U29" s="34"/>
+      <c r="V29" s="77">
         <f t="shared" si="0"/>
-        <v>0.76</v>
-      </c>
-      <c r="V29" s="15"/>
-      <c r="W29" s="81">
+        <v>1.5</v>
+      </c>
+      <c r="W29" s="15"/>
+      <c r="X29" s="79">
         <v>3</v>
       </c>
-      <c r="X29" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W29,C$2:C$80)</f>
-        <v>155</v>
-      </c>
       <c r="Y29" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W29,D$2:D$80)</f>
-        <v>9</v>
-      </c>
-      <c r="Z29" s="8">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X29,C$2:C$80)</f>
+        <v>8</v>
+      </c>
+      <c r="Z29" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X29,D$2:D$80)</f>
+        <v>1</v>
+      </c>
+      <c r="AA29" s="8">
         <f t="shared" si="1"/>
-        <v>17.484999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B30" s="23" t="s">
         <v>143</v>
       </c>
@@ -3551,74 +3794,80 @@
         <v>0.5</v>
       </c>
       <c r="R30" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="S30" s="36">
         <v>0.75</v>
       </c>
-      <c r="S30" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="T30" s="34"/>
-      <c r="U30" s="77">
+      <c r="T30" s="36">
+        <v>1</v>
+      </c>
+      <c r="U30" s="34"/>
+      <c r="V30" s="77">
         <f t="shared" si="0"/>
-        <v>2.15</v>
-      </c>
-      <c r="V30" s="15"/>
-      <c r="W30" s="81">
+        <v>1.75</v>
+      </c>
+      <c r="W30" s="15"/>
+      <c r="X30" s="79">
         <v>3.5</v>
       </c>
-      <c r="X30" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W30,C$2:C$80)</f>
-        <v>0</v>
-      </c>
       <c r="Y30" s="6">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W30,D$2:D$80)</f>
-        <v>0</v>
-      </c>
-      <c r="Z30" s="8">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X30,C$2:C$80)</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X30,D$2:D$80)</f>
+        <v>0</v>
+      </c>
+      <c r="AA30" s="8">
         <f t="shared" si="1"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C31" s="14">
         <v>2</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K31" s="34"/>
       <c r="L31" s="34"/>
       <c r="M31" s="36"/>
-      <c r="S31" s="36">
-        <v>1</v>
-      </c>
-      <c r="T31" s="34">
+      <c r="R31" s="36">
+        <v>1</v>
+      </c>
+      <c r="T31" s="36">
+        <v>1</v>
+      </c>
+      <c r="U31" s="34">
         <v>2</v>
       </c>
-      <c r="U31" s="77">
+      <c r="V31" s="77">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="V31" s="15"/>
-      <c r="W31" s="83">
+      <c r="W31" s="15"/>
+      <c r="X31" s="81">
         <v>4</v>
       </c>
-      <c r="X31" s="47">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W31,C$2:C$80)</f>
-        <v>0</v>
-      </c>
       <c r="Y31" s="47">
-        <f>SUMIF(U$2:U$80,"&gt;=" &amp; W31,D$2:D$80)</f>
-        <v>0</v>
-      </c>
-      <c r="Z31" s="9">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X31,C$2:C$80)</f>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="47">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X31,D$2:D$80)</f>
+        <v>0</v>
+      </c>
+      <c r="AA31" s="9">
         <f t="shared" si="1"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="23" t="s">
         <v>144</v>
@@ -3668,17 +3917,20 @@
       <c r="S32" s="36">
         <v>1</v>
       </c>
-      <c r="T32" s="34"/>
-      <c r="U32" s="77">
+      <c r="T32" s="36">
+        <v>1</v>
+      </c>
+      <c r="U32" s="34"/>
+      <c r="V32" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V32" s="15"/>
-      <c r="W32" s="3"/>
-      <c r="X32"/>
+        <v>2</v>
+      </c>
+      <c r="W32" s="15"/>
+      <c r="X32" s="3"/>
       <c r="Y32"/>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Z32"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B33" s="23" t="s">
         <v>145</v>
       </c>
@@ -3695,19 +3947,22 @@
         <v>1</v>
       </c>
       <c r="R33" s="36">
+        <v>0</v>
+      </c>
+      <c r="S33" s="36">
         <v>0.5</v>
       </c>
-      <c r="S33" s="36">
-        <v>0</v>
-      </c>
-      <c r="T33" s="34"/>
-      <c r="U33" s="77">
+      <c r="T33" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="U33" s="34"/>
+      <c r="V33" s="77">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="V33" s="15"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="W33" s="15"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B34" s="23" t="s">
         <v>146</v>
       </c>
@@ -3754,14 +4009,17 @@
       <c r="S34" s="36">
         <v>1</v>
       </c>
-      <c r="T34" s="34"/>
-      <c r="U34" s="77">
+      <c r="T34" s="36">
+        <v>1</v>
+      </c>
+      <c r="U34" s="34"/>
+      <c r="V34" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V34" s="15"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="W34" s="15"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B35" s="23" t="s">
         <v>147</v>
       </c>
@@ -3787,21 +4045,24 @@
       <c r="P35" s="36">
         <v>0.5</v>
       </c>
-      <c r="S35" s="36">
-        <v>1</v>
-      </c>
-      <c r="T35" s="34"/>
-      <c r="U35" s="77">
+      <c r="R35" s="36">
+        <v>1</v>
+      </c>
+      <c r="T35" s="36">
+        <v>0</v>
+      </c>
+      <c r="U35" s="34"/>
+      <c r="V35" s="77">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V35" s="15"/>
-      <c r="W35" s="84"/>
-    </row>
-    <row r="36" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="W35" s="15"/>
+      <c r="X35" s="82"/>
+    </row>
+    <row r="36" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C36" s="14">
         <v>3</v>
@@ -3812,7 +4073,7 @@
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
       <c r="I36" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J36" s="36"/>
       <c r="K36" s="34"/>
@@ -3822,21 +4083,22 @@
       <c r="O36" s="36"/>
       <c r="P36" s="36"/>
       <c r="Q36" s="36"/>
-      <c r="R36" s="36"/>
-      <c r="S36" s="36">
-        <v>1</v>
-      </c>
-      <c r="T36" s="34">
+      <c r="R36" s="36">
+        <v>1</v>
+      </c>
+      <c r="S36" s="36"/>
+      <c r="T36" s="36"/>
+      <c r="U36" s="34">
         <v>2</v>
       </c>
-      <c r="U36" s="77">
+      <c r="V36" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V36" s="15"/>
-      <c r="W36" s="84"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="W36" s="15"/>
+      <c r="X36" s="82"/>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B37" s="23" t="s">
         <v>148</v>
       </c>
@@ -3875,20 +4137,23 @@
         <v>1</v>
       </c>
       <c r="R37" s="36">
+        <v>0</v>
+      </c>
+      <c r="S37" s="36">
         <v>0.75</v>
       </c>
-      <c r="S37" s="36">
-        <v>0</v>
-      </c>
-      <c r="T37" s="34"/>
-      <c r="U37" s="77">
+      <c r="T37" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="U37" s="34"/>
+      <c r="V37" s="77">
         <f t="shared" si="0"/>
-        <v>1.75</v>
-      </c>
-      <c r="V37" s="15"/>
-      <c r="W37" s="84"/>
-    </row>
-    <row r="38" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1.25</v>
+      </c>
+      <c r="W37" s="15"/>
+      <c r="X37" s="82"/>
+    </row>
+    <row r="38" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="23" t="s">
         <v>149</v>
@@ -3936,15 +4201,18 @@
       <c r="S38" s="36">
         <v>1</v>
       </c>
-      <c r="T38" s="34"/>
-      <c r="U38" s="77">
+      <c r="T38" s="36">
+        <v>1</v>
+      </c>
+      <c r="U38" s="34"/>
+      <c r="V38" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V38" s="15"/>
-      <c r="W38" s="84"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="W38" s="15"/>
+      <c r="X38" s="82"/>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B39" s="23" t="s">
         <v>150</v>
       </c>
@@ -3975,21 +4243,24 @@
         <v>1</v>
       </c>
       <c r="R39" s="36">
+        <v>0</v>
+      </c>
+      <c r="S39" s="36">
         <v>0.5</v>
       </c>
-      <c r="S39" s="36">
-        <v>0</v>
-      </c>
-      <c r="T39" s="34"/>
-      <c r="U39" s="77">
+      <c r="T39" s="36">
+        <v>0</v>
+      </c>
+      <c r="U39" s="34"/>
+      <c r="V39" s="77">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="V39" s="15"/>
-      <c r="W39" s="84"/>
-      <c r="Z39" s="6"/>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W39" s="15"/>
+      <c r="X39" s="82"/>
+      <c r="AA39" s="6"/>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B40" s="23" t="s">
         <v>183</v>
       </c>
@@ -4002,17 +4273,20 @@
       <c r="P40" s="36">
         <v>1</v>
       </c>
-      <c r="S40" s="36">
-        <v>0</v>
-      </c>
-      <c r="T40" s="34"/>
-      <c r="U40" s="77">
+      <c r="R40" s="36">
+        <v>0</v>
+      </c>
+      <c r="T40" s="36">
+        <v>0</v>
+      </c>
+      <c r="U40" s="34"/>
+      <c r="V40" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V40" s="15"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W40" s="15"/>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>116</v>
       </c>
@@ -4066,16 +4340,19 @@
       <c r="S41" s="35">
         <v>1</v>
       </c>
-      <c r="T41" s="35"/>
-      <c r="U41" s="78">
+      <c r="T41" s="35">
+        <v>1</v>
+      </c>
+      <c r="U41" s="35"/>
+      <c r="V41" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V41" s="15"/>
+        <v>2</v>
+      </c>
       <c r="W41" s="15"/>
-      <c r="X41" s="6"/>
-    </row>
-    <row r="42" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X41" s="15"/>
+      <c r="Y41" s="6"/>
+    </row>
+    <row r="42" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="30"/>
       <c r="B42" s="31" t="s">
         <v>152</v>
@@ -4127,21 +4404,24 @@
       <c r="S42" s="36">
         <v>1</v>
       </c>
-      <c r="T42" s="36"/>
-      <c r="U42" s="77">
+      <c r="T42" s="36">
+        <v>1</v>
+      </c>
+      <c r="U42" s="36"/>
+      <c r="V42" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V42" s="15"/>
-      <c r="W42" s="3"/>
-      <c r="X42"/>
+        <v>2</v>
+      </c>
+      <c r="W42" s="15"/>
+      <c r="X42" s="3"/>
       <c r="Y42"/>
-      <c r="AA42"/>
+      <c r="Z42"/>
       <c r="AB42"/>
       <c r="AC42"/>
       <c r="AD42"/>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE42"/>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" s="30"/>
       <c r="B43" s="31" t="s">
         <v>153</v>
@@ -4189,18 +4469,21 @@
       <c r="S43" s="36">
         <v>1</v>
       </c>
-      <c r="T43" s="36"/>
-      <c r="U43" s="77">
+      <c r="T43" s="36">
+        <v>1</v>
+      </c>
+      <c r="U43" s="36"/>
+      <c r="V43" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V43" s="15"/>
-      <c r="AA43" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="W43" s="15"/>
       <c r="AB43" s="6"/>
       <c r="AC43" s="6"/>
       <c r="AD43" s="6"/>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE43" s="6"/>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
       <c r="B44" s="31" t="s">
         <v>154</v>
@@ -4223,18 +4506,21 @@
       <c r="Q44" s="36">
         <v>0.5</v>
       </c>
-      <c r="S44" s="36">
-        <v>0</v>
-      </c>
-      <c r="T44" s="36"/>
-      <c r="U44" s="77">
+      <c r="R44" s="36">
+        <v>0</v>
+      </c>
+      <c r="T44" s="36">
+        <v>0</v>
+      </c>
+      <c r="U44" s="36"/>
+      <c r="V44" s="77">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="V44" s="15"/>
-      <c r="Z44" s="6"/>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="W44" s="15"/>
+      <c r="AA44" s="6"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" s="30"/>
       <c r="B45" s="31" t="s">
         <v>155</v>
@@ -4279,16 +4565,19 @@
       <c r="S45" s="36">
         <v>1</v>
       </c>
-      <c r="T45" s="36"/>
-      <c r="U45" s="77">
+      <c r="T45" s="36">
+        <v>0</v>
+      </c>
+      <c r="U45" s="36"/>
+      <c r="V45" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V45" s="15"/>
+        <v>1</v>
+      </c>
       <c r="W45" s="15"/>
-      <c r="X45" s="6"/>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X45" s="15"/>
+      <c r="Y45" s="6"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" s="30"/>
       <c r="B46" s="31" t="s">
         <v>156</v>
@@ -4333,15 +4622,18 @@
       <c r="S46" s="36">
         <v>1</v>
       </c>
-      <c r="T46" s="36"/>
-      <c r="U46" s="77">
+      <c r="T46" s="36">
+        <v>1</v>
+      </c>
+      <c r="U46" s="36"/>
+      <c r="V46" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V46" s="15"/>
-      <c r="Y46" s="6"/>
-    </row>
-    <row r="47" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="W46" s="15"/>
+      <c r="Z46" s="6"/>
+    </row>
+    <row r="47" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
       <c r="B47" s="31" t="s">
         <v>157</v>
@@ -4389,22 +4681,25 @@
       <c r="S47" s="36">
         <v>1</v>
       </c>
-      <c r="T47" s="36"/>
-      <c r="U47" s="77">
+      <c r="T47" s="36">
+        <v>1</v>
+      </c>
+      <c r="U47" s="36"/>
+      <c r="V47" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V47" s="15"/>
-      <c r="W47" s="3"/>
-      <c r="X47"/>
+        <v>2</v>
+      </c>
+      <c r="W47" s="15"/>
+      <c r="X47" s="3"/>
       <c r="Y47"/>
       <c r="Z47"/>
       <c r="AA47"/>
       <c r="AB47"/>
       <c r="AC47"/>
       <c r="AD47"/>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE47"/>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" s="30"/>
       <c r="B48" s="31" t="s">
         <v>158</v>
@@ -4452,14 +4747,17 @@
       <c r="S48" s="36">
         <v>1</v>
       </c>
-      <c r="T48" s="36"/>
-      <c r="U48" s="77">
+      <c r="T48" s="36">
+        <v>1</v>
+      </c>
+      <c r="U48" s="36"/>
+      <c r="V48" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V48" s="15"/>
-    </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="W48" s="15"/>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" s="30"/>
       <c r="B49" s="31" t="s">
         <v>159</v>
@@ -4505,14 +4803,17 @@
       <c r="S49" s="36">
         <v>1</v>
       </c>
-      <c r="T49" s="36"/>
-      <c r="U49" s="77">
+      <c r="T49" s="36">
+        <v>1</v>
+      </c>
+      <c r="U49" s="36"/>
+      <c r="V49" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V49" s="15"/>
-    </row>
-    <row r="50" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="W49" s="15"/>
+    </row>
+    <row r="50" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="10"/>
       <c r="B50" s="23" t="s">
         <v>160</v>
@@ -4557,25 +4858,28 @@
         <v>0.5</v>
       </c>
       <c r="R50" s="36">
+        <v>1</v>
+      </c>
+      <c r="S50" s="36">
         <v>0.5</v>
       </c>
-      <c r="S50" s="36">
-        <v>1</v>
-      </c>
-      <c r="T50" s="34"/>
-      <c r="U50" s="77">
+      <c r="T50" s="36">
+        <v>1</v>
+      </c>
+      <c r="U50" s="34"/>
+      <c r="V50" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V50" s="15"/>
+        <v>1.5</v>
+      </c>
       <c r="W50" s="15"/>
-      <c r="Z50"/>
+      <c r="X50" s="15"/>
       <c r="AA50"/>
       <c r="AB50"/>
       <c r="AC50"/>
       <c r="AD50"/>
-    </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE50"/>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>115</v>
       </c>
@@ -4616,23 +4920,26 @@
       <c r="P51" s="35"/>
       <c r="Q51" s="35"/>
       <c r="R51" s="35">
+        <v>0</v>
+      </c>
+      <c r="S51" s="35">
         <v>0.5</v>
       </c>
-      <c r="S51" s="35">
-        <v>0</v>
-      </c>
-      <c r="T51" s="35"/>
-      <c r="U51" s="78">
+      <c r="T51" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="U51" s="35"/>
+      <c r="V51" s="77">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="V51" s="15"/>
-      <c r="AA51" s="33"/>
-      <c r="AB51" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="W51" s="15"/>
+      <c r="AB51" s="33"/>
       <c r="AC51" s="6"/>
       <c r="AD51" s="6"/>
-    </row>
-    <row r="52" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE51" s="6"/>
+    </row>
+    <row r="52" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="10"/>
       <c r="B52" s="23" t="s">
         <v>162</v>
@@ -4682,25 +4989,28 @@
       <c r="S52" s="36">
         <v>1</v>
       </c>
-      <c r="T52" s="34"/>
-      <c r="U52" s="77">
+      <c r="T52" s="36">
+        <v>1</v>
+      </c>
+      <c r="U52" s="34"/>
+      <c r="V52" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V52" s="15"/>
-      <c r="W52" s="3"/>
-      <c r="X52"/>
+        <v>2</v>
+      </c>
+      <c r="W52" s="15"/>
+      <c r="X52" s="3"/>
       <c r="Y52"/>
       <c r="Z52"/>
-      <c r="AA52" s="33"/>
-      <c r="AB52"/>
+      <c r="AA52"/>
+      <c r="AB52" s="33"/>
       <c r="AC52"/>
       <c r="AD52"/>
-    </row>
-    <row r="53" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE52"/>
+    </row>
+    <row r="53" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="10"/>
       <c r="B53" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C53" s="14">
         <v>2</v>
@@ -4711,7 +5021,7 @@
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
       <c r="I53" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J53" s="36"/>
       <c r="K53" s="34"/>
@@ -4721,54 +5031,55 @@
       <c r="O53" s="36"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="36"/>
-      <c r="R53" s="36"/>
-      <c r="S53" s="36">
-        <v>1</v>
-      </c>
-      <c r="T53" s="34">
+      <c r="R53" s="36">
+        <v>1</v>
+      </c>
+      <c r="S53" s="36"/>
+      <c r="T53" s="36"/>
+      <c r="U53" s="34">
         <v>2</v>
       </c>
-      <c r="U53" s="77">
+      <c r="V53" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V53" s="15"/>
-      <c r="W53" s="3"/>
-      <c r="X53" s="33"/>
+        <v>2</v>
+      </c>
+      <c r="W53" s="15"/>
+      <c r="X53" s="3"/>
       <c r="Y53" s="33"/>
       <c r="Z53" s="33"/>
       <c r="AA53" s="33"/>
       <c r="AB53" s="33"/>
       <c r="AC53" s="33"/>
       <c r="AD53" s="33"/>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE53" s="33"/>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B54" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C54" s="14">
+        <v>1</v>
+      </c>
+      <c r="I54" s="22" t="s">
         <v>194</v>
-      </c>
-      <c r="C54" s="14">
-        <v>1</v>
-      </c>
-      <c r="I54" s="22" t="s">
-        <v>195</v>
       </c>
       <c r="K54" s="34"/>
       <c r="L54" s="34"/>
       <c r="M54" s="36"/>
-      <c r="S54" s="36">
-        <v>1</v>
-      </c>
-      <c r="T54" s="34">
+      <c r="R54" s="36">
+        <v>1</v>
+      </c>
+      <c r="U54" s="34">
         <v>2</v>
       </c>
-      <c r="U54" s="77">
-        <f>SUM(Q54:T54)</f>
-        <v>3</v>
-      </c>
-      <c r="V54" s="15"/>
-      <c r="AA54" s="33"/>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="V54" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W54" s="15"/>
+      <c r="AB54" s="33"/>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B55" s="23" t="s">
         <v>163</v>
       </c>
@@ -4815,15 +5126,18 @@
       <c r="S55" s="36">
         <v>1</v>
       </c>
-      <c r="T55" s="34"/>
-      <c r="U55" s="77">
+      <c r="T55" s="36">
+        <v>1</v>
+      </c>
+      <c r="U55" s="34"/>
+      <c r="V55" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V55" s="15"/>
-      <c r="AA55" s="33"/>
-    </row>
-    <row r="56" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="W55" s="15"/>
+      <c r="AB55" s="33"/>
+    </row>
+    <row r="56" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="10"/>
       <c r="B56" s="23" t="s">
         <v>164</v>
@@ -4849,19 +5163,22 @@
       <c r="O56" s="36"/>
       <c r="P56" s="36"/>
       <c r="Q56" s="36"/>
-      <c r="R56" s="36"/>
-      <c r="S56" s="36">
+      <c r="R56" s="36">
         <v>0.5</v>
       </c>
-      <c r="T56" s="34"/>
-      <c r="U56" s="77">
+      <c r="S56" s="36"/>
+      <c r="T56" s="36">
+        <v>0</v>
+      </c>
+      <c r="U56" s="34"/>
+      <c r="V56" s="77">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="V56" s="15"/>
-      <c r="W56" s="3"/>
-    </row>
-    <row r="57" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="W56" s="15"/>
+      <c r="X56" s="3"/>
+    </row>
+    <row r="57" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="10"/>
       <c r="B57" s="23" t="s">
         <v>165</v>
@@ -4885,19 +5202,22 @@
       <c r="O57" s="36"/>
       <c r="P57" s="36"/>
       <c r="Q57" s="36"/>
-      <c r="R57" s="36"/>
-      <c r="S57" s="36">
-        <v>0</v>
-      </c>
-      <c r="T57" s="34"/>
-      <c r="U57" s="77">
+      <c r="R57" s="36">
+        <v>0</v>
+      </c>
+      <c r="S57" s="36"/>
+      <c r="T57" s="36">
+        <v>0</v>
+      </c>
+      <c r="U57" s="34"/>
+      <c r="V57" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V57" s="15"/>
-      <c r="W57" s="3"/>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W57" s="15"/>
+      <c r="X57" s="3"/>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B58" s="23" t="s">
         <v>186</v>
       </c>
@@ -4919,16 +5239,19 @@
       <c r="S58" s="36">
         <v>0.7</v>
       </c>
-      <c r="T58" s="34"/>
-      <c r="U58" s="77">
+      <c r="T58" s="36">
+        <v>1</v>
+      </c>
+      <c r="U58" s="34"/>
+      <c r="V58" s="77">
         <f t="shared" si="0"/>
-        <v>1.4</v>
-      </c>
-      <c r="V58" s="15"/>
-      <c r="Y58" s="6"/>
-      <c r="AA58" s="33"/>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+        <v>1.7</v>
+      </c>
+      <c r="W58" s="15"/>
+      <c r="Z58" s="6"/>
+      <c r="AB58" s="33"/>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B59" s="23" t="s">
         <v>166</v>
       </c>
@@ -4949,20 +5272,23 @@
         <v>1</v>
       </c>
       <c r="R59" s="36">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="S59" s="36">
-        <v>0.7</v>
-      </c>
-      <c r="T59" s="34"/>
-      <c r="U59" s="77">
+        <v>1</v>
+      </c>
+      <c r="T59" s="36">
+        <v>1</v>
+      </c>
+      <c r="U59" s="34"/>
+      <c r="V59" s="77">
         <f t="shared" si="0"/>
-        <v>1.7</v>
-      </c>
-      <c r="V59" s="15"/>
-      <c r="AA59" s="33"/>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="W59" s="15"/>
+      <c r="AB59" s="33"/>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B60" s="23" t="s">
         <v>167</v>
       </c>
@@ -5004,21 +5330,24 @@
         <v>1</v>
       </c>
       <c r="R60" s="36">
+        <v>1</v>
+      </c>
+      <c r="S60" s="36">
         <v>0.5</v>
       </c>
-      <c r="S60" s="36">
-        <v>1</v>
-      </c>
-      <c r="T60" s="34"/>
-      <c r="U60" s="77">
+      <c r="T60" s="36">
+        <v>1</v>
+      </c>
+      <c r="U60" s="34"/>
+      <c r="V60" s="77">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="V60" s="15"/>
-      <c r="Z60" s="6"/>
-      <c r="AA60" s="33"/>
-    </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+        <v>1.5</v>
+      </c>
+      <c r="W60" s="15"/>
+      <c r="AA60" s="6"/>
+      <c r="AB60" s="33"/>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>114</v>
       </c>
@@ -5059,20 +5388,23 @@
         <v>1</v>
       </c>
       <c r="R61" s="35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S61" s="35">
-        <v>0</v>
-      </c>
-      <c r="T61" s="35"/>
-      <c r="U61" s="78">
+        <v>1</v>
+      </c>
+      <c r="T61" s="35">
+        <v>1</v>
+      </c>
+      <c r="U61" s="35"/>
+      <c r="V61" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="V61" s="15"/>
-      <c r="AA61" s="33"/>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W61" s="15"/>
+      <c r="AB61" s="33"/>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B62" s="23" t="s">
         <v>169</v>
       </c>
@@ -5119,18 +5451,21 @@
       <c r="S62" s="36">
         <v>1</v>
       </c>
-      <c r="T62" s="34"/>
-      <c r="U62" s="77">
+      <c r="T62" s="36">
+        <v>1</v>
+      </c>
+      <c r="U62" s="34"/>
+      <c r="V62" s="77">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V62" s="15"/>
-      <c r="AA62" s="33"/>
-      <c r="AB62" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="W62" s="15"/>
+      <c r="AB62" s="33"/>
       <c r="AC62" s="6"/>
       <c r="AD62" s="6"/>
-    </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE62" s="6"/>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B63" s="23" t="s">
         <v>170</v>
       </c>
@@ -5169,23 +5504,26 @@
         <v>1</v>
       </c>
       <c r="R63" s="36">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="S63" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="T63" s="34"/>
-      <c r="U63" s="77">
+        <v>1</v>
+      </c>
+      <c r="T63" s="36">
+        <v>1</v>
+      </c>
+      <c r="U63" s="34"/>
+      <c r="V63" s="77">
         <f t="shared" si="0"/>
-        <v>1.9</v>
-      </c>
-      <c r="V63" s="15"/>
-      <c r="AA63" s="33"/>
-    </row>
-    <row r="64" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="W63" s="15"/>
+      <c r="AB63" s="33"/>
+    </row>
+    <row r="64" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="10"/>
       <c r="B64" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C64" s="14">
         <v>6</v>
@@ -5196,7 +5534,7 @@
       <c r="G64" s="14"/>
       <c r="H64" s="14"/>
       <c r="I64" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J64" s="36"/>
       <c r="K64" s="34"/>
@@ -5206,21 +5544,22 @@
       <c r="O64" s="36"/>
       <c r="P64" s="36"/>
       <c r="Q64" s="36"/>
-      <c r="R64" s="36"/>
-      <c r="S64" s="36">
-        <v>1</v>
-      </c>
-      <c r="T64" s="34">
-        <v>1</v>
-      </c>
-      <c r="U64" s="77">
+      <c r="R64" s="36">
+        <v>1</v>
+      </c>
+      <c r="S64" s="36"/>
+      <c r="T64" s="36"/>
+      <c r="U64" s="34">
+        <v>1</v>
+      </c>
+      <c r="V64" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V64" s="15"/>
-      <c r="W64" s="3"/>
-    </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="W64" s="15"/>
+      <c r="X64" s="3"/>
+    </row>
+    <row r="65" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B65" s="23" t="s">
         <v>171</v>
       </c>
@@ -5231,19 +5570,19 @@
       <c r="L65" s="2">
         <v>0</v>
       </c>
-      <c r="S65" s="36">
-        <v>0</v>
-      </c>
-      <c r="T65" s="34"/>
-      <c r="U65" s="77">
+      <c r="R65" s="36">
+        <v>0</v>
+      </c>
+      <c r="U65" s="34"/>
+      <c r="V65" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V65" s="15"/>
-      <c r="Z65" s="6"/>
-      <c r="AA65" s="33"/>
-    </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W65" s="15"/>
+      <c r="AA65" s="6"/>
+      <c r="AB65" s="33"/>
+    </row>
+    <row r="66" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>113</v>
       </c>
@@ -5277,22 +5616,23 @@
       <c r="Q66" s="35">
         <v>1</v>
       </c>
-      <c r="R66" s="35"/>
-      <c r="S66" s="35">
-        <v>1</v>
-      </c>
+      <c r="R66" s="35">
+        <v>1</v>
+      </c>
+      <c r="S66" s="35"/>
       <c r="T66" s="35"/>
-      <c r="U66" s="78">
+      <c r="U66" s="35"/>
+      <c r="V66" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V66" s="15"/>
-      <c r="AA66" s="33"/>
-    </row>
-    <row r="67" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="W66" s="15"/>
+      <c r="AB66" s="33"/>
+    </row>
+    <row r="67" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="30"/>
       <c r="B67" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C67" s="14">
         <v>3</v>
@@ -5303,7 +5643,7 @@
       <c r="G67" s="14"/>
       <c r="H67" s="14"/>
       <c r="I67" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J67" s="36"/>
       <c r="K67" s="36"/>
@@ -5313,24 +5653,25 @@
       <c r="O67" s="36"/>
       <c r="P67" s="36"/>
       <c r="Q67" s="36"/>
-      <c r="R67" s="36"/>
-      <c r="S67" s="36">
-        <v>1</v>
-      </c>
-      <c r="T67" s="36">
-        <v>1</v>
-      </c>
-      <c r="U67" s="77">
+      <c r="R67" s="36">
+        <v>1</v>
+      </c>
+      <c r="S67" s="36"/>
+      <c r="T67" s="36"/>
+      <c r="U67" s="36">
+        <v>1</v>
+      </c>
+      <c r="V67" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V67" s="15"/>
-      <c r="W67" s="3"/>
-    </row>
-    <row r="68" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="W67" s="15"/>
+      <c r="X67" s="3"/>
+    </row>
+    <row r="68" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="30"/>
       <c r="B68" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C68" s="14">
         <v>3</v>
@@ -5341,7 +5682,7 @@
       <c r="G68" s="14"/>
       <c r="H68" s="14"/>
       <c r="I68" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J68" s="36"/>
       <c r="K68" s="36"/>
@@ -5351,24 +5692,25 @@
       <c r="O68" s="36"/>
       <c r="P68" s="36"/>
       <c r="Q68" s="36"/>
-      <c r="R68" s="36"/>
-      <c r="S68" s="36">
-        <v>1</v>
-      </c>
-      <c r="T68" s="36">
-        <v>1</v>
-      </c>
-      <c r="U68" s="77">
+      <c r="R68" s="36">
+        <v>1</v>
+      </c>
+      <c r="S68" s="36"/>
+      <c r="T68" s="36"/>
+      <c r="U68" s="36">
+        <v>1</v>
+      </c>
+      <c r="V68" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V68" s="15"/>
-      <c r="W68" s="3"/>
-    </row>
-    <row r="69" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="W68" s="15"/>
+      <c r="X68" s="3"/>
+    </row>
+    <row r="69" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="30"/>
       <c r="B69" s="31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C69" s="14">
         <v>3</v>
@@ -5379,7 +5721,7 @@
       <c r="G69" s="14"/>
       <c r="H69" s="14"/>
       <c r="I69" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J69" s="36"/>
       <c r="K69" s="36"/>
@@ -5389,24 +5731,25 @@
       <c r="O69" s="36"/>
       <c r="P69" s="36"/>
       <c r="Q69" s="36"/>
-      <c r="R69" s="36"/>
-      <c r="S69" s="36">
-        <v>1</v>
-      </c>
-      <c r="T69" s="36">
-        <v>1</v>
-      </c>
-      <c r="U69" s="77">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V69" s="15"/>
-      <c r="W69" s="3"/>
-    </row>
-    <row r="70" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R69" s="36">
+        <v>1</v>
+      </c>
+      <c r="S69" s="36"/>
+      <c r="T69" s="36"/>
+      <c r="U69" s="36">
+        <v>1</v>
+      </c>
+      <c r="V69" s="77">
+        <f t="shared" ref="V69:V79" si="2">SUM(S69:U69)</f>
+        <v>1</v>
+      </c>
+      <c r="W69" s="15"/>
+      <c r="X69" s="3"/>
+    </row>
+    <row r="70" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="30"/>
       <c r="B70" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C70" s="14">
         <v>2</v>
@@ -5417,7 +5760,7 @@
       <c r="G70" s="14"/>
       <c r="H70" s="14"/>
       <c r="I70" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J70" s="36"/>
       <c r="K70" s="36"/>
@@ -5427,21 +5770,22 @@
       <c r="O70" s="36"/>
       <c r="P70" s="36"/>
       <c r="Q70" s="36"/>
-      <c r="R70" s="36"/>
-      <c r="S70" s="36">
+      <c r="R70" s="36">
         <v>0.9</v>
       </c>
-      <c r="T70" s="36">
-        <v>1</v>
-      </c>
-      <c r="U70" s="77">
-        <f t="shared" si="0"/>
-        <v>1.9</v>
-      </c>
-      <c r="V70" s="15"/>
-      <c r="W70" s="3"/>
-    </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="S70" s="36"/>
+      <c r="T70" s="36"/>
+      <c r="U70" s="36">
+        <v>1</v>
+      </c>
+      <c r="V70" s="77">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W70" s="15"/>
+      <c r="X70" s="3"/>
+    </row>
+    <row r="71" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B71" s="23" t="s">
         <v>173</v>
       </c>
@@ -5464,17 +5808,17 @@
       <c r="Q71" s="36">
         <v>1</v>
       </c>
-      <c r="S71" s="36">
-        <v>0</v>
-      </c>
-      <c r="T71" s="34"/>
-      <c r="U71" s="77">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V71" s="15"/>
-    </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="R71" s="36">
+        <v>0</v>
+      </c>
+      <c r="U71" s="34"/>
+      <c r="V71" s="77">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W71" s="15"/>
+    </row>
+    <row r="72" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
         <v>74</v>
       </c>
@@ -5513,19 +5857,22 @@
         <v>1</v>
       </c>
       <c r="R72" s="35">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="S72" s="35">
-        <v>0.9</v>
-      </c>
-      <c r="T72" s="35"/>
-      <c r="U72" s="78">
-        <f t="shared" si="0"/>
-        <v>2.9</v>
-      </c>
-      <c r="V72" s="15"/>
-    </row>
-    <row r="73" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="T72" s="35">
+        <v>1</v>
+      </c>
+      <c r="U72" s="35"/>
+      <c r="V72" s="77">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="W72" s="15"/>
+    </row>
+    <row r="73" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="30"/>
       <c r="B73" s="31" t="s">
         <v>82</v>
@@ -5565,22 +5912,25 @@
       <c r="S73" s="36">
         <v>1</v>
       </c>
-      <c r="T73" s="36"/>
-      <c r="U73" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V73" s="15"/>
-      <c r="W73" s="3"/>
-      <c r="X73"/>
+      <c r="T73" s="36">
+        <v>1</v>
+      </c>
+      <c r="U73" s="36"/>
+      <c r="V73" s="77">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="W73" s="15"/>
+      <c r="X73" s="3"/>
       <c r="Y73"/>
       <c r="Z73"/>
       <c r="AA73"/>
       <c r="AB73"/>
       <c r="AC73"/>
       <c r="AD73"/>
-    </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE73"/>
+    </row>
+    <row r="74" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B74" s="23" t="s">
         <v>93</v>
       </c>
@@ -5599,16 +5949,16 @@
       <c r="L74" s="2">
         <v>1</v>
       </c>
-      <c r="T74" s="34"/>
-      <c r="U74" s="77">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V74" s="15"/>
-      <c r="X74" s="33"/>
-      <c r="Z74" s="6"/>
-    </row>
-    <row r="75" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U74" s="34"/>
+      <c r="V74" s="77">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W74" s="15"/>
+      <c r="Y74" s="33"/>
+      <c r="AA74" s="6"/>
+    </row>
+    <row r="75" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="10"/>
       <c r="B75" s="23" t="s">
         <v>94</v>
@@ -5650,16 +6000,19 @@
       <c r="S75" s="36">
         <v>1</v>
       </c>
-      <c r="T75" s="34"/>
-      <c r="U75" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V75" s="15"/>
-      <c r="W75" s="3"/>
-      <c r="Z75" s="6"/>
-    </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="T75" s="36">
+        <v>1</v>
+      </c>
+      <c r="U75" s="34"/>
+      <c r="V75" s="77">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="W75" s="15"/>
+      <c r="X75" s="3"/>
+      <c r="AA75" s="6"/>
+    </row>
+    <row r="76" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B76" s="23" t="s">
         <v>180</v>
       </c>
@@ -5673,21 +6026,21 @@
       <c r="O76" s="36">
         <v>1</v>
       </c>
-      <c r="S76" s="36">
-        <v>1</v>
-      </c>
-      <c r="T76" s="34"/>
-      <c r="U76" s="77">
-        <f t="shared" ref="U76:U79" si="2">SUM(Q76:T76)</f>
-        <v>1</v>
-      </c>
-      <c r="V76" s="15"/>
-      <c r="AA76" s="6"/>
+      <c r="R76" s="36">
+        <v>1</v>
+      </c>
+      <c r="U76" s="34"/>
+      <c r="V76" s="77">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W76" s="15"/>
       <c r="AB76" s="6"/>
       <c r="AC76" s="6"/>
       <c r="AD76" s="6"/>
-    </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE76" s="6"/>
+    </row>
+    <row r="77" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B77" s="23" t="s">
         <v>95</v>
       </c>
@@ -5724,14 +6077,17 @@
       <c r="S77" s="36">
         <v>1</v>
       </c>
-      <c r="T77" s="34"/>
-      <c r="U77" s="77">
+      <c r="T77" s="36">
+        <v>1</v>
+      </c>
+      <c r="U77" s="34"/>
+      <c r="V77" s="77">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="V77" s="15"/>
-    </row>
-    <row r="78" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="W77" s="15"/>
+    </row>
+    <row r="78" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="10"/>
       <c r="B78" s="23" t="s">
         <v>96</v>
@@ -5773,22 +6129,25 @@
       <c r="S78" s="36">
         <v>1</v>
       </c>
-      <c r="T78" s="34"/>
-      <c r="U78" s="77">
+      <c r="T78" s="36">
+        <v>1</v>
+      </c>
+      <c r="U78" s="34"/>
+      <c r="V78" s="77">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="V78" s="15"/>
-      <c r="W78" s="3"/>
-      <c r="X78"/>
+        <v>2</v>
+      </c>
+      <c r="W78" s="15"/>
+      <c r="X78" s="3"/>
       <c r="Y78"/>
       <c r="Z78"/>
       <c r="AA78"/>
       <c r="AB78"/>
       <c r="AC78"/>
       <c r="AD78"/>
-    </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE78"/>
+    </row>
+    <row r="79" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B79" s="24" t="s">
         <v>97</v>
       </c>
@@ -5820,28 +6179,31 @@
         <v>1</v>
       </c>
       <c r="R79" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S79" s="37">
-        <v>0</v>
-      </c>
-      <c r="T79" s="37"/>
-      <c r="U79" s="79">
+        <v>1</v>
+      </c>
+      <c r="T79" s="37">
+        <v>1</v>
+      </c>
+      <c r="U79" s="37"/>
+      <c r="V79" s="77">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="V79" s="15"/>
-    </row>
-    <row r="80" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W79" s="15"/>
+    </row>
+    <row r="80" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
-      <c r="V80" s="15"/>
-      <c r="Y80" s="33"/>
-    </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W80" s="15"/>
+      <c r="Z80" s="33"/>
+    </row>
+    <row r="81" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I81" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="J81" s="85"/>
+      <c r="J81" s="83"/>
       <c r="K81" s="65"/>
       <c r="L81" s="65"/>
       <c r="M81" s="65"/>
@@ -5849,29 +6211,30 @@
       <c r="O81" s="65"/>
       <c r="P81" s="65"/>
       <c r="Q81" s="65">
-        <f t="array" ref="Q81">SUM($C2:$C79*(Q2:Q79&gt;=0.9)*($U2:$U79&gt;=$W$12))</f>
-        <v>179</v>
+        <f t="array" ref="Q81">SUM($C2:$C79*(Q2:Q79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
+        <v>172</v>
       </c>
       <c r="R81" s="65">
-        <f t="array" ref="R81">SUM($C2:$C79*(R2:R79&gt;=0.9)*($U2:$U79&gt;=$W$12))</f>
+        <f t="array" ref="R81">SUM($C2:$C79*(R2:R79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
+        <v>206</v>
+      </c>
+      <c r="S81" s="65">
+        <f t="array" ref="S81">SUM($C2:$C79*(S2:S79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
         <v>187</v>
       </c>
-      <c r="S81" s="65">
-        <f t="array" ref="S81">SUM($C2:$C79*(S2:S79&gt;=0.9)*($U2:$U79&gt;=$W$12))</f>
-        <v>213</v>
-      </c>
-      <c r="T81" s="66"/>
-      <c r="V81" s="15"/>
-      <c r="AA81" s="6"/>
+      <c r="T81" s="65"/>
+      <c r="U81" s="66"/>
+      <c r="W81" s="15"/>
       <c r="AB81" s="6"/>
       <c r="AC81" s="6"/>
       <c r="AD81" s="6"/>
-    </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE81" s="6"/>
+    </row>
+    <row r="82" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I82" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="J82" s="86"/>
+      <c r="J82" s="84"/>
       <c r="K82" s="68"/>
       <c r="L82" s="68"/>
       <c r="M82" s="68"/>
@@ -5879,21 +6242,22 @@
       <c r="O82" s="68"/>
       <c r="P82" s="68"/>
       <c r="Q82" s="68">
-        <f t="array" ref="Q82">SUM($C2:$C79*Q2:Q79*($U2:$U79&gt;=$W$12))</f>
-        <v>186</v>
+        <f t="array" ref="Q82">SUM($C2:$C79*Q2:Q79*($V2:$V79&gt;=$X$12))</f>
+        <v>179</v>
       </c>
       <c r="R82" s="68">
-        <f t="array" ref="R82">SUM($C2:$C79*R2:R79*($U2:$U79&gt;=$W$12))</f>
-        <v>206.6</v>
+        <f t="array" ref="R82">SUM($C2:$C79*R2:R79*($V2:$V79&gt;=$X$12))</f>
+        <v>216.3</v>
       </c>
       <c r="S82" s="68">
-        <f t="array" ref="S82">SUM($C2:$C79*S2:S79*($U2:$U79&gt;=$W$12))</f>
-        <v>223.23000000000002</v>
-      </c>
-      <c r="T82" s="69"/>
-      <c r="V82" s="15"/>
-    </row>
-    <row r="83" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="array" ref="S82">SUM($C2:$C79*S2:S79*($V2:$V79&gt;=$X$12))</f>
+        <v>214.85</v>
+      </c>
+      <c r="T82" s="68"/>
+      <c r="U82" s="69"/>
+      <c r="W82" s="15"/>
+    </row>
+    <row r="83" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="10"/>
       <c r="B83" s="23"/>
       <c r="C83" s="14"/>
@@ -5905,7 +6269,7 @@
       <c r="I83" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="J83" s="86"/>
+      <c r="J83" s="84"/>
       <c r="K83" s="68"/>
       <c r="L83" s="68"/>
       <c r="M83" s="68"/>
@@ -5913,34 +6277,35 @@
       <c r="O83" s="68"/>
       <c r="P83" s="68"/>
       <c r="Q83" s="68">
-        <f t="array" ref="Q83">SUM($C$2:$C$79*(Q$2:Q$79&gt;=0.1)*($U$2:$U$79&gt;=$W$12))</f>
-        <v>193</v>
+        <f t="array" ref="Q83">SUM($C$2:$C$79*(Q$2:Q$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
+        <v>186</v>
       </c>
       <c r="R83" s="68">
-        <f t="array" ref="R83">SUM($C$2:$C$79*(R$2:R$79&gt;=0.1)*($U$2:$U$79&gt;=$W$12))</f>
-        <v>216</v>
+        <f t="array" ref="R83">SUM($C$2:$C$79*(R$2:R$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
+        <v>227</v>
       </c>
       <c r="S83" s="68">
-        <f t="array" ref="S83">SUM($C$2:$C$79*(S$2:S$79&gt;=0.1)*($U$2:$U$79&gt;=$W$12))</f>
-        <v>234</v>
-      </c>
-      <c r="T83" s="69"/>
-      <c r="U83" s="3"/>
-      <c r="V83" s="15"/>
-      <c r="W83" s="3"/>
-      <c r="X83"/>
+        <f t="array" ref="S83">SUM($C$2:$C$79*(S$2:S$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
+        <v>229</v>
+      </c>
+      <c r="T83" s="68"/>
+      <c r="U83" s="69"/>
+      <c r="V83" s="3"/>
+      <c r="W83" s="15"/>
+      <c r="X83" s="3"/>
       <c r="Y83"/>
       <c r="Z83"/>
       <c r="AA83"/>
       <c r="AB83"/>
       <c r="AC83"/>
       <c r="AD83"/>
-    </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE83"/>
+    </row>
+    <row r="84" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I84" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="J84" s="86"/>
+      <c r="J84" s="84"/>
       <c r="K84" s="68"/>
       <c r="L84" s="68"/>
       <c r="M84" s="68"/>
@@ -5948,29 +6313,30 @@
       <c r="O84" s="68"/>
       <c r="P84" s="68"/>
       <c r="Q84" s="68">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>257</v>
+        <f>LOOKUP($X$12,$X23:$X31,$Y23:$Y31)</f>
+        <v>260</v>
       </c>
       <c r="R84" s="68">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>257</v>
+        <f>LOOKUP($X$12,$X23:$X31,$Y23:$Y31)</f>
+        <v>260</v>
       </c>
       <c r="S84" s="68">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>257</v>
-      </c>
-      <c r="T84" s="69"/>
-      <c r="V84" s="15"/>
-      <c r="AA84" s="6"/>
+        <f>LOOKUP($X$12,$X23:$X31,$Y23:$Y31)</f>
+        <v>260</v>
+      </c>
+      <c r="T84" s="68"/>
+      <c r="U84" s="69"/>
+      <c r="W84" s="15"/>
       <c r="AB84" s="6"/>
       <c r="AC84" s="6"/>
       <c r="AD84" s="6"/>
-    </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE84" s="6"/>
+    </row>
+    <row r="85" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I85" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="J85" s="86"/>
+      <c r="J85" s="84"/>
       <c r="K85" s="70"/>
       <c r="L85" s="70"/>
       <c r="M85" s="70"/>
@@ -5978,26 +6344,27 @@
       <c r="O85" s="70"/>
       <c r="P85" s="70"/>
       <c r="Q85" s="70">
-        <f t="shared" ref="Q85:S85" si="3">Q82/Q84</f>
-        <v>0.72373540856031127</v>
+        <f t="shared" ref="Q85:R85" si="3">Q82/Q84</f>
+        <v>0.68846153846153846</v>
       </c>
       <c r="R85" s="70">
         <f t="shared" si="3"/>
-        <v>0.80389105058365762</v>
+        <v>0.83192307692307699</v>
       </c>
       <c r="S85" s="70">
-        <f t="shared" si="3"/>
-        <v>0.86859922178988336</v>
-      </c>
-      <c r="T85" s="71"/>
-      <c r="V85" s="15"/>
-    </row>
-    <row r="86" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f>S82/S84</f>
+        <v>0.82634615384615384</v>
+      </c>
+      <c r="T85" s="70"/>
+      <c r="U85" s="71"/>
+      <c r="W85" s="15"/>
+    </row>
+    <row r="86" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C86" s="33"/>
       <c r="I86" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="J86" s="87"/>
+      <c r="J86" s="85"/>
       <c r="K86" s="73"/>
       <c r="L86" s="73"/>
       <c r="M86" s="73"/>
@@ -6005,93 +6372,94 @@
       <c r="O86" s="73"/>
       <c r="P86" s="73"/>
       <c r="Q86" s="73">
-        <f t="shared" ref="Q86:S86" si="4">Q84-Q82</f>
-        <v>71</v>
+        <f t="shared" ref="Q86:R86" si="4">Q84-Q82</f>
+        <v>81</v>
       </c>
       <c r="R86" s="73">
         <f t="shared" si="4"/>
-        <v>50.400000000000006</v>
+        <v>43.699999999999989</v>
       </c>
       <c r="S86" s="73">
-        <f t="shared" si="4"/>
-        <v>33.769999999999982</v>
-      </c>
-      <c r="T86" s="74"/>
-      <c r="V86" s="15"/>
-      <c r="AA86" s="6"/>
+        <f>S84-S82</f>
+        <v>45.150000000000006</v>
+      </c>
+      <c r="T86" s="73"/>
+      <c r="U86" s="74"/>
+      <c r="W86" s="15"/>
       <c r="AB86" s="6"/>
       <c r="AC86" s="6"/>
       <c r="AD86" s="6"/>
-    </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE86" s="6"/>
+    </row>
+    <row r="87" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C87" s="33"/>
-      <c r="V87" s="15"/>
-    </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W87" s="15"/>
+    </row>
+    <row r="88" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C88" s="33"/>
       <c r="I88" s="14"/>
       <c r="J88" s="14"/>
       <c r="K88" s="14"/>
       <c r="L88" s="14"/>
       <c r="N88" s="14"/>
-      <c r="V88" s="15"/>
-    </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W88" s="15"/>
+    </row>
+    <row r="89" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C89" s="33"/>
       <c r="I89" s="14"/>
       <c r="J89" s="14"/>
       <c r="K89" s="14"/>
       <c r="L89" s="14"/>
       <c r="N89" s="14"/>
-      <c r="V89" s="15"/>
-    </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W89" s="15"/>
+    </row>
+    <row r="90" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I90" s="14"/>
       <c r="J90" s="14"/>
       <c r="K90" s="14"/>
       <c r="L90" s="14"/>
       <c r="N90" s="14"/>
-      <c r="V90" s="15"/>
-    </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W90" s="15"/>
+    </row>
+    <row r="91" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I91" s="14"/>
       <c r="J91" s="14"/>
       <c r="K91" s="14"/>
       <c r="L91" s="14"/>
       <c r="N91" s="14"/>
-      <c r="V91" s="15"/>
-      <c r="Z91" s="33"/>
-    </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W91" s="15"/>
+      <c r="AA91" s="33"/>
+    </row>
+    <row r="92" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I92" s="14"/>
       <c r="J92" s="14"/>
       <c r="K92" s="14"/>
       <c r="L92" s="14"/>
       <c r="N92" s="14"/>
-      <c r="V92" s="15"/>
-    </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W92" s="15"/>
+    </row>
+    <row r="93" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I93" s="14"/>
       <c r="J93" s="14"/>
       <c r="K93" s="14"/>
       <c r="L93" s="14"/>
       <c r="N93" s="14"/>
     </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I94" s="14"/>
       <c r="J94" s="14"/>
       <c r="K94" s="14"/>
       <c r="L94" s="14"/>
       <c r="N94" s="14"/>
     </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I95" s="14"/>
       <c r="J95" s="14"/>
       <c r="K95" s="14"/>
       <c r="L95" s="14"/>
       <c r="N95" s="14"/>
     </row>
-    <row r="96" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="10"/>
       <c r="B96" s="23"/>
       <c r="C96" s="14"/>
@@ -6111,52 +6479,53 @@
       <c r="Q96" s="36"/>
       <c r="R96" s="36"/>
       <c r="S96" s="36"/>
-      <c r="T96" s="2"/>
-      <c r="U96" s="3"/>
+      <c r="T96" s="36"/>
+      <c r="U96" s="2"/>
       <c r="V96" s="3"/>
       <c r="W96" s="3"/>
-      <c r="X96"/>
+      <c r="X96" s="3"/>
       <c r="Y96"/>
       <c r="Z96"/>
       <c r="AA96"/>
       <c r="AB96"/>
       <c r="AC96"/>
       <c r="AD96"/>
-    </row>
-    <row r="99" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA99" s="6"/>
+      <c r="AE96"/>
+    </row>
+    <row r="99" spans="28:31" x14ac:dyDescent="0.2">
       <c r="AB99" s="6"/>
       <c r="AC99" s="6"/>
       <c r="AD99" s="6"/>
-    </row>
-    <row r="103" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA103" s="6"/>
+      <c r="AE99" s="6"/>
+    </row>
+    <row r="103" spans="28:31" x14ac:dyDescent="0.2">
       <c r="AB103" s="6"/>
       <c r="AC103" s="6"/>
       <c r="AD103" s="6"/>
-    </row>
-    <row r="108" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA108" s="6"/>
+      <c r="AE103" s="6"/>
+    </row>
+    <row r="108" spans="28:31" x14ac:dyDescent="0.2">
       <c r="AB108" s="6"/>
       <c r="AC108" s="6"/>
       <c r="AD108" s="6"/>
-    </row>
-    <row r="121" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA121" s="33"/>
+      <c r="AE108" s="6"/>
+    </row>
+    <row r="121" spans="28:31" x14ac:dyDescent="0.2">
       <c r="AB121" s="33"/>
       <c r="AC121" s="33"/>
       <c r="AD121" s="33"/>
+      <c r="AE121" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U79">
+  <conditionalFormatting sqref="B2:V79">
     <cfRule type="expression" dxfId="2" priority="37" stopIfTrue="1">
-      <formula>$U2&gt;=(0.5+$W$12)</formula>
+      <formula>$V2&gt;=(0.5+$X$12)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="38" stopIfTrue="1">
-      <formula>$U2&gt;=$W$12</formula>
+      <formula>$V2&gt;=$X$12</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="39">
-      <formula>$U2&gt;=($W$12-0.5)</formula>
+      <formula>$V2&gt;=($X$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6166,379 +6535,379 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A73"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
       <selection sqref="A1:A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
minor changes to spreadsheet for spring 2020
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2020spring.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsubrama/Documents/Github/131/StudentGuideModule1/what_labs_to_include/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\131\StudentGuideModule1\what_labs_to_include\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF7A6EB-FC51-AF41-BA9C-05689C34F770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9320" yWindow="460" windowWidth="49100" windowHeight="26720" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9324" yWindow="456" windowWidth="49104" windowHeight="26724" tabRatio="539"/>
   </bookViews>
   <sheets>
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,12 +28,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Matt Trawick</author>
   </authors>
   <commentList>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="Y11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -180,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="Z19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -205,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="X22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -238,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="Y22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -262,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="AA22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -287,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R61" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="R61" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -946,7 +945,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1955,23 +1954,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2007,23 +1989,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2199,34 +2164,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T57" sqref="T57"/>
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.33203125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="14" customWidth="1"/>
-    <col min="4" max="8" width="5.83203125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="28.5" style="20" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" style="36" customWidth="1"/>
-    <col min="11" max="12" width="8.83203125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="20" customWidth="1"/>
-    <col min="14" max="14" width="10.1640625" style="36" customWidth="1"/>
-    <col min="15" max="20" width="8.83203125" style="36" customWidth="1"/>
-    <col min="21" max="21" width="8.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="14" customWidth="1"/>
+    <col min="4" max="8" width="5.77734375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" style="36" customWidth="1"/>
+    <col min="11" max="12" width="8.77734375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" style="20" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" style="36" customWidth="1"/>
+    <col min="15" max="20" width="8.77734375" style="36" customWidth="1"/>
+    <col min="21" max="21" width="8.77734375" style="2" customWidth="1"/>
     <col min="22" max="22" width="11" style="3" customWidth="1"/>
-    <col min="23" max="23" width="2.5" style="3" customWidth="1"/>
+    <col min="23" max="23" width="2.44140625" style="3" customWidth="1"/>
     <col min="24" max="24" width="10.33203125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="9.5" customWidth="1"/>
-    <col min="27" max="27" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.44140625" customWidth="1"/>
+    <col min="27" max="27" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>73</v>
       </c>
@@ -2303,7 +2268,7 @@
       <c r="AD1" s="33"/>
       <c r="AE1" s="33"/>
     </row>
-    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>86</v>
       </c>
@@ -2349,7 +2314,7 @@
       <c r="AD2" s="33"/>
       <c r="AE2" s="33"/>
     </row>
-    <row r="3" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48"/>
       <c r="B3" s="54" t="s">
         <v>88</v>
@@ -2393,7 +2358,7 @@
       <c r="AD3" s="33"/>
       <c r="AE3" s="33"/>
     </row>
-    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>110</v>
       </c>
@@ -2457,7 +2422,7 @@
       <c r="AD4" s="33"/>
       <c r="AE4" s="33"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>120</v>
       </c>
@@ -2489,7 +2454,7 @@
       <c r="AD5" s="33"/>
       <c r="AE5" s="33"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="31" t="s">
         <v>121</v>
@@ -2521,7 +2486,7 @@
       <c r="AD6" s="33"/>
       <c r="AE6" s="33"/>
     </row>
-    <row r="7" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="23" t="s">
         <v>122</v>
@@ -2561,7 +2526,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="15"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>123</v>
       </c>
@@ -2590,7 +2555,7 @@
       <c r="AD8" s="33"/>
       <c r="AE8" s="33"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>124</v>
       </c>
@@ -2655,7 +2620,7 @@
       <c r="AD9" s="33"/>
       <c r="AE9" s="33"/>
     </row>
-    <row r="10" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
         <v>125</v>
       </c>
@@ -2720,7 +2685,7 @@
       <c r="AD10" s="33"/>
       <c r="AE10" s="33"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>126</v>
       </c>
@@ -2784,7 +2749,7 @@
       <c r="AD11" s="33"/>
       <c r="AE11" s="33"/>
     </row>
-    <row r="12" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
         <v>127</v>
       </c>
@@ -2817,7 +2782,7 @@
       <c r="AD12" s="33"/>
       <c r="AE12" s="33"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
         <v>175</v>
       </c>
@@ -2876,7 +2841,7 @@
       <c r="AD13" s="33"/>
       <c r="AE13" s="33"/>
     </row>
-    <row r="14" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
         <v>128</v>
       </c>
@@ -2939,7 +2904,7 @@
       <c r="AD14" s="33"/>
       <c r="AE14" s="33"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
         <v>174</v>
       </c>
@@ -2980,7 +2945,7 @@
       <c r="AD15" s="33"/>
       <c r="AE15" s="33"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
         <v>129</v>
       </c>
@@ -3021,7 +2986,7 @@
       <c r="AD16" s="33"/>
       <c r="AE16" s="33"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
         <v>130</v>
       </c>
@@ -3079,7 +3044,7 @@
       <c r="AD17" s="33"/>
       <c r="AE17" s="33"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
         <v>131</v>
       </c>
@@ -3148,7 +3113,7 @@
       <c r="AD18" s="33"/>
       <c r="AE18" s="33"/>
     </row>
-    <row r="19" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
         <v>132</v>
       </c>
@@ -3183,7 +3148,7 @@
       <c r="AD19" s="33"/>
       <c r="AE19" s="33"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
         <v>133</v>
       </c>
@@ -3211,7 +3176,7 @@
       <c r="AD20" s="33"/>
       <c r="AE20" s="33"/>
     </row>
-    <row r="21" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="23" t="s">
         <v>134</v>
       </c>
@@ -3242,7 +3207,7 @@
       <c r="AD21" s="33"/>
       <c r="AE21" s="33"/>
     </row>
-    <row r="22" spans="1:31" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
         <v>135</v>
       </c>
@@ -3279,7 +3244,7 @@
       <c r="AD22" s="33"/>
       <c r="AE22" s="33"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
         <v>136</v>
       </c>
@@ -3319,7 +3284,7 @@
       <c r="AD23" s="33"/>
       <c r="AE23" s="33"/>
     </row>
-    <row r="24" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="23" t="s">
         <v>137</v>
@@ -3383,7 +3348,7 @@
       </c>
       <c r="Y24" s="6">
         <f t="shared" si="1"/>
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="Z24" s="6">
         <f t="shared" si="2"/>
@@ -3391,14 +3356,14 @@
       </c>
       <c r="AA24" s="8">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>25.610000000000003</v>
       </c>
       <c r="AB24" s="33"/>
       <c r="AC24" s="33"/>
       <c r="AD24" s="33"/>
       <c r="AE24" s="33"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
         <v>138</v>
       </c>
@@ -3446,7 +3411,7 @@
       </c>
       <c r="Y25" s="6">
         <f t="shared" si="1"/>
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="Z25" s="6">
         <f t="shared" si="2"/>
@@ -3454,14 +3419,14 @@
       </c>
       <c r="AA25" s="8">
         <f t="shared" si="3"/>
-        <v>24.7</v>
+        <v>24.310000000000006</v>
       </c>
       <c r="AB25" s="33"/>
       <c r="AC25" s="33"/>
       <c r="AD25" s="33"/>
       <c r="AE25" s="33"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
         <v>139</v>
       </c>
@@ -3519,7 +3484,7 @@
       </c>
       <c r="Y26" s="31">
         <f t="shared" si="1"/>
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="Z26" s="31">
         <f t="shared" si="2"/>
@@ -3527,14 +3492,14 @@
       </c>
       <c r="AA26" s="8">
         <f t="shared" si="3"/>
-        <v>22.1</v>
+        <v>22.165000000000003</v>
       </c>
       <c r="AB26" s="33"/>
       <c r="AC26" s="33"/>
       <c r="AD26" s="33"/>
       <c r="AE26" s="33"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>117</v>
       </c>
@@ -3600,7 +3565,7 @@
       </c>
       <c r="Y27" s="6">
         <f t="shared" si="1"/>
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="Z27" s="6">
         <f t="shared" si="2"/>
@@ -3608,10 +3573,10 @@
       </c>
       <c r="AA27" s="8">
         <f t="shared" si="3"/>
-        <v>20.605</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+        <v>20.67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
         <v>141</v>
       </c>
@@ -3666,7 +3631,7 @@
       </c>
       <c r="Y28" s="6">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Z28" s="6">
         <f t="shared" si="2"/>
@@ -3674,10 +3639,10 @@
       </c>
       <c r="AA28" s="8">
         <f t="shared" si="3"/>
-        <v>4.8099999999999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+        <v>4.875</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
         <v>142</v>
       </c>
@@ -3711,7 +3676,7 @@
       </c>
       <c r="Y29" s="6">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z29" s="6">
         <f t="shared" si="2"/>
@@ -3719,10 +3684,10 @@
       </c>
       <c r="AA29" s="8">
         <f t="shared" si="3"/>
-        <v>4.8099999999999996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+        <v>4.7450000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
         <v>143</v>
       </c>
@@ -3775,7 +3740,7 @@
       </c>
       <c r="Y30" s="6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z30" s="6">
         <f t="shared" si="2"/>
@@ -3783,10 +3748,10 @@
       </c>
       <c r="AA30" s="8">
         <f t="shared" si="3"/>
-        <v>4.03</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3.9000000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="23" t="s">
         <v>195</v>
       </c>
@@ -3808,12 +3773,10 @@
       <c r="T31" s="36">
         <v>1</v>
       </c>
-      <c r="U31" s="34">
-        <v>2</v>
-      </c>
+      <c r="U31" s="34"/>
       <c r="V31" s="77">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W31" s="15"/>
       <c r="X31" s="81">
@@ -3821,7 +3784,7 @@
       </c>
       <c r="Y31" s="47">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z31" s="47">
         <f t="shared" si="2"/>
@@ -3829,10 +3792,10 @@
       </c>
       <c r="AA31" s="9">
         <f t="shared" si="3"/>
-        <v>4.03</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3.9000000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="23" t="s">
         <v>144</v>
@@ -3895,7 +3858,7 @@
       <c r="Y32"/>
       <c r="Z32"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="s">
         <v>145</v>
       </c>
@@ -3927,7 +3890,7 @@
       </c>
       <c r="W33" s="15"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B34" s="23" t="s">
         <v>146</v>
       </c>
@@ -3984,7 +3947,7 @@
       </c>
       <c r="W34" s="15"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="s">
         <v>147</v>
       </c>
@@ -4021,7 +3984,7 @@
       <c r="W35" s="15"/>
       <c r="X35" s="82"/>
     </row>
-    <row r="36" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="23" t="s">
         <v>198</v>
@@ -4060,7 +4023,7 @@
       <c r="W36" s="15"/>
       <c r="X36" s="82"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="s">
         <v>148</v>
       </c>
@@ -4115,7 +4078,7 @@
       <c r="W37" s="15"/>
       <c r="X37" s="82"/>
     </row>
-    <row r="38" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="23" t="s">
         <v>149</v>
@@ -4174,7 +4137,7 @@
       <c r="W38" s="15"/>
       <c r="X38" s="82"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B39" s="23" t="s">
         <v>150</v>
       </c>
@@ -4219,7 +4182,7 @@
       <c r="X39" s="82"/>
       <c r="AA39" s="6"/>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B40" s="23" t="s">
         <v>183</v>
       </c>
@@ -4242,7 +4205,7 @@
       </c>
       <c r="W40" s="15"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>116</v>
       </c>
@@ -4308,7 +4271,7 @@
       <c r="X41" s="15"/>
       <c r="Y41" s="6"/>
     </row>
-    <row r="42" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="30"/>
       <c r="B42" s="31" t="s">
         <v>152</v>
@@ -4377,7 +4340,7 @@
       <c r="AD42"/>
       <c r="AE42"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" s="30"/>
       <c r="B43" s="31" t="s">
         <v>153</v>
@@ -4439,7 +4402,7 @@
       <c r="AD43" s="6"/>
       <c r="AE43" s="6"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" s="30"/>
       <c r="B44" s="31" t="s">
         <v>154</v>
@@ -4473,7 +4436,7 @@
       <c r="W44" s="15"/>
       <c r="AA44" s="6"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" s="30"/>
       <c r="B45" s="31" t="s">
         <v>155</v>
@@ -4527,7 +4490,7 @@
       <c r="X45" s="15"/>
       <c r="Y45" s="6"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" s="30"/>
       <c r="B46" s="31" t="s">
         <v>156</v>
@@ -4583,7 +4546,7 @@
       <c r="W46" s="15"/>
       <c r="Z46" s="6"/>
     </row>
-    <row r="47" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30"/>
       <c r="B47" s="31" t="s">
         <v>157</v>
@@ -4649,7 +4612,7 @@
       <c r="AD47"/>
       <c r="AE47"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="30"/>
       <c r="B48" s="31" t="s">
         <v>158</v>
@@ -4707,7 +4670,7 @@
       </c>
       <c r="W48" s="15"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="30"/>
       <c r="B49" s="31" t="s">
         <v>159</v>
@@ -4763,7 +4726,7 @@
       </c>
       <c r="W49" s="15"/>
     </row>
-    <row r="50" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="23" t="s">
         <v>160</v>
@@ -4829,7 +4792,7 @@
       <c r="AD50"/>
       <c r="AE50"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>115</v>
       </c>
@@ -4889,7 +4852,7 @@
       <c r="AD51" s="6"/>
       <c r="AE51" s="6"/>
     </row>
-    <row r="52" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="23" t="s">
         <v>162</v>
@@ -4957,7 +4920,7 @@
       <c r="AD52"/>
       <c r="AE52"/>
     </row>
-    <row r="53" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10"/>
       <c r="B53" s="23" t="s">
         <v>197</v>
@@ -4985,13 +4948,15 @@
         <v>1</v>
       </c>
       <c r="S53" s="36"/>
-      <c r="T53" s="36"/>
+      <c r="T53" s="36">
+        <v>0.5</v>
+      </c>
       <c r="U53" s="34">
         <v>2</v>
       </c>
       <c r="V53" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="W53" s="15"/>
       <c r="X53" s="3"/>
@@ -5003,7 +4968,7 @@
       <c r="AD53" s="33"/>
       <c r="AE53" s="33"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B54" s="23" t="s">
         <v>193</v>
       </c>
@@ -5019,17 +4984,20 @@
       <c r="R54" s="36">
         <v>1</v>
       </c>
+      <c r="T54" s="36">
+        <v>1</v>
+      </c>
       <c r="U54" s="34">
         <v>2</v>
       </c>
       <c r="V54" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W54" s="15"/>
       <c r="AB54" s="33"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B55" s="23" t="s">
         <v>163</v>
       </c>
@@ -5087,7 +5055,7 @@
       <c r="W55" s="15"/>
       <c r="AB55" s="33"/>
     </row>
-    <row r="56" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10"/>
       <c r="B56" s="23" t="s">
         <v>164</v>
@@ -5128,7 +5096,7 @@
       <c r="W56" s="15"/>
       <c r="X56" s="3"/>
     </row>
-    <row r="57" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="10"/>
       <c r="B57" s="23" t="s">
         <v>165</v>
@@ -5165,7 +5133,7 @@
       <c r="W57" s="15"/>
       <c r="X57" s="3"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
         <v>186</v>
       </c>
@@ -5199,7 +5167,7 @@
       <c r="Z58" s="6"/>
       <c r="AB58" s="33"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B59" s="23" t="s">
         <v>166</v>
       </c>
@@ -5236,7 +5204,7 @@
       <c r="W59" s="15"/>
       <c r="AB59" s="33"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B60" s="23" t="s">
         <v>167</v>
       </c>
@@ -5295,7 +5263,7 @@
       <c r="AA60" s="6"/>
       <c r="AB60" s="33"/>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>114</v>
       </c>
@@ -5352,7 +5320,7 @@
       <c r="W61" s="15"/>
       <c r="AB61" s="33"/>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
         <v>169</v>
       </c>
@@ -5413,7 +5381,7 @@
       <c r="AD62" s="6"/>
       <c r="AE62" s="6"/>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B63" s="23" t="s">
         <v>170</v>
       </c>
@@ -5468,7 +5436,7 @@
       <c r="W63" s="15"/>
       <c r="AB63" s="33"/>
     </row>
-    <row r="64" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="10"/>
       <c r="B64" s="23" t="s">
         <v>199</v>
@@ -5496,18 +5464,20 @@
         <v>1</v>
       </c>
       <c r="S64" s="36"/>
-      <c r="T64" s="36"/>
+      <c r="T64" s="36">
+        <v>1</v>
+      </c>
       <c r="U64" s="34">
         <v>1</v>
       </c>
       <c r="V64" s="77">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W64" s="15"/>
       <c r="X64" s="3"/>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B65" s="23" t="s">
         <v>171</v>
       </c>
@@ -5530,7 +5500,7 @@
       <c r="AA65" s="6"/>
       <c r="AB65" s="33"/>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
         <v>113</v>
       </c>
@@ -5577,7 +5547,7 @@
       <c r="W66" s="15"/>
       <c r="AB66" s="33"/>
     </row>
-    <row r="67" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="30"/>
       <c r="B67" s="31" t="s">
         <v>200</v>
@@ -5608,17 +5578,15 @@
         <v>1</v>
       </c>
       <c r="T67" s="36"/>
-      <c r="U67" s="36">
-        <v>1</v>
-      </c>
+      <c r="U67" s="36"/>
       <c r="V67" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W67" s="15"/>
       <c r="X67" s="3"/>
     </row>
-    <row r="68" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="30"/>
       <c r="B68" s="31" t="s">
         <v>201</v>
@@ -5647,17 +5615,15 @@
       </c>
       <c r="S68" s="36"/>
       <c r="T68" s="36"/>
-      <c r="U68" s="36">
-        <v>1</v>
-      </c>
+      <c r="U68" s="36"/>
       <c r="V68" s="77">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W68" s="15"/>
       <c r="X68" s="3"/>
     </row>
-    <row r="69" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="30"/>
       <c r="B69" s="31" t="s">
         <v>202</v>
@@ -5686,17 +5652,15 @@
       </c>
       <c r="S69" s="36"/>
       <c r="T69" s="36"/>
-      <c r="U69" s="36">
-        <v>1</v>
-      </c>
+      <c r="U69" s="36"/>
       <c r="V69" s="77">
         <f t="shared" ref="V69:V79" si="4">SUM(S69:U69)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W69" s="15"/>
       <c r="X69" s="3"/>
     </row>
-    <row r="70" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="30"/>
       <c r="B70" s="31" t="s">
         <v>203</v>
@@ -5727,17 +5691,15 @@
         <v>1</v>
       </c>
       <c r="T70" s="36"/>
-      <c r="U70" s="36">
-        <v>1</v>
-      </c>
+      <c r="U70" s="36"/>
       <c r="V70" s="77">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W70" s="15"/>
       <c r="X70" s="3"/>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B71" s="23" t="s">
         <v>173</v>
       </c>
@@ -5770,7 +5732,7 @@
       </c>
       <c r="W71" s="15"/>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>74</v>
       </c>
@@ -5824,7 +5786,7 @@
       </c>
       <c r="W72" s="15"/>
     </row>
-    <row r="73" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="30"/>
       <c r="B73" s="31" t="s">
         <v>82</v>
@@ -5882,7 +5844,7 @@
       <c r="AD73"/>
       <c r="AE73"/>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B74" s="23" t="s">
         <v>93</v>
       </c>
@@ -5910,7 +5872,7 @@
       <c r="Y74" s="33"/>
       <c r="AA74" s="6"/>
     </row>
-    <row r="75" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="10"/>
       <c r="B75" s="23" t="s">
         <v>94</v>
@@ -5964,7 +5926,7 @@
       <c r="X75" s="3"/>
       <c r="AA75" s="6"/>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B76" s="23" t="s">
         <v>180</v>
       </c>
@@ -5992,7 +5954,7 @@
       <c r="AD76" s="6"/>
       <c r="AE76" s="6"/>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B77" s="23" t="s">
         <v>95</v>
       </c>
@@ -6039,7 +6001,7 @@
       </c>
       <c r="W77" s="15"/>
     </row>
-    <row r="78" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="10"/>
       <c r="B78" s="23" t="s">
         <v>96</v>
@@ -6099,7 +6061,7 @@
       <c r="AD78"/>
       <c r="AE78"/>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B79" s="24" t="s">
         <v>97</v>
       </c>
@@ -6146,12 +6108,12 @@
       </c>
       <c r="W79" s="15"/>
     </row>
-    <row r="80" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="11"/>
       <c r="W80" s="15"/>
       <c r="Z80" s="33"/>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I81" s="64" t="s">
         <v>98</v>
       </c>
@@ -6170,7 +6132,7 @@
       </c>
       <c r="T81" s="65">
         <f t="array" ref="T81">SUM($C2:$C79*(T2:T79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="U81" s="66"/>
       <c r="W81" s="15"/>
@@ -6179,7 +6141,7 @@
       <c r="AD81" s="6"/>
       <c r="AE81" s="6"/>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I82" s="67" t="s">
         <v>100</v>
       </c>
@@ -6198,12 +6160,12 @@
       </c>
       <c r="T82" s="68">
         <f t="array" ref="T82">SUM($C2:$C79*T2:T79*($V2:$V79&gt;=$X$12))</f>
-        <v>212.75</v>
+        <v>220.75</v>
       </c>
       <c r="U82" s="69"/>
       <c r="W82" s="15"/>
     </row>
-    <row r="83" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="10"/>
       <c r="B83" s="23"/>
       <c r="C83" s="14"/>
@@ -6230,7 +6192,7 @@
       </c>
       <c r="T83" s="68">
         <f t="array" ref="T83">SUM($C$2:$C$79*(T$2:T$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="U83" s="69"/>
       <c r="V83" s="3"/>
@@ -6244,7 +6206,7 @@
       <c r="AD83"/>
       <c r="AE83"/>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I84" s="67" t="s">
         <v>101</v>
       </c>
@@ -6259,11 +6221,11 @@
       <c r="R84" s="68"/>
       <c r="S84" s="68">
         <f>LOOKUP($X$12,$X23:$X31,$Y23:$Y31)</f>
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="T84" s="68">
         <f>LOOKUP($X$12,$X23:$X31,$Y23:$Y31)</f>
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="U84" s="69"/>
       <c r="W84" s="15"/>
@@ -6272,7 +6234,7 @@
       <c r="AD84" s="6"/>
       <c r="AE84" s="6"/>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I85" s="67" t="s">
         <v>102</v>
       </c>
@@ -6287,16 +6249,16 @@
       <c r="R85" s="70"/>
       <c r="S85" s="70">
         <f>S82/S84</f>
-        <v>0.87211538461538463</v>
+        <v>0.89271653543307083</v>
       </c>
       <c r="T85" s="70">
         <f>T82/T84</f>
-        <v>0.81826923076923075</v>
+        <v>0.86909448818897639</v>
       </c>
       <c r="U85" s="71"/>
       <c r="W85" s="15"/>
     </row>
-    <row r="86" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C86" s="33"/>
       <c r="I86" s="72" t="s">
         <v>80</v>
@@ -6312,11 +6274,11 @@
       <c r="R86" s="73"/>
       <c r="S86" s="73">
         <f>S84-S82</f>
-        <v>33.25</v>
+        <v>27.25</v>
       </c>
       <c r="T86" s="73">
         <f>T84-T82</f>
-        <v>47.25</v>
+        <v>33.25</v>
       </c>
       <c r="U86" s="74"/>
       <c r="W86" s="15"/>
@@ -6325,11 +6287,11 @@
       <c r="AD86" s="6"/>
       <c r="AE86" s="6"/>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C87" s="33"/>
       <c r="W87" s="15"/>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C88" s="33"/>
       <c r="I88" s="14"/>
       <c r="J88" s="14"/>
@@ -6338,7 +6300,7 @@
       <c r="N88" s="14"/>
       <c r="W88" s="15"/>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C89" s="33"/>
       <c r="I89" s="14"/>
       <c r="J89" s="14"/>
@@ -6347,7 +6309,7 @@
       <c r="N89" s="14"/>
       <c r="W89" s="15"/>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I90" s="14"/>
       <c r="J90" s="14"/>
       <c r="K90" s="14"/>
@@ -6355,7 +6317,7 @@
       <c r="N90" s="14"/>
       <c r="W90" s="15"/>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I91" s="14"/>
       <c r="J91" s="14"/>
       <c r="K91" s="14"/>
@@ -6364,7 +6326,7 @@
       <c r="W91" s="15"/>
       <c r="AA91" s="33"/>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I92" s="14"/>
       <c r="J92" s="14"/>
       <c r="K92" s="14"/>
@@ -6372,28 +6334,28 @@
       <c r="N92" s="14"/>
       <c r="W92" s="15"/>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I93" s="14"/>
       <c r="J93" s="14"/>
       <c r="K93" s="14"/>
       <c r="L93" s="14"/>
       <c r="N93" s="14"/>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I94" s="14"/>
       <c r="J94" s="14"/>
       <c r="K94" s="14"/>
       <c r="L94" s="14"/>
       <c r="N94" s="14"/>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I95" s="14"/>
       <c r="J95" s="14"/>
       <c r="K95" s="14"/>
       <c r="L95" s="14"/>
       <c r="N95" s="14"/>
     </row>
-    <row r="96" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="10"/>
       <c r="B96" s="23"/>
       <c r="C96" s="14"/>
@@ -6426,25 +6388,25 @@
       <c r="AD96"/>
       <c r="AE96"/>
     </row>
-    <row r="99" spans="28:31" x14ac:dyDescent="0.2">
+    <row r="99" spans="28:31" x14ac:dyDescent="0.3">
       <c r="AB99" s="6"/>
       <c r="AC99" s="6"/>
       <c r="AD99" s="6"/>
       <c r="AE99" s="6"/>
     </row>
-    <row r="103" spans="28:31" x14ac:dyDescent="0.2">
+    <row r="103" spans="28:31" x14ac:dyDescent="0.3">
       <c r="AB103" s="6"/>
       <c r="AC103" s="6"/>
       <c r="AD103" s="6"/>
       <c r="AE103" s="6"/>
     </row>
-    <row r="108" spans="28:31" x14ac:dyDescent="0.2">
+    <row r="108" spans="28:31" x14ac:dyDescent="0.3">
       <c r="AB108" s="6"/>
       <c r="AC108" s="6"/>
       <c r="AD108" s="6"/>
       <c r="AE108" s="6"/>
     </row>
-    <row r="121" spans="28:31" x14ac:dyDescent="0.2">
+    <row r="121" spans="28:31" x14ac:dyDescent="0.3">
       <c r="AB121" s="33"/>
       <c r="AC121" s="33"/>
       <c r="AD121" s="33"/>
@@ -6469,379 +6431,379 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A73"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
       <selection sqref="A1:A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>71</v>
       </c>

</xml_diff>